<commit_message>
New points - POTEC
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA39E5EA-6D50-4F2E-A14F-E1EF719AC19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC26BBE-DE65-4B95-993E-D6F9E9FD051F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -1596,7 +1596,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2552,7 @@
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New points - POTEC lab 5
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC26BBE-DE65-4B95-993E-D6F9E9FD051F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FE9F87-847C-4430-8D1F-8FEBC4C2A219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -1018,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1121,6 +1121,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,16 +1218,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1218,22 +1227,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1595,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,60 +1622,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="42"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="38"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="45"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="H5" s="39" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="41"/>
-      <c r="K5" s="39" t="s">
+      <c r="I5" s="48"/>
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1738,37 +1735,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="42"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="43">
+      <c r="B10" s="50">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="E10" s="47"/>
-      <c r="G10" s="43">
+      <c r="C10" s="50"/>
+      <c r="E10" s="54"/>
+      <c r="G10" s="50">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>57.3</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="E11" s="48"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1793,46 +1790,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="H17" s="39" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="H17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
-      <c r="L17" s="42" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="L17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="42"/>
-      <c r="O17" s="42" t="s">
+      <c r="M17" s="49"/>
+      <c r="O17" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="42"/>
+      <c r="P17" s="49"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1862,17 +1859,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="43">
+      <c r="L18" s="50">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="43"/>
-      <c r="O18" s="43">
+      <c r="M18" s="50"/>
+      <c r="O18" s="50">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="43"/>
-      <c r="R18" s="32"/>
+      <c r="P18" s="50"/>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1887,11 +1884,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="R19" s="32"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1916,56 +1913,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
-      <c r="N23" s="43" t="s">
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="42"/>
+      <c r="N23" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="43"/>
+      <c r="O23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="45"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="F26" s="46" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="F26" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="39" t="s">
+      <c r="K26" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="41"/>
+      <c r="L26" s="48"/>
       <c r="N26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2001,11 +1998,11 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="49">
+      <c r="N27" s="56">
         <f>SUM(B28:D28,F28:I28,K28:L28)</f>
         <v>1</v>
       </c>
-      <c r="O27" s="47"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -2019,8 +2016,8 @@
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="48"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="55"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -2045,39 +2042,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="35"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="42"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="46"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="41"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -2105,25 +2102,25 @@
       <c r="C37" s="2"/>
       <c r="E37" s="2">
         <f>C56</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F37" s="2">
         <f>G51</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="F40" s="43" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="43"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2140,10 +2137,12 @@
       <c r="F41" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2">
+        <v>9</v>
+      </c>
       <c r="I41" s="2">
         <f>SUM(B37:C37,E37:H37)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J41" s="7"/>
       <c r="L41" s="7"/>
@@ -2171,7 +2170,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="42" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2180,19 +2179,21 @@
         <v>106</v>
       </c>
       <c r="C44" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="42"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2">
+        <v>4</v>
+      </c>
       <c r="F45" s="2" t="s">
         <v>121</v>
       </c>
@@ -2233,7 +2234,7 @@
       <c r="G48" s="2"/>
       <c r="I48" s="2">
         <f>50-SUM(B37:C37,E37:H37)</f>
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -2262,7 +2263,7 @@
       </c>
       <c r="G51" s="2">
         <f>SUM(G41:G49)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -2289,7 +2290,7 @@
       </c>
       <c r="C56" s="2">
         <f>SUM(C41:C54)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2315,70 +2316,70 @@
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-      <c r="M60" s="34"/>
-      <c r="N60" s="34"/>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
-      <c r="Q60" s="34"/>
-      <c r="R60" s="34"/>
-      <c r="S60" s="35"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="41"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="41"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="41"/>
+      <c r="S60" s="42"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
-      <c r="M61" s="37"/>
-      <c r="N61" s="37"/>
-      <c r="O61" s="37"/>
-      <c r="P61" s="37"/>
-      <c r="Q61" s="37"/>
-      <c r="R61" s="37"/>
-      <c r="S61" s="38"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="44"/>
+      <c r="M61" s="44"/>
+      <c r="N61" s="44"/>
+      <c r="O61" s="44"/>
+      <c r="P61" s="44"/>
+      <c r="Q61" s="44"/>
+      <c r="R61" s="44"/>
+      <c r="S61" s="45"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
-      <c r="M63" s="46" t="s">
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
+      <c r="M63" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="46"/>
-      <c r="O63" s="46"/>
-      <c r="P63" s="46"/>
-      <c r="R63" s="46" t="s">
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="R63" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="46"/>
+      <c r="S63" s="53"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -2467,37 +2468,37 @@
       <c r="S65" s="2"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="42" t="s">
+      <c r="B68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="42"/>
+      <c r="C68" s="49"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="42" t="s">
+      <c r="G68" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="42"/>
+      <c r="H68" s="49"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="43">
+      <c r="B69" s="50">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>17</v>
       </c>
-      <c r="C69" s="43"/>
-      <c r="E69" s="32"/>
-      <c r="G69" s="43">
+      <c r="C69" s="50"/>
+      <c r="E69" s="39"/>
+      <c r="G69" s="50">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>33</v>
       </c>
-      <c r="H69" s="43"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
-      <c r="E70" s="32"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="E70" s="39"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -2580,60 +2581,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="53"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="56"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="63"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2715,28 +2716,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="43">
+      <c r="B10" s="50">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="E10" s="47">
+      <c r="C10" s="50"/>
+      <c r="E10" s="54">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="E11" s="48"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2761,40 +2762,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="F17" s="46" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="F17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="J17" s="42" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="J17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="42"/>
+      <c r="K17" s="49"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2818,12 +2819,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="50">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="43"/>
-      <c r="M18" s="32">
+      <c r="K18" s="50"/>
+      <c r="M18" s="39">
         <v>5</v>
       </c>
     </row>
@@ -2846,9 +2847,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="M19" s="32"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2873,46 +2874,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="53"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="60"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="63"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="E26" s="39" t="s">
+      <c r="C26" s="53"/>
+      <c r="E26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="41"/>
-      <c r="I26" s="46" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2947,12 +2948,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="57">
+      <c r="M27" s="64">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="32">
+      <c r="O27" s="39">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2982,9 +2983,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="57"/>
+      <c r="M28" s="64"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="32"/>
+      <c r="O28" s="39"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3010,39 +3011,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="53"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="54"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="56"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="63"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="F35" s="46" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="F35" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3099,14 +3100,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="F40" s="43" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="43"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3162,7 +3163,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="42" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3179,7 +3180,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="42"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3323,67 +3324,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="51" t="s">
+      <c r="B58" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="52"/>
-      <c r="M58" s="52"/>
-      <c r="N58" s="52"/>
-      <c r="O58" s="52"/>
-      <c r="P58" s="52"/>
-      <c r="Q58" s="52"/>
-      <c r="R58" s="53"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
+      <c r="K58" s="59"/>
+      <c r="L58" s="59"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="59"/>
+      <c r="Q58" s="59"/>
+      <c r="R58" s="60"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="54"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="55"/>
-      <c r="N59" s="55"/>
-      <c r="O59" s="55"/>
-      <c r="P59" s="55"/>
-      <c r="Q59" s="55"/>
-      <c r="R59" s="56"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="62"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="62"/>
+      <c r="Q59" s="62"/>
+      <c r="R59" s="63"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="M61" s="46" t="s">
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+      <c r="M61" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="46"/>
-      <c r="O61" s="46"/>
-      <c r="Q61" s="46" t="s">
+      <c r="N61" s="53"/>
+      <c r="O61" s="53"/>
+      <c r="Q61" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="46"/>
+      <c r="R61" s="53"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3480,28 +3481,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="42"/>
+      <c r="C66" s="49"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="43">
+      <c r="B67" s="50">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="43"/>
-      <c r="E67" s="32">
+      <c r="C67" s="50"/>
+      <c r="E67" s="39">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="E68" s="32"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="E68" s="39"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3526,26 +3527,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="51" t="s">
+      <c r="B72" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="52"/>
-      <c r="D72" s="52"/>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="G72" s="52"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="53"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="60"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="54"/>
-      <c r="C73" s="55"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55"/>
-      <c r="G73" s="55"/>
-      <c r="H73" s="55"/>
-      <c r="I73" s="56"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="63"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3572,10 +3573,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="42" t="s">
+      <c r="K75" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="42"/>
+      <c r="L75" s="49"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3605,11 +3606,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="43">
+      <c r="K76" s="50">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="43"/>
+      <c r="L76" s="50"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -4189,53 +4190,53 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
-      <c r="F2" s="62" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
+      <c r="F2" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="64"/>
-      <c r="J2" s="62" t="s">
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="J2" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="67"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="K3" s="66" t="s">
+      <c r="K3" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="L3" s="67" t="s">
+      <c r="L3" s="36" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="37" t="s">
         <v>133</v>
       </c>
       <c r="C4" s="14">
@@ -4244,14 +4245,14 @@
       <c r="D4" s="14">
         <v>4</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="37" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="14">
         <v>5</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="J4" s="68" t="s">
+      <c r="J4" s="37" t="s">
         <v>199</v>
       </c>
       <c r="K4" s="14">
@@ -4260,7 +4261,7 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="38" t="s">
         <v>134</v>
       </c>
       <c r="C5" s="2">
@@ -4269,14 +4270,14 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="38" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="38" t="s">
         <v>200</v>
       </c>
       <c r="K5" s="2">
@@ -4285,7 +4286,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="38" t="s">
         <v>135</v>
       </c>
       <c r="C6" s="2">
@@ -4294,14 +4295,14 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="38" t="s">
         <v>77</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="38" t="s">
         <v>201</v>
       </c>
       <c r="K6" s="2">
@@ -4310,7 +4311,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="38" t="s">
         <v>136</v>
       </c>
       <c r="C7" s="2">
@@ -4319,14 +4320,14 @@
       <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="38" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="38" t="s">
         <v>202</v>
       </c>
       <c r="K7" s="2">
@@ -4335,7 +4336,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="38" t="s">
         <v>137</v>
       </c>
       <c r="C8" s="2">
@@ -4344,14 +4345,14 @@
       <c r="D8" s="2">
         <v>4.5</v>
       </c>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="38" t="s">
         <v>80</v>
       </c>
       <c r="G8" s="2">
         <v>11</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="38" t="s">
         <v>203</v>
       </c>
       <c r="K8" s="2">
@@ -4360,7 +4361,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="38" t="s">
         <v>138</v>
       </c>
       <c r="C9" s="2">
@@ -4369,36 +4370,36 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61">
+      <c r="C11" s="69"/>
+      <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61">
+      <c r="G11" s="69"/>
+      <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="K11" s="60"/>
-      <c r="L11" s="61">
+      <c r="K11" s="69"/>
+      <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Points from the colloquium 1 - POTEC
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B005063B-2C41-45D2-B4E8-5D2F36428623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34F131B-8E13-4E22-8B4D-9D282295A033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -660,6 +660,18 @@
   </si>
   <si>
     <t>III semestr (25Z)</t>
+  </si>
+  <si>
+    <t>LAB1 (γ)</t>
+  </si>
+  <si>
+    <t>LAB3 (Lepkość)</t>
+  </si>
+  <si>
+    <t>LAB2 (Interferencja)</t>
+  </si>
+  <si>
+    <t>LAB4 (Magnetyzm)</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1165,12 +1177,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1241,6 +1247,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8585"/>
+      <color rgb="FFFDBF8B"/>
+      <color rgb="FFFDAF6F"/>
+      <color rgb="FFFFCC66"/>
       <color rgb="FFDEEDF4"/>
       <color rgb="FFE3EAEF"/>
     </mruColors>
@@ -1593,7 +1603,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1614,7 @@
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
@@ -1659,23 +1669,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="51"/>
-      <c r="H5" s="50" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="49"/>
+      <c r="H5" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="K5" s="50" t="s">
+      <c r="I5" s="49"/>
+      <c r="K5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="49"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1735,37 +1745,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="53"/>
+      <c r="C9" s="51"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="53"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="54">
+      <c r="B10" s="52">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="52"/>
       <c r="E10" s="46"/>
-      <c r="G10" s="54">
+      <c r="G10" s="52">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>56.3</v>
       </c>
-      <c r="H10" s="54"/>
+      <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
       <c r="E11" s="47"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1817,19 +1827,19 @@
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="L17" s="53" t="s">
+      <c r="I17" s="50"/>
+      <c r="J17" s="49"/>
+      <c r="L17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="53"/>
-      <c r="O17" s="53" t="s">
+      <c r="M17" s="51"/>
+      <c r="O17" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="53"/>
+      <c r="P17" s="51"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1859,17 +1869,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="54">
+      <c r="L18" s="52">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="54"/>
-      <c r="O18" s="54">
+      <c r="M18" s="52"/>
+      <c r="O18" s="52">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="R18" s="55"/>
+      <c r="P18" s="52"/>
+      <c r="R18" s="53"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1884,11 +1894,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="54"/>
-      <c r="R19" s="55"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="R19" s="53"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1926,10 +1936,10 @@
       <c r="J23" s="41"/>
       <c r="K23" s="41"/>
       <c r="L23" s="42"/>
-      <c r="N23" s="54" t="s">
+      <c r="N23" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="54"/>
+      <c r="O23" s="52"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="43"/>
@@ -1943,8 +1953,8 @@
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
       <c r="L24" s="45"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="39" t="s">
@@ -1959,14 +1969,11 @@
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="50" t="s">
+      <c r="K26" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="51"/>
-      <c r="N26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26" s="9" t="s">
+      <c r="L26" s="49"/>
+      <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1981,16 +1988,16 @@
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>73</v>
@@ -1998,11 +2005,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="48">
-        <f>SUM(B28:D28,F28:I28,K28:L28)</f>
-        <v>1</v>
-      </c>
-      <c r="O27" s="46"/>
+      <c r="N27" s="46"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -2011,13 +2014,14 @@
         <v>1</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="47"/>
+      <c r="N28" s="47"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -2069,12 +2073,12 @@
       </c>
       <c r="C35" s="39"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="51"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="49"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -2098,7 +2102,9 @@
       <c r="O36" s="7"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
+      <c r="B37" s="2">
+        <v>17</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="E37" s="2">
         <f>C56</f>
@@ -2113,14 +2119,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="F40" s="54" t="s">
+      <c r="C40" s="55"/>
+      <c r="F40" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="54"/>
+      <c r="G40" s="52"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2142,7 +2148,7 @@
       </c>
       <c r="I41" s="2">
         <f>SUM(B37:C37,E37:H37)</f>
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="J41" s="7"/>
       <c r="L41" s="7"/>
@@ -2170,7 +2176,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="53" t="s">
+      <c r="I43" s="51" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2185,7 +2191,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="53"/>
+      <c r="I44" s="51"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2234,7 +2240,7 @@
       <c r="G48" s="2"/>
       <c r="I48" s="2">
         <f>50-SUM(B37:C37,E37:H37)</f>
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -2468,40 +2474,40 @@
       <c r="S65" s="2"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="53" t="s">
+      <c r="B68" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="53"/>
+      <c r="C68" s="51"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="53" t="s">
+      <c r="G68" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="53"/>
+      <c r="H68" s="51"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="54">
+      <c r="B69" s="52">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>17</v>
       </c>
-      <c r="C69" s="54"/>
-      <c r="E69" s="55"/>
-      <c r="G69" s="54">
+      <c r="C69" s="52"/>
+      <c r="E69" s="53"/>
+      <c r="G69" s="52">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>33</v>
       </c>
-      <c r="H69" s="54"/>
+      <c r="H69" s="52"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="E70" s="55"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="E70" s="53"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="38">
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2530,7 +2536,6 @@
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="O27:O28"/>
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="K26:L26"/>
@@ -2581,40 +2586,40 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="60"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="58"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="61"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="63"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="61"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2629,12 +2634,12 @@
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="49"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2716,27 +2721,27 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="53"/>
+      <c r="C9" s="51"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="54">
+      <c r="B10" s="52">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="52"/>
       <c r="E10" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
       <c r="E11" s="47"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2762,24 +2767,24 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="39" t="s">
@@ -2792,10 +2797,10 @@
       </c>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
-      <c r="J17" s="53" t="s">
+      <c r="J17" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="53"/>
+      <c r="K17" s="51"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2819,12 +2824,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="52">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="54"/>
-      <c r="M18" s="55">
+      <c r="K18" s="52"/>
+      <c r="M18" s="53">
         <v>5</v>
       </c>
     </row>
@@ -2847,9 +2852,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="M19" s="55"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="M19" s="53"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2874,41 +2879,41 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="60"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="58"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="63"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="61"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="39" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="39"/>
-      <c r="E26" s="50" t="s">
+      <c r="E26" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="49"/>
       <c r="I26" s="39" t="s">
         <v>20</v>
       </c>
@@ -2948,12 +2953,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="64">
+      <c r="M27" s="62">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="55">
+      <c r="O27" s="53">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2983,9 +2988,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="64"/>
+      <c r="M28" s="62"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="55"/>
+      <c r="O28" s="53"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3011,26 +3016,26 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="60"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="61"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="39" t="s">
@@ -3100,14 +3105,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="F40" s="54" t="s">
+      <c r="C40" s="55"/>
+      <c r="F40" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="54"/>
+      <c r="G40" s="52"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3163,7 +3168,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="53" t="s">
+      <c r="I43" s="51" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3180,7 +3185,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="53"/>
+      <c r="I44" s="51"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3324,44 +3329,44 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="59"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59"/>
-      <c r="I58" s="59"/>
-      <c r="J58" s="59"/>
-      <c r="K58" s="59"/>
-      <c r="L58" s="59"/>
-      <c r="M58" s="59"/>
-      <c r="N58" s="59"/>
-      <c r="O58" s="59"/>
-      <c r="P58" s="59"/>
-      <c r="Q58" s="59"/>
-      <c r="R58" s="60"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="57"/>
+      <c r="N58" s="57"/>
+      <c r="O58" s="57"/>
+      <c r="P58" s="57"/>
+      <c r="Q58" s="57"/>
+      <c r="R58" s="58"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="61"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
-      <c r="F59" s="62"/>
-      <c r="G59" s="62"/>
-      <c r="H59" s="62"/>
-      <c r="I59" s="62"/>
-      <c r="J59" s="62"/>
-      <c r="K59" s="62"/>
-      <c r="L59" s="62"/>
-      <c r="M59" s="62"/>
-      <c r="N59" s="62"/>
-      <c r="O59" s="62"/>
-      <c r="P59" s="62"/>
-      <c r="Q59" s="62"/>
-      <c r="R59" s="63"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="60"/>
+      <c r="N59" s="60"/>
+      <c r="O59" s="60"/>
+      <c r="P59" s="60"/>
+      <c r="Q59" s="60"/>
+      <c r="R59" s="61"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="39" t="s">
@@ -3481,28 +3486,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="53" t="s">
+      <c r="B66" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="53"/>
+      <c r="C66" s="51"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="54">
+      <c r="B67" s="52">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="54"/>
-      <c r="E67" s="55">
+      <c r="C67" s="52"/>
+      <c r="E67" s="53">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="54"/>
-      <c r="C68" s="54"/>
-      <c r="E68" s="55"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="52"/>
+      <c r="E68" s="53"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3527,26 +3532,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="60"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
+      <c r="E72" s="57"/>
+      <c r="F72" s="57"/>
+      <c r="G72" s="57"/>
+      <c r="H72" s="57"/>
+      <c r="I72" s="58"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="61"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
-      <c r="H73" s="62"/>
-      <c r="I73" s="63"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="60"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="60"/>
+      <c r="F73" s="60"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="60"/>
+      <c r="I73" s="61"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3573,10 +3578,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="53" t="s">
+      <c r="K75" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="53"/>
+      <c r="L75" s="51"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3606,11 +3611,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="54">
+      <c r="K76" s="52">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="54"/>
+      <c r="L76" s="52"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -4190,21 +4195,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="63" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="67"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
+      <c r="F2" s="63" t="s">
         <v>205</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
-      <c r="J2" s="65" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="65"/>
+      <c r="J2" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4379,26 +4384,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="68" t="s">
+      <c r="F11" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="G11" s="69"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="K11" s="69"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - POTEC lab8
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34F131B-8E13-4E22-8B4D-9D282295A033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DC516C-F8E4-45B0-9B1F-5B593EB407A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t>LAB4 (Magnetyzm)</t>
+  </si>
+  <si>
+    <t>Laboratoria [ocena]</t>
   </si>
 </sst>
 </file>
@@ -1152,56 +1155,56 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1602,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,23 +1672,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="49"/>
-      <c r="H5" s="48" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="K5" s="48" t="s">
+      <c r="I5" s="48"/>
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="49"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1745,37 +1748,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="51"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="52">
+      <c r="B10" s="50">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="E10" s="46"/>
-      <c r="G10" s="52">
+      <c r="C10" s="50"/>
+      <c r="E10" s="54"/>
+      <c r="G10" s="50">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>56.3</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="E11" s="47"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1820,26 +1823,26 @@
       <c r="H15" s="45"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="H17" s="48" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="H17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="49"/>
-      <c r="L17" s="51" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="L17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="51"/>
-      <c r="O17" s="51" t="s">
+      <c r="M17" s="49"/>
+      <c r="O17" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="51"/>
+      <c r="P17" s="49"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1869,17 +1872,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="52">
+      <c r="L18" s="50">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="52"/>
-      <c r="O18" s="52">
+      <c r="M18" s="50"/>
+      <c r="O18" s="50">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="52"/>
-      <c r="R18" s="53"/>
+      <c r="P18" s="50"/>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1894,11 +1897,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="52"/>
-      <c r="R19" s="53"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1936,10 +1939,10 @@
       <c r="J23" s="41"/>
       <c r="K23" s="41"/>
       <c r="L23" s="42"/>
-      <c r="N23" s="52" t="s">
+      <c r="N23" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="52"/>
+      <c r="O23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="43"/>
@@ -1953,26 +1956,26 @@
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
       <c r="L24" s="45"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="F26" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="F26" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="48" t="s">
+      <c r="K26" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="49"/>
+      <c r="L26" s="48"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2005,7 +2008,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="46"/>
+      <c r="N27" s="54"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -2021,7 +2024,7 @@
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="47"/>
+      <c r="N28" s="55"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -2068,17 +2071,17 @@
       <c r="I33" s="45"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="39"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="49"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -2108,7 +2111,7 @@
       <c r="C37" s="2"/>
       <c r="E37" s="2">
         <f>C56</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F37" s="2">
         <f>G51</f>
@@ -2119,14 +2122,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="F40" s="52" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2148,7 +2151,7 @@
       </c>
       <c r="I41" s="2">
         <f>SUM(B37:C37,E37:H37)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J41" s="7"/>
       <c r="L41" s="7"/>
@@ -2176,7 +2179,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="51" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2191,7 +2194,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="51"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2233,14 +2236,16 @@
       <c r="B48" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
       <c r="F48" s="2" t="s">
         <v>124</v>
       </c>
       <c r="G48" s="2"/>
       <c r="I48" s="2">
         <f>50-SUM(B37:C37,E37:H37)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -2296,7 +2301,7 @@
       </c>
       <c r="C56" s="2">
         <f>SUM(C41:C54)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2364,28 +2369,28 @@
       <c r="S61" s="45"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="39" t="s">
+      <c r="B63" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="M63" s="39" t="s">
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
+      <c r="M63" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="39"/>
-      <c r="O63" s="39"/>
-      <c r="P63" s="39"/>
-      <c r="R63" s="39" t="s">
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="R63" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="39"/>
+      <c r="S63" s="53"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -2474,40 +2479,62 @@
       <c r="S65" s="2"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="51" t="s">
+      <c r="B68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="51"/>
+      <c r="C68" s="49"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="51" t="s">
+      <c r="G68" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="51"/>
+      <c r="H68" s="49"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="52">
+      <c r="B69" s="50">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>17</v>
       </c>
-      <c r="C69" s="52"/>
-      <c r="E69" s="53"/>
-      <c r="G69" s="52">
+      <c r="C69" s="50"/>
+      <c r="E69" s="39"/>
+      <c r="G69" s="50">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>33</v>
       </c>
-      <c r="H69" s="52"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="52"/>
-      <c r="C70" s="52"/>
-      <c r="E70" s="53"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="E70" s="39"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2524,28 +2551,6 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2623,23 +2628,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="49"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2721,28 +2726,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="52">
+      <c r="B10" s="50">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="E10" s="46">
+      <c r="C10" s="50"/>
+      <c r="E10" s="54">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2787,20 +2792,20 @@
       <c r="H15" s="61"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="F17" s="39" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="F17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="J17" s="51" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="J17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="51"/>
+      <c r="K17" s="49"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2824,12 +2829,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="50">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="52"/>
-      <c r="M18" s="53">
+      <c r="K18" s="50"/>
+      <c r="M18" s="39">
         <v>5</v>
       </c>
     </row>
@@ -2852,9 +2857,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="M19" s="53"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2905,20 +2910,20 @@
       <c r="K24" s="61"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="E26" s="48" t="s">
+      <c r="C26" s="53"/>
+      <c r="E26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="49"/>
-      <c r="I26" s="39" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="53">
+      <c r="O27" s="39">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2990,7 +2995,7 @@
       </c>
       <c r="M28" s="62"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="53"/>
+      <c r="O28" s="39"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3038,17 +3043,17 @@
       <c r="I33" s="61"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="F35" s="39" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="F35" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3105,14 +3110,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="F40" s="52" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3168,7 +3173,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="51" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3185,7 +3190,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="51"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3369,27 +3374,27 @@
       <c r="R59" s="61"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="M61" s="39" t="s">
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+      <c r="M61" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-      <c r="Q61" s="39" t="s">
+      <c r="N61" s="53"/>
+      <c r="O61" s="53"/>
+      <c r="Q61" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="39"/>
+      <c r="R61" s="53"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3486,28 +3491,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="51" t="s">
+      <c r="B66" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="51"/>
+      <c r="C66" s="49"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="52">
+      <c r="B67" s="50">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="52"/>
-      <c r="E67" s="53">
+      <c r="C67" s="50"/>
+      <c r="E67" s="39">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="52"/>
-      <c r="C68" s="52"/>
-      <c r="E68" s="53"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="E68" s="39"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3578,10 +3583,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="51" t="s">
+      <c r="K75" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="51"/>
+      <c r="L75" s="49"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3611,11 +3616,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="52">
+      <c r="K76" s="50">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="52"/>
+      <c r="L76" s="50"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3643,20 +3648,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -3667,16 +3668,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New points - MAT3 and FIZ1 + corrections in schedule
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C5EFB-E949-48F7-8098-9385FD81E2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC88167-D2D0-4AC6-BB78-6E55CB9408F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="218">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -431,9 +431,6 @@
     <t>Ćwiczenia [C = 0,6K+0,4P]</t>
   </si>
   <si>
-    <t>Kolokwium</t>
-  </si>
-  <si>
     <t>Mini-projekt</t>
   </si>
   <si>
@@ -678,6 +675,24 @@
   </si>
   <si>
     <t>W16</t>
+  </si>
+  <si>
+    <t>1. RSA</t>
+  </si>
+  <si>
+    <t>Sieć sortująca</t>
+  </si>
+  <si>
+    <t>Projekt #2</t>
+  </si>
+  <si>
+    <t>6. Zliczanie orbit</t>
+  </si>
+  <si>
+    <t>Kolokwium [15 pkt]</t>
+  </si>
+  <si>
+    <t>Zliczanie orbit</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,22 +1713,26 @@
     </row>
     <row r="6" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1756,9 @@
       <c r="C7" s="2">
         <v>2.7</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
@@ -1766,13 +1787,13 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="52">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>9.6999999999999993</v>
+        <v>12.7</v>
       </c>
       <c r="C10" s="52"/>
       <c r="E10" s="46"/>
       <c r="G10" s="52">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>56.3</v>
+        <v>53.3</v>
       </c>
       <c r="H10" s="52"/>
     </row>
@@ -1852,13 +1873,13 @@
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>92</v>
@@ -1943,7 +1964,7 @@
       <c r="K23" s="41"/>
       <c r="L23" s="42"/>
       <c r="N23" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O23" s="52"/>
     </row>
@@ -1969,7 +1990,7 @@
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
       <c r="F26" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
@@ -1985,25 +2006,25 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>73</v>
@@ -2014,7 +2035,9 @@
       <c r="N27" s="46"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <v>1</v>
@@ -2080,7 +2103,7 @@
       <c r="C35" s="39"/>
       <c r="D35" s="7"/>
       <c r="E35" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F35" s="50"/>
       <c r="G35" s="50"/>
@@ -2421,7 +2444,7 @@
         <v>81</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>85</v>
@@ -2459,10 +2482,10 @@
         <v>2</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H65" s="2">
         <v>2</v>
@@ -2477,7 +2500,9 @@
       <c r="M65" s="2">
         <v>5</v>
       </c>
-      <c r="N65" s="2"/>
+      <c r="N65" s="2">
+        <v>5</v>
+      </c>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
       <c r="R65" s="2"/>
@@ -2499,13 +2524,13 @@
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B69" s="52">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C69" s="52"/>
       <c r="E69" s="53"/>
       <c r="G69" s="52">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H69" s="52"/>
     </row>
@@ -2597,7 +2622,7 @@
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" s="57"/>
       <c r="D2" s="57"/>
@@ -2778,7 +2803,7 @@
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="57"/>
       <c r="D14" s="57"/>
@@ -2890,7 +2915,7 @@
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" s="56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -3027,7 +3052,7 @@
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="57"/>
@@ -3340,7 +3365,7 @@
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B58" s="56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C58" s="57"/>
       <c r="D58" s="57"/>
@@ -3543,7 +3568,7 @@
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B72" s="56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C72" s="57"/>
       <c r="D72" s="57"/>
@@ -3565,28 +3590,28 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="I75" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="K75" s="51" t="s">
         <v>22</v>
@@ -3695,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
-  <dimension ref="B1:F34"/>
+  <dimension ref="B1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,16 +3737,16 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="E2" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3735,10 +3760,10 @@
         <v>45763</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -3749,13 +3774,13 @@
         <v>77</v>
       </c>
       <c r="D4" s="20">
-        <v>45810</v>
+        <v>45803</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -3769,10 +3794,10 @@
         <v>45817</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -3792,7 +3817,7 @@
         <v>103</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -3809,7 +3834,7 @@
         <v>104</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -3826,24 +3851,24 @@
         <v>105</v>
       </c>
       <c r="F9" s="27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="28">
+        <v>45785</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="20">
-        <v>45785</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -3860,7 +3885,7 @@
         <v>107</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -3871,7 +3896,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="28">
         <v>45728</v>
@@ -3880,7 +3905,7 @@
         <v>84</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -3888,33 +3913,33 @@
         <v>1</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="28">
         <v>45747</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="28">
+        <v>45784</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="F14" s="27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="20">
-        <v>45782</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="F15" s="27" t="s">
         <v>165</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -3922,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D16" s="20">
         <v>45796</v>
@@ -3931,7 +3956,7 @@
         <v>85</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -3939,16 +3964,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" s="20">
         <v>45817</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -3956,16 +3981,16 @@
         <v>0</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" s="20">
         <v>45819</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -3977,13 +4002,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" s="20">
         <v>45820</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -3991,13 +4016,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" s="20">
         <v>45820</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -4015,10 +4040,10 @@
         <v>45728</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -4032,10 +4057,10 @@
         <v>45742</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4049,10 +4074,10 @@
         <v>45756</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -4066,27 +4091,27 @@
         <v>45770</v>
       </c>
       <c r="E26" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="28">
+        <v>45784</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="F26" s="29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="20">
-        <v>45784</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>189</v>
+      <c r="F27" s="27" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -4100,10 +4125,10 @@
         <v>45798</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -4117,9 +4142,11 @@
         <v>45812</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="17"/>
+        <v>179</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C30" s="31"/>
@@ -4135,10 +4162,10 @@
         <v>45764</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -4155,24 +4182,41 @@
         <v>45767</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="19" t="b">
+      <c r="B34" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="28">
+        <v>45775</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C35" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="20">
-        <v>45775</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>150</v>
+      <c r="D35" s="20">
+        <v>45794</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4206,53 +4250,53 @@
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="65"/>
       <c r="F2" s="63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G2" s="64"/>
       <c r="H2" s="65"/>
       <c r="J2" s="63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K2" s="64"/>
       <c r="L2" s="65"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>197</v>
-      </c>
       <c r="H3" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="J3" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>197</v>
-      </c>
       <c r="L3" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4268,7 +4312,7 @@
       </c>
       <c r="H4" s="14"/>
       <c r="J4" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K4" s="14">
         <v>4</v>
@@ -4277,7 +4321,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -4293,7 +4337,7 @@
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K5" s="2">
         <v>4</v>
@@ -4302,7 +4346,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4318,7 +4362,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="J6" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K6" s="2">
         <v>5</v>
@@ -4327,7 +4371,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4343,7 +4387,7 @@
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K7" s="2">
         <v>5</v>
@@ -4352,7 +4396,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -4368,7 +4412,7 @@
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K8" s="2">
         <v>12</v>
@@ -4377,7 +4421,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -4395,7 +4439,7 @@
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="33">
@@ -4403,7 +4447,7 @@
         <v>4.4333333333333336</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G11" s="67"/>
       <c r="H11" s="33">
@@ -4411,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K11" s="67"/>
       <c r="L11" s="33">

</xml_diff>

<commit_message>
MAT3 - points from the colloquium and corrections in schedule
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC88167-D2D0-4AC6-BB78-6E55CB9408F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF068950-203A-42A1-AF03-542A2F69086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="223">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -693,6 +693,21 @@
   </si>
   <si>
     <t>Zliczanie orbit</t>
+  </si>
+  <si>
+    <t>Praca domowa</t>
+  </si>
+  <si>
+    <t>Poprawa kolosa</t>
+  </si>
+  <si>
+    <t>Mechanika</t>
+  </si>
+  <si>
+    <t>Wahadło odwrócone</t>
+  </si>
+  <si>
+    <t>Projekt</t>
   </si>
 </sst>
 </file>
@@ -703,7 +718,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-415]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +766,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1051,7 +1083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1173,57 +1205,57 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,6 +1291,44 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1623,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,23 +1760,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="49"/>
-      <c r="H5" s="48" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="K5" s="48" t="s">
+      <c r="I5" s="48"/>
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="49"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1763,7 +1833,9 @@
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>12</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2">
@@ -1772,37 +1844,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="51"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="52">
+      <c r="B10" s="50">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>12.7</v>
-      </c>
-      <c r="C10" s="52"/>
-      <c r="E10" s="46"/>
-      <c r="G10" s="52">
+        <v>24.7</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="E10" s="54"/>
+      <c r="G10" s="50">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>53.3</v>
-      </c>
-      <c r="H10" s="52"/>
+        <v>41.3</v>
+      </c>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="E11" s="47"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1847,26 +1919,26 @@
       <c r="H15" s="45"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="H17" s="48" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="H17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="49"/>
-      <c r="L17" s="51" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="L17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="51"/>
-      <c r="O17" s="51" t="s">
+      <c r="M17" s="49"/>
+      <c r="O17" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="51"/>
+      <c r="P17" s="49"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1896,17 +1968,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="52">
+      <c r="L18" s="50">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="52"/>
-      <c r="O18" s="52">
+      <c r="M18" s="50"/>
+      <c r="O18" s="50">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="52"/>
-      <c r="R18" s="53"/>
+      <c r="P18" s="50"/>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1921,11 +1993,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="52"/>
-      <c r="R19" s="53"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1963,10 +2035,10 @@
       <c r="J23" s="41"/>
       <c r="K23" s="41"/>
       <c r="L23" s="42"/>
-      <c r="N23" s="52" t="s">
+      <c r="N23" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="52"/>
+      <c r="O23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="43"/>
@@ -1980,26 +2052,26 @@
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
       <c r="L24" s="45"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="F26" s="39" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="F26" s="53" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="48" t="s">
+      <c r="K26" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="49"/>
+      <c r="L26" s="48"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2032,7 +2104,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="46"/>
+      <c r="N27" s="54"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -2050,7 +2122,7 @@
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="47"/>
+      <c r="N28" s="55"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -2097,17 +2169,17 @@
       <c r="I33" s="45"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="39"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="49"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -2148,14 +2220,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="F40" s="52" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2205,7 +2277,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="51" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2220,7 +2292,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="51"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2395,28 +2467,28 @@
       <c r="S61" s="45"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="39" t="s">
+      <c r="B63" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="M63" s="39" t="s">
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="53"/>
+      <c r="M63" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="39"/>
-      <c r="O63" s="39"/>
-      <c r="P63" s="39"/>
-      <c r="R63" s="39" t="s">
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="R63" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="39"/>
+      <c r="S63" s="53"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -2509,40 +2581,62 @@
       <c r="S65" s="2"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="51" t="s">
+      <c r="B68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="51"/>
+      <c r="C68" s="49"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="51" t="s">
+      <c r="G68" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="51"/>
+      <c r="H68" s="49"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="52">
+      <c r="B69" s="50">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>24</v>
       </c>
-      <c r="C69" s="52"/>
-      <c r="E69" s="53"/>
-      <c r="G69" s="52">
+      <c r="C69" s="50"/>
+      <c r="E69" s="39"/>
+      <c r="G69" s="50">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>26</v>
       </c>
-      <c r="H69" s="52"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="52"/>
-      <c r="C70" s="52"/>
-      <c r="E70" s="53"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="E70" s="39"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2559,28 +2653,6 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2658,23 +2730,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="49"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2756,28 +2828,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="52">
+      <c r="B10" s="50">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="E10" s="46">
+      <c r="C10" s="50"/>
+      <c r="E10" s="54">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2822,20 +2894,20 @@
       <c r="H15" s="61"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="F17" s="39" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="F17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="J17" s="51" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="J17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="51"/>
+      <c r="K17" s="49"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2859,12 +2931,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="52">
+      <c r="J18" s="50">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="52"/>
-      <c r="M18" s="53">
+      <c r="K18" s="50"/>
+      <c r="M18" s="39">
         <v>5</v>
       </c>
     </row>
@@ -2887,9 +2959,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="M19" s="53"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2940,20 +3012,20 @@
       <c r="K24" s="61"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="E26" s="48" t="s">
+      <c r="C26" s="53"/>
+      <c r="E26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="49"/>
-      <c r="I26" s="39" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2993,7 +3065,7 @@
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="53">
+      <c r="O27" s="39">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3025,7 +3097,7 @@
       </c>
       <c r="M28" s="62"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="53"/>
+      <c r="O28" s="39"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3073,17 +3145,17 @@
       <c r="I33" s="61"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="F35" s="39" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="F35" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3140,14 +3212,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="F40" s="52" t="s">
+      <c r="C40" s="52"/>
+      <c r="F40" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="52"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3203,7 +3275,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="51" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3220,7 +3292,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="51"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3404,27 +3476,27 @@
       <c r="R59" s="61"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="M61" s="39" t="s">
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+      <c r="M61" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-      <c r="Q61" s="39" t="s">
+      <c r="N61" s="53"/>
+      <c r="O61" s="53"/>
+      <c r="Q61" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="39"/>
+      <c r="R61" s="53"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3521,28 +3593,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="51" t="s">
+      <c r="B66" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="51"/>
+      <c r="C66" s="49"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="52">
+      <c r="B67" s="50">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="52"/>
-      <c r="E67" s="53">
+      <c r="C67" s="50"/>
+      <c r="E67" s="39">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="52"/>
-      <c r="C68" s="52"/>
-      <c r="E68" s="53"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="E68" s="39"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3613,10 +3685,10 @@
       <c r="I75" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K75" s="51" t="s">
+      <c r="K75" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="51"/>
+      <c r="L75" s="49"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3646,11 +3718,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="52">
+      <c r="K76" s="50">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="52"/>
+      <c r="L76" s="50"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3678,20 +3750,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -3702,16 +3770,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3720,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
-  <dimension ref="B1:F35"/>
+  <dimension ref="B1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3784,19 +3856,19 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="b">
+      <c r="B5" s="73" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="75">
         <v>45817</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="77" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4169,24 +4241,19 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="31"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="28">
-        <v>45767</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>190</v>
-      </c>
+      <c r="B32" s="68" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="70">
+        <v>45815</v>
+      </c>
+      <c r="E32" s="71" t="s">
+        <v>218</v>
+      </c>
+      <c r="F32" s="72"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="b">
@@ -4196,27 +4263,78 @@
         <v>78</v>
       </c>
       <c r="D34" s="28">
+        <v>45767</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="28">
         <v>45775</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E35" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="b">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C36" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D36" s="20">
         <v>45794</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E36" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F36" s="17" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="20">
+        <v>45797</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="20">
+        <v>45804</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colloquium 2 (MAT3) added to schedule
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF068950-203A-42A1-AF03-542A2F69086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166723B2-D992-4CD2-9CCF-90079B51C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="224">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>Projekt</t>
+  </si>
+  <si>
+    <t>Przekształcenia wektorowe, liniowe, itd..</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,56 +1208,75 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1306,28 +1328,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,60 +1723,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="47"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="45"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="50"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-      <c r="H5" s="46" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="54"/>
+      <c r="H5" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="K5" s="46" t="s">
+      <c r="I5" s="54"/>
+      <c r="K5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="54"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1839,42 +1839,42 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="56"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="56"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="50">
+      <c r="B10" s="57">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>24.7</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="54"/>
-      <c r="G10" s="50">
+        <v>25.7</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="E10" s="51"/>
+      <c r="G10" s="57">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>41.3</v>
-      </c>
-      <c r="H10" s="50"/>
+        <v>40.299999999999997</v>
+      </c>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="E11" s="55"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="E11" s="52"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1899,46 +1899,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="45"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="50"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="H17" s="46" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="H17" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
-      <c r="L17" s="49" t="s">
+      <c r="I17" s="55"/>
+      <c r="J17" s="54"/>
+      <c r="L17" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="49"/>
-      <c r="O17" s="49" t="s">
+      <c r="M17" s="56"/>
+      <c r="O17" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="49"/>
+      <c r="P17" s="56"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1968,17 +1968,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="50">
+      <c r="L18" s="57">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="50"/>
-      <c r="O18" s="50">
+      <c r="M18" s="57"/>
+      <c r="O18" s="57">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="50"/>
-      <c r="R18" s="39"/>
+      <c r="P18" s="57"/>
+      <c r="R18" s="58"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1993,11 +1993,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="R19" s="39"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="R19" s="58"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2022,56 +2022,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="42"/>
-      <c r="N23" s="50" t="s">
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="47"/>
+      <c r="N23" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="50"/>
+      <c r="O23" s="57"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="45"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="50"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="F26" s="53" t="s">
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="F26" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="46" t="s">
+      <c r="K26" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="48"/>
+      <c r="L26" s="54"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="54"/>
+      <c r="N27" s="51"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -2122,7 +2122,7 @@
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="55"/>
+      <c r="N28" s="52"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -2147,39 +2147,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="42"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="47"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="45"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="53"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="54"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -2220,14 +2220,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="F40" s="50" t="s">
+      <c r="C40" s="60"/>
+      <c r="F40" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="50"/>
+      <c r="G40" s="57"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="49" t="s">
+      <c r="I43" s="56" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2292,7 +2292,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="49"/>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2425,70 +2425,70 @@
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="42"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="46"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="46"/>
+      <c r="N60" s="46"/>
+      <c r="O60" s="46"/>
+      <c r="P60" s="46"/>
+      <c r="Q60" s="46"/>
+      <c r="R60" s="46"/>
+      <c r="S60" s="47"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="44"/>
-      <c r="M61" s="44"/>
-      <c r="N61" s="44"/>
-      <c r="O61" s="44"/>
-      <c r="P61" s="44"/>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="44"/>
-      <c r="S61" s="45"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="49"/>
+      <c r="M61" s="49"/>
+      <c r="N61" s="49"/>
+      <c r="O61" s="49"/>
+      <c r="P61" s="49"/>
+      <c r="Q61" s="49"/>
+      <c r="R61" s="49"/>
+      <c r="S61" s="50"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="53" t="s">
+      <c r="B63" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="53"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="53"/>
-      <c r="M63" s="53" t="s">
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
+      <c r="K63" s="44"/>
+      <c r="M63" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="53"/>
-      <c r="O63" s="53"/>
-      <c r="P63" s="53"/>
-      <c r="R63" s="53" t="s">
+      <c r="N63" s="44"/>
+      <c r="O63" s="44"/>
+      <c r="P63" s="44"/>
+      <c r="R63" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="53"/>
+      <c r="S63" s="44"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -2581,62 +2581,40 @@
       <c r="S65" s="2"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="49"/>
+      <c r="C68" s="56"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="49" t="s">
+      <c r="G68" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="49"/>
+      <c r="H68" s="56"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="50">
+      <c r="B69" s="57">
         <f>SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>24</v>
       </c>
-      <c r="C69" s="50"/>
-      <c r="E69" s="39"/>
-      <c r="G69" s="50">
+      <c r="C69" s="57"/>
+      <c r="E69" s="58"/>
+      <c r="G69" s="57">
         <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
         <v>26</v>
       </c>
-      <c r="H69" s="50"/>
+      <c r="H69" s="57"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="E70" s="39"/>
-      <c r="G70" s="50"/>
-      <c r="H70" s="50"/>
+      <c r="B70" s="57"/>
+      <c r="C70" s="57"/>
+      <c r="E70" s="58"/>
+      <c r="G70" s="57"/>
+      <c r="H70" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2653,6 +2631,28 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2693,60 +2693,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="58"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="66"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="54"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2828,28 +2828,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="56"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="50">
+      <c r="B10" s="57">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="54">
+      <c r="C10" s="57"/>
+      <c r="E10" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="E11" s="55"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="E11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2874,40 +2874,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="61"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="F17" s="53" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="F17" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="J17" s="49" t="s">
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="J17" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="49"/>
+      <c r="K17" s="56"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2931,12 +2931,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="50">
+      <c r="J18" s="57">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="M18" s="39">
+      <c r="K18" s="57"/>
+      <c r="M18" s="58">
         <v>5</v>
       </c>
     </row>
@@ -2959,9 +2959,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="M19" s="39"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="M19" s="58"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2986,46 +2986,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="58"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="59"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="61"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="E26" s="46" t="s">
+      <c r="C26" s="44"/>
+      <c r="E26" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
-      <c r="I26" s="53" t="s">
+      <c r="F26" s="55"/>
+      <c r="G26" s="54"/>
+      <c r="I26" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3060,12 +3060,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="62">
+      <c r="M27" s="67">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="39">
+      <c r="O27" s="58">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3095,9 +3095,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="62"/>
+      <c r="M28" s="67"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="39"/>
+      <c r="O28" s="58"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3123,39 +3123,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="63"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="59"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="61"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="66"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="F35" s="53" t="s">
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="F35" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3212,14 +3212,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="F40" s="50" t="s">
+      <c r="C40" s="60"/>
+      <c r="F40" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="50"/>
+      <c r="G40" s="57"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3275,7 +3275,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="49" t="s">
+      <c r="I43" s="56" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3292,7 +3292,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="49"/>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3436,67 +3436,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="57"/>
-      <c r="O58" s="57"/>
-      <c r="P58" s="57"/>
-      <c r="Q58" s="57"/>
-      <c r="R58" s="58"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="62"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="62"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="62"/>
+      <c r="P58" s="62"/>
+      <c r="Q58" s="62"/>
+      <c r="R58" s="63"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="59"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="60"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="60"/>
-      <c r="N59" s="60"/>
-      <c r="O59" s="60"/>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="60"/>
-      <c r="R59" s="61"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
+      <c r="J59" s="65"/>
+      <c r="K59" s="65"/>
+      <c r="L59" s="65"/>
+      <c r="M59" s="65"/>
+      <c r="N59" s="65"/>
+      <c r="O59" s="65"/>
+      <c r="P59" s="65"/>
+      <c r="Q59" s="65"/>
+      <c r="R59" s="66"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="53"/>
-      <c r="M61" s="53" t="s">
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="M61" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="53"/>
-      <c r="O61" s="53"/>
-      <c r="Q61" s="53" t="s">
+      <c r="N61" s="44"/>
+      <c r="O61" s="44"/>
+      <c r="Q61" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="53"/>
+      <c r="R61" s="44"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3593,28 +3593,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="56"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="50">
+      <c r="B67" s="57">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="50"/>
-      <c r="E67" s="39">
+      <c r="C67" s="57"/>
+      <c r="E67" s="58">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="E68" s="39"/>
+      <c r="B68" s="57"/>
+      <c r="C68" s="57"/>
+      <c r="E68" s="58"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3639,26 +3639,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="56" t="s">
+      <c r="B72" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="57"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="58"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="62"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="63"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="59"/>
-      <c r="C73" s="60"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
-      <c r="H73" s="60"/>
-      <c r="I73" s="61"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="65"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="66"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3685,10 +3685,10 @@
       <c r="I75" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K75" s="49" t="s">
+      <c r="K75" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="49"/>
+      <c r="L75" s="56"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3718,11 +3718,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="50">
+      <c r="K76" s="57">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="50"/>
+      <c r="L76" s="57"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3750,6 +3750,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B23:K24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B72:I73"/>
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="K76:L76"/>
@@ -3760,30 +3784,6 @@
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B23:K24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3792,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
-  <dimension ref="B1:F39"/>
+  <dimension ref="B1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,19 +3856,19 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="b">
+      <c r="B5" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="41">
         <v>45817</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="43" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4241,35 +4241,34 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="68" t="b">
+      <c r="B32" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="70">
+      <c r="D32" s="20">
         <v>45815</v>
       </c>
-      <c r="E32" s="71" t="s">
+      <c r="E32" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="F32" s="72"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="28">
-        <v>45767</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>190</v>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="73" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="75">
+        <v>45764</v>
+      </c>
+      <c r="E33" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="F33" s="76" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -4280,44 +4279,44 @@
         <v>78</v>
       </c>
       <c r="D35" s="28">
+        <v>45767</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="28">
         <v>45775</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E36" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="21" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D37" s="28">
         <v>45794</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E37" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F37" s="27" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="20">
-        <v>45797</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -4328,12 +4327,29 @@
         <v>79</v>
       </c>
       <c r="D39" s="20">
+        <v>45797</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="20">
         <v>45804</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E40" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F40" s="17" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4367,21 +4383,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="63" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="70"/>
+      <c r="F2" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="J2" s="63" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="J2" s="68" t="s">
         <v>205</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4556,26 +4572,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="67"/>
+      <c r="G11" s="72"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="72"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - PBL2 - and new grade - labs FIZ1
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A26558-A96B-4669-95AE-8FBBB8B239D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF09843-948A-4068-B4D0-581168967817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="226">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -714,6 +714,9 @@
   </si>
   <si>
     <t>Kolos</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -839,6 +842,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -1089,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1230,6 +1245,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1315,6 +1336,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1678,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1725,7 @@
     <col min="13" max="13" width="15.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="14.28515625" style="1" customWidth="1"/>
@@ -1710,60 +1734,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="48"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="52"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="54"/>
-      <c r="H5" s="53" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="56"/>
+      <c r="H5" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="K5" s="53" t="s">
+      <c r="I5" s="56"/>
+      <c r="K5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="54"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1831,37 +1855,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="56"/>
+      <c r="C9" s="58"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="57">
+      <c r="B10" s="59">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>25.7</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="E10" s="51"/>
-      <c r="G10" s="57">
+      <c r="C10" s="59"/>
+      <c r="E10" s="53"/>
+      <c r="G10" s="59">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>40.299999999999997</v>
       </c>
-      <c r="H10" s="57"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="E11" s="52"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="E11" s="54"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1886,46 +1910,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="H17" s="53" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="H17" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="54"/>
-      <c r="L17" s="56" t="s">
+      <c r="I17" s="57"/>
+      <c r="J17" s="56"/>
+      <c r="L17" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="56"/>
-      <c r="O17" s="56" t="s">
+      <c r="M17" s="58"/>
+      <c r="O17" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="56"/>
+      <c r="P17" s="58"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1955,17 +1979,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="57">
+      <c r="L18" s="59">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="57"/>
-      <c r="O18" s="57">
+      <c r="M18" s="59"/>
+      <c r="O18" s="59">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="57"/>
-      <c r="R18" s="58"/>
+      <c r="P18" s="59"/>
+      <c r="R18" s="60"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1980,11 +2004,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="57"/>
-      <c r="R19" s="58"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="R19" s="60"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2009,56 +2033,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-      <c r="N23" s="57" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="49"/>
+      <c r="N23" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="57"/>
+      <c r="O23" s="59"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="50"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="52"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="F26" s="44" t="s">
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="F26" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="53" t="s">
+      <c r="K26" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="54"/>
+      <c r="L26" s="56"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2091,7 +2115,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="51"/>
+      <c r="N27" s="53"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -2107,526 +2131,550 @@
       <c r="G28" s="2">
         <v>5</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2">
+        <v>4.5</v>
+      </c>
       <c r="I28" s="2">
         <v>5</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="52"/>
-    </row>
-    <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="45" t="s">
+      <c r="N28" s="54"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="F29" s="45">
+        <v>5</v>
+      </c>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="N29" s="44"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47"/>
-    </row>
-    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="44" t="s">
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="49"/>
+    </row>
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="52"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="53" t="s">
+      <c r="C36" s="46"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="54"/>
-    </row>
-    <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="56"/>
+    </row>
+    <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
         <v>17</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="E37" s="2">
-        <f>C56</f>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2">
+        <f>C57</f>
         <v>15</v>
       </c>
-      <c r="F37" s="2">
-        <f>G51</f>
+      <c r="F38" s="2">
+        <f>G52</f>
         <v>9</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="O37" s="7"/>
-    </row>
-    <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="59" t="s">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="F40" s="57" t="s">
+      <c r="C41" s="62"/>
+      <c r="F41" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="57"/>
-      <c r="I40" s="9" t="s">
+      <c r="G41" s="59"/>
+      <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J40" s="11"/>
-      <c r="L40" s="11"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G41" s="2">
-        <v>9</v>
-      </c>
-      <c r="I41" s="2">
-        <f>SUM(B37:C37,E37:H37)</f>
-        <v>41</v>
-      </c>
-      <c r="J41" s="7"/>
-      <c r="L41" s="7"/>
+      <c r="J41" s="11"/>
+      <c r="L41" s="11"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
       <c r="F42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="I42" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="G42" s="2">
+        <v>9</v>
+      </c>
+      <c r="I42" s="2">
+        <f>SUM(B38:C38,E38:H38)</f>
+        <v>41</v>
+      </c>
       <c r="J42" s="7"/>
+      <c r="L42" s="7"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="2">
-        <v>3</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="56" t="s">
-        <v>67</v>
-      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C44" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="56"/>
+      <c r="I44" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="2">
         <v>4</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="I45" s="13"/>
+      <c r="I45" s="58"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="C46" s="2">
+        <v>4</v>
+      </c>
       <c r="F46" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G46" s="2"/>
+      <c r="I46" s="13"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G47" s="2"/>
-      <c r="I47" s="9" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="2">
-        <v>2</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="I48" s="2">
-        <f>50-SUM(B37:C37,E37:H37)</f>
-        <v>9</v>
+      <c r="I48" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2</v>
+      </c>
       <c r="F49" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G49" s="2"/>
+      <c r="I49" s="2">
+        <f>50-SUM(B38:C38,E38:H38)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="F51" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G51" s="2">
-        <f>SUM(G41:G49)</f>
-        <v>9</v>
-      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2"/>
+      <c r="F52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="2">
+        <f>SUM(G42:G50)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="2">
-        <f>SUM(C41:C54)</f>
+      <c r="C57" s="2">
+        <f>SUM(C42:C55)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6"/>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
-      <c r="S58" s="6"/>
-    </row>
-    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="45" t="s">
+    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+    </row>
+    <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="46"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="46"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="46"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="46"/>
-      <c r="P60" s="46"/>
-      <c r="Q60" s="46"/>
-      <c r="R60" s="46"/>
-      <c r="S60" s="47"/>
-    </row>
-    <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="48"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-      <c r="N61" s="49"/>
-      <c r="O61" s="49"/>
-      <c r="P61" s="49"/>
-      <c r="Q61" s="49"/>
-      <c r="R61" s="49"/>
-      <c r="S61" s="50"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="44" t="s">
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
+      <c r="P61" s="48"/>
+      <c r="Q61" s="48"/>
+      <c r="R61" s="48"/>
+      <c r="S61" s="49"/>
+    </row>
+    <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="51"/>
+      <c r="O62" s="51"/>
+      <c r="P62" s="51"/>
+      <c r="Q62" s="51"/>
+      <c r="R62" s="51"/>
+      <c r="S62" s="52"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B64" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="44"/>
-      <c r="M63" s="44" t="s">
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="46"/>
+      <c r="K64" s="46"/>
+      <c r="M64" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="44"/>
-      <c r="O63" s="44"/>
-      <c r="P63" s="44"/>
-      <c r="R63" s="44" t="s">
+      <c r="N64" s="46"/>
+      <c r="O64" s="46"/>
+      <c r="P64" s="46"/>
+      <c r="R64" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="44"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
+      <c r="S64" s="46"/>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I65" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="K65" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M64" s="2" t="s">
+      <c r="M65" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="N65" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O64" s="2" t="s">
+      <c r="O65" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="P65" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R64" s="2" t="s">
+      <c r="R65" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S64" s="2" t="s">
+      <c r="S65" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B65" s="2">
+    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
         <v>2</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C66" s="2">
         <v>2</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D66" s="2">
         <v>2</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E66" s="2">
         <v>2</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H66" s="2">
         <v>2</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I66" s="2">
         <v>2</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J66" s="2">
         <v>2</v>
       </c>
-      <c r="K65" s="2"/>
-      <c r="M65" s="2">
+      <c r="K66" s="2"/>
+      <c r="M66" s="2">
         <v>5</v>
       </c>
-      <c r="N65" s="2">
+      <c r="N66" s="2">
         <v>5</v>
       </c>
-      <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
-      <c r="R65" s="2"/>
-      <c r="S65" s="2"/>
-    </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="56" t="s">
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="R66" s="2"/>
+      <c r="S66" s="2"/>
+    </row>
+    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="56"/>
-      <c r="E68" s="9" t="s">
+      <c r="C69" s="58"/>
+      <c r="E69" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="56" t="s">
+      <c r="G69" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="56"/>
-    </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="57">
-        <f>SUM(B65:K65,M65:P65,R65:S65)</f>
-        <v>24</v>
-      </c>
-      <c r="C69" s="57"/>
-      <c r="E69" s="58"/>
-      <c r="G69" s="57">
-        <f>50-SUM(B65:K65,M65:P65,R65:S65)</f>
-        <v>26</v>
-      </c>
-      <c r="H69" s="57"/>
+      <c r="H69" s="58"/>
+      <c r="K69" s="75" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="57"/>
-      <c r="C70" s="57"/>
-      <c r="E70" s="58"/>
-      <c r="G70" s="57"/>
-      <c r="H70" s="57"/>
+      <c r="B70" s="59">
+        <f>SUM(B66:K66,M66:P66,R66:S66,K70)</f>
+        <v>27</v>
+      </c>
+      <c r="C70" s="59"/>
+      <c r="E70" s="60"/>
+      <c r="G70" s="59">
+        <f>50-SUM(B66:K66,M66:P66,R66:S66,K70)</f>
+        <v>23</v>
+      </c>
+      <c r="H70" s="59"/>
+      <c r="K70" s="59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B71" s="59"/>
+      <c r="C71" s="59"/>
+      <c r="E71" s="60"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="K71" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="42">
+    <mergeCell ref="K70:K71"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B2:P3"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="L18:M19"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="N23:O24"/>
     <mergeCell ref="O18:P19"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C71"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H71"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="O17:P17"/>
@@ -2639,11 +2687,14 @@
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="B23:L24"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="B61:S62"/>
+    <mergeCell ref="M64:P64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2684,60 +2735,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="68"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="54"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2819,28 +2870,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="56"/>
+      <c r="C9" s="58"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="57">
+      <c r="B10" s="59">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="E10" s="51">
+      <c r="C10" s="59"/>
+      <c r="E10" s="53">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="E11" s="54"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2865,40 +2916,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="F17" s="44" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="F17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="J17" s="56" t="s">
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="J17" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="56"/>
+      <c r="K17" s="58"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2922,12 +2973,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="57">
+      <c r="J18" s="59">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="M18" s="58">
+      <c r="K18" s="59"/>
+      <c r="M18" s="60">
         <v>5</v>
       </c>
     </row>
@@ -2950,9 +3001,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="M19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="M19" s="60"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2977,46 +3028,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="65"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="64"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="66"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="E26" s="53" t="s">
+      <c r="C26" s="46"/>
+      <c r="E26" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="55"/>
-      <c r="G26" s="54"/>
-      <c r="I26" s="44" t="s">
+      <c r="F26" s="57"/>
+      <c r="G26" s="56"/>
+      <c r="I26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3051,12 +3102,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="67">
+      <c r="M27" s="69">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="58">
+      <c r="O27" s="60">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3086,9 +3137,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="67"/>
+      <c r="M28" s="69"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="58"/>
+      <c r="O28" s="60"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3114,39 +3165,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="65"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="64"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="F35" s="44" t="s">
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="F35" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3203,14 +3254,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="F40" s="57" t="s">
+      <c r="C40" s="62"/>
+      <c r="F40" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="57"/>
+      <c r="G40" s="59"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3266,7 +3317,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="56" t="s">
+      <c r="I43" s="58" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3283,7 +3334,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="56"/>
+      <c r="I44" s="58"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3427,67 +3478,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="63" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="62"/>
-      <c r="D58" s="62"/>
-      <c r="E58" s="62"/>
-      <c r="F58" s="62"/>
-      <c r="G58" s="62"/>
-      <c r="H58" s="62"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="62"/>
-      <c r="K58" s="62"/>
-      <c r="L58" s="62"/>
-      <c r="M58" s="62"/>
-      <c r="N58" s="62"/>
-      <c r="O58" s="62"/>
-      <c r="P58" s="62"/>
-      <c r="Q58" s="62"/>
-      <c r="R58" s="63"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="64"/>
+      <c r="H58" s="64"/>
+      <c r="I58" s="64"/>
+      <c r="J58" s="64"/>
+      <c r="K58" s="64"/>
+      <c r="L58" s="64"/>
+      <c r="M58" s="64"/>
+      <c r="N58" s="64"/>
+      <c r="O58" s="64"/>
+      <c r="P58" s="64"/>
+      <c r="Q58" s="64"/>
+      <c r="R58" s="65"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="64"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
-      <c r="J59" s="65"/>
-      <c r="K59" s="65"/>
-      <c r="L59" s="65"/>
-      <c r="M59" s="65"/>
-      <c r="N59" s="65"/>
-      <c r="O59" s="65"/>
-      <c r="P59" s="65"/>
-      <c r="Q59" s="65"/>
-      <c r="R59" s="66"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="67"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="67"/>
+      <c r="G59" s="67"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="67"/>
+      <c r="J59" s="67"/>
+      <c r="K59" s="67"/>
+      <c r="L59" s="67"/>
+      <c r="M59" s="67"/>
+      <c r="N59" s="67"/>
+      <c r="O59" s="67"/>
+      <c r="P59" s="67"/>
+      <c r="Q59" s="67"/>
+      <c r="R59" s="68"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
-      <c r="M61" s="44" t="s">
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="M61" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="44"/>
-      <c r="O61" s="44"/>
-      <c r="Q61" s="44" t="s">
+      <c r="N61" s="46"/>
+      <c r="O61" s="46"/>
+      <c r="Q61" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="44"/>
+      <c r="R61" s="46"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3584,28 +3635,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="56"/>
+      <c r="C66" s="58"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="57">
+      <c r="B67" s="59">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="57"/>
-      <c r="E67" s="58">
+      <c r="C67" s="59"/>
+      <c r="E67" s="60">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
-      <c r="E68" s="58"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="59"/>
+      <c r="E68" s="60"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3630,26 +3681,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="61" t="s">
+      <c r="B72" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="62"/>
-      <c r="F72" s="62"/>
-      <c r="G72" s="62"/>
-      <c r="H72" s="62"/>
-      <c r="I72" s="63"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="66"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="67"/>
+      <c r="H73" s="67"/>
+      <c r="I73" s="68"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3676,10 +3727,10 @@
       <c r="I75" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K75" s="56" t="s">
+      <c r="K75" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="56"/>
+      <c r="L75" s="58"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3709,11 +3760,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="57">
+      <c r="K76" s="59">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="57"/>
+      <c r="L76" s="59"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -4391,21 +4442,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="70"/>
-      <c r="F2" s="68" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
+      <c r="F2" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="J2" s="68" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
+      <c r="J2" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="72"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4580,26 +4631,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="72"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="71" t="s">
+      <c r="J11" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="72"/>
+      <c r="K11" s="74"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
POTEC - new points -> passed
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF09843-948A-4068-B4D0-581168967817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B41023-C553-44AC-BF28-ADE8015752C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="226">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -1104,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1248,10 +1248,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1272,28 +1275,16 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1302,6 +1293,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1338,7 +1341,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1704,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,59 +1758,59 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="52"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="56"/>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="54" t="s">
         <v>82</v>
       </c>
       <c r="I5" s="56"/>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
       <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
@@ -1855,37 +1879,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="57"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="58"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="59">
+      <c r="B10" s="46">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>25.7</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="E10" s="53"/>
-      <c r="G10" s="59">
+      <c r="C10" s="46"/>
+      <c r="E10" s="61"/>
+      <c r="G10" s="46">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>40.299999999999997</v>
       </c>
-      <c r="H10" s="59"/>
+      <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="E11" s="54"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="62"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1910,46 +1934,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="H17" s="55" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="H17" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="57"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="56"/>
-      <c r="L17" s="58" t="s">
+      <c r="L17" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="58"/>
-      <c r="O17" s="58" t="s">
+      <c r="M17" s="57"/>
+      <c r="O17" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="58"/>
+      <c r="P17" s="57"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1979,17 +2003,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="59">
+      <c r="L18" s="46">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>29.5</v>
       </c>
-      <c r="M18" s="59"/>
-      <c r="O18" s="59">
+      <c r="M18" s="46"/>
+      <c r="O18" s="46">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>20.5</v>
       </c>
-      <c r="P18" s="59"/>
-      <c r="R18" s="60"/>
+      <c r="P18" s="46"/>
+      <c r="R18" s="47"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -2004,11 +2028,11 @@
         <v>26.5</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="R19" s="60"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="R19" s="47"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2033,53 +2057,53 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="49"/>
-      <c r="N23" s="59" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
+      <c r="N23" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="59"/>
+      <c r="O23" s="46"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="52"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="53"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="F26" s="46" t="s">
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="F26" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="55" t="s">
+      <c r="K26" s="54" t="s">
         <v>128</v>
       </c>
       <c r="L26" s="56"/>
@@ -2115,7 +2139,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="53"/>
+      <c r="N27" s="61"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -2139,20 +2163,20 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="54"/>
+      <c r="N28" s="62"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="F29" s="45">
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="F29" s="63">
         <v>5</v>
       </c>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
       <c r="N29" s="44"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2178,38 +2202,38 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="49"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="78"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="50"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="52"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="81"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="46"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
       <c r="H36" s="56"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,25 +2264,25 @@
       <c r="C38" s="2"/>
       <c r="E38" s="2">
         <f>C57</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F38" s="2">
         <f>G52</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="F41" s="59" t="s">
+      <c r="C41" s="59"/>
+      <c r="F41" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="59"/>
+      <c r="G41" s="46"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -2280,7 +2304,7 @@
       </c>
       <c r="I42" s="2">
         <f>SUM(B38:C38,E38:H38)</f>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="J42" s="7"/>
       <c r="L42" s="7"/>
@@ -2293,7 +2317,9 @@
       <c r="F43" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2">
+        <v>10</v>
+      </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
@@ -2308,7 +2334,7 @@
         <v>119</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="58" t="s">
+      <c r="I44" s="57" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2323,7 +2349,7 @@
         <v>120</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="I45" s="58"/>
+      <c r="I45" s="57"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2336,7 +2362,9 @@
         <v>121</v>
       </c>
       <c r="G46" s="2"/>
-      <c r="I46" s="13"/>
+      <c r="I46" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
@@ -2357,9 +2385,7 @@
         <v>123</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="I48" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="I48" s="82"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
@@ -2372,10 +2398,7 @@
         <v>124</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="I49" s="2">
-        <f>50-SUM(B38:C38,E38:H38)</f>
-        <v>9</v>
-      </c>
+      <c r="I49" s="83"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
@@ -2391,7 +2414,9 @@
       <c r="B51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
@@ -2403,7 +2428,7 @@
       </c>
       <c r="G52" s="2">
         <f>SUM(G42:G50)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
@@ -2430,7 +2455,7 @@
       </c>
       <c r="C57" s="2">
         <f>SUM(C42:C55)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2456,70 +2481,70 @@
     </row>
     <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
-      <c r="M61" s="48"/>
-      <c r="N61" s="48"/>
-      <c r="O61" s="48"/>
-      <c r="P61" s="48"/>
-      <c r="Q61" s="48"/>
-      <c r="R61" s="48"/>
-      <c r="S61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="49"/>
+      <c r="M61" s="49"/>
+      <c r="N61" s="49"/>
+      <c r="O61" s="49"/>
+      <c r="P61" s="49"/>
+      <c r="Q61" s="49"/>
+      <c r="R61" s="49"/>
+      <c r="S61" s="50"/>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="50"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="51"/>
-      <c r="K62" s="51"/>
-      <c r="L62" s="51"/>
-      <c r="M62" s="51"/>
-      <c r="N62" s="51"/>
-      <c r="O62" s="51"/>
-      <c r="P62" s="51"/>
-      <c r="Q62" s="51"/>
-      <c r="R62" s="51"/>
-      <c r="S62" s="52"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="52"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
+      <c r="Q62" s="52"/>
+      <c r="R62" s="52"/>
+      <c r="S62" s="53"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="46"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="46"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="46"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="46"/>
-      <c r="M64" s="46" t="s">
+      <c r="C64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="60"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="60"/>
+      <c r="J64" s="60"/>
+      <c r="K64" s="60"/>
+      <c r="M64" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="N64" s="46"/>
-      <c r="O64" s="46"/>
-      <c r="P64" s="46"/>
-      <c r="R64" s="46" t="s">
+      <c r="N64" s="60"/>
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="R64" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="S64" s="46"/>
+      <c r="S64" s="60"/>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
@@ -2612,47 +2637,73 @@
       <c r="S66" s="2"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C69" s="58"/>
+      <c r="C69" s="57"/>
       <c r="E69" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="58" t="s">
+      <c r="G69" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="H69" s="58"/>
-      <c r="K69" s="75" t="s">
+      <c r="H69" s="57"/>
+      <c r="K69" s="45" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="59">
+      <c r="B70" s="46">
         <f>SUM(B66:K66,M66:P66,R66:S66,K70)</f>
         <v>27</v>
       </c>
-      <c r="C70" s="59"/>
-      <c r="E70" s="60"/>
-      <c r="G70" s="59">
+      <c r="C70" s="46"/>
+      <c r="E70" s="47"/>
+      <c r="G70" s="46">
         <f>50-SUM(B66:K66,M66:P66,R66:S66,K70)</f>
         <v>23</v>
       </c>
-      <c r="H70" s="59"/>
-      <c r="K70" s="59">
+      <c r="H70" s="46"/>
+      <c r="K70" s="46">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B71" s="59"/>
-      <c r="C71" s="59"/>
-      <c r="E71" s="60"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="59"/>
-      <c r="K71" s="59"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="E71" s="47"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="46"/>
+      <c r="K71" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="B61:S62"/>
+    <mergeCell ref="M64:P64"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C71"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H71"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="K70:K71"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
@@ -2669,32 +2720,6 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C71"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H71"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="B33:I34"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="B61:S62"/>
-    <mergeCell ref="M64:P64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2735,59 +2760,59 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="66"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="68"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="69"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
       <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
@@ -2870,28 +2895,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="57"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="59">
+      <c r="B10" s="46">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="E10" s="53">
+      <c r="C10" s="46"/>
+      <c r="E10" s="61">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="E11" s="54"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="62"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2916,40 +2941,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="F17" s="46" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="F17" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="J17" s="58" t="s">
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="J17" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="58"/>
+      <c r="K17" s="57"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2973,12 +2998,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="59">
+      <c r="J18" s="46">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="59"/>
-      <c r="M18" s="60">
+      <c r="K18" s="46"/>
+      <c r="M18" s="47">
         <v>5</v>
       </c>
     </row>
@@ -3001,9 +3026,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="M19" s="60"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="M19" s="47"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3028,46 +3053,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="66"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="66"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="68"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="E26" s="55" t="s">
+      <c r="C26" s="60"/>
+      <c r="E26" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="57"/>
+      <c r="F26" s="55"/>
       <c r="G26" s="56"/>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3102,12 +3127,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="69">
+      <c r="M27" s="70">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="60">
+      <c r="O27" s="47">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3137,9 +3162,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="69"/>
+      <c r="M28" s="70"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="60"/>
+      <c r="O28" s="47"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3165,39 +3190,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="66"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="66"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="68"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="69"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="F35" s="46" t="s">
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="F35" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3254,14 +3279,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="F40" s="59" t="s">
+      <c r="C40" s="59"/>
+      <c r="F40" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="59"/>
+      <c r="G40" s="46"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3317,7 +3342,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="58" t="s">
+      <c r="I43" s="57" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3334,7 +3359,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="58"/>
+      <c r="I44" s="57"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3478,67 +3503,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="63" t="s">
+      <c r="B58" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="64"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
-      <c r="K58" s="64"/>
-      <c r="L58" s="64"/>
-      <c r="M58" s="64"/>
-      <c r="N58" s="64"/>
-      <c r="O58" s="64"/>
-      <c r="P58" s="64"/>
-      <c r="Q58" s="64"/>
-      <c r="R58" s="65"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="65"/>
+      <c r="K58" s="65"/>
+      <c r="L58" s="65"/>
+      <c r="M58" s="65"/>
+      <c r="N58" s="65"/>
+      <c r="O58" s="65"/>
+      <c r="P58" s="65"/>
+      <c r="Q58" s="65"/>
+      <c r="R58" s="66"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="66"/>
-      <c r="C59" s="67"/>
-      <c r="D59" s="67"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="67"/>
-      <c r="G59" s="67"/>
-      <c r="H59" s="67"/>
-      <c r="I59" s="67"/>
-      <c r="J59" s="67"/>
-      <c r="K59" s="67"/>
-      <c r="L59" s="67"/>
-      <c r="M59" s="67"/>
-      <c r="N59" s="67"/>
-      <c r="O59" s="67"/>
-      <c r="P59" s="67"/>
-      <c r="Q59" s="67"/>
-      <c r="R59" s="68"/>
+      <c r="B59" s="67"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="68"/>
+      <c r="I59" s="68"/>
+      <c r="J59" s="68"/>
+      <c r="K59" s="68"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="68"/>
+      <c r="N59" s="68"/>
+      <c r="O59" s="68"/>
+      <c r="P59" s="68"/>
+      <c r="Q59" s="68"/>
+      <c r="R59" s="69"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="M61" s="46" t="s">
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
+      <c r="M61" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="46"/>
-      <c r="O61" s="46"/>
-      <c r="Q61" s="46" t="s">
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
+      <c r="Q61" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="46"/>
+      <c r="R61" s="60"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3635,28 +3660,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="58" t="s">
+      <c r="B66" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="58"/>
+      <c r="C66" s="57"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="59">
+      <c r="B67" s="46">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="59"/>
-      <c r="E67" s="60">
+      <c r="C67" s="46"/>
+      <c r="E67" s="47">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="59"/>
-      <c r="C68" s="59"/>
-      <c r="E68" s="60"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="E68" s="47"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3681,26 +3706,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
-      <c r="H72" s="64"/>
-      <c r="I72" s="65"/>
+      <c r="C72" s="65"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="65"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="66"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="66"/>
-      <c r="C73" s="67"/>
-      <c r="D73" s="67"/>
-      <c r="E73" s="67"/>
-      <c r="F73" s="67"/>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
-      <c r="I73" s="68"/>
+      <c r="B73" s="67"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="68"/>
+      <c r="H73" s="68"/>
+      <c r="I73" s="69"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3727,10 +3752,10 @@
       <c r="I75" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K75" s="58" t="s">
+      <c r="K75" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="58"/>
+      <c r="L75" s="57"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3760,11 +3785,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="59">
+      <c r="K76" s="46">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="59"/>
+      <c r="L76" s="46"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3792,20 +3817,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -3816,16 +3837,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4442,21 +4467,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
-      <c r="F2" s="70" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="73"/>
+      <c r="F2" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
-      <c r="J2" s="70" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="J2" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="K2" s="71"/>
-      <c r="L2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="73"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4631,26 +4656,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="74"/>
+      <c r="G11" s="75"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="73" t="s">
+      <c r="J11" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="74"/>
+      <c r="K11" s="75"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - FIZ1 passed!
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B41023-C553-44AC-BF28-ADE8015752C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374CC67-EA74-4F6A-AC75-6B427581DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="225">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -428,12 +428,6 @@
     <t>Egzamin [20+10 pkt]</t>
   </si>
   <si>
-    <t>Ćwiczenia [C = 0,6K+0,4P]</t>
-  </si>
-  <si>
-    <t>Mini-projekt</t>
-  </si>
-  <si>
     <t>W = 0,4E + 0,3C + 0,3L</t>
   </si>
   <si>
@@ -717,6 +711,9 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>Mini-projekt [10 pkt]</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1305,6 +1302,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1339,30 +1354,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1728,15 +1719,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
@@ -1818,25 +1809,25 @@
     </row>
     <row r="6" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
@@ -1980,13 +1971,13 @@
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>92</v>
@@ -2057,47 +2048,53 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="50"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="66"/>
       <c r="N23" s="46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O23" s="46"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="53"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="69"/>
       <c r="N24" s="46"/>
       <c r="O24" s="46"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="60" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="C26" s="60"/>
       <c r="D26" s="60"/>
       <c r="F26" s="60" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G26" s="60"/>
       <c r="H26" s="60"/>
@@ -2113,25 +2110,25 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>130</v>
+        <v>224</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="H27" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>73</v>
@@ -2139,13 +2136,18 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="61"/>
+      <c r="N27" s="61">
+        <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
+        <v>4.2133333333333329</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>13</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>10</v>
+      </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
@@ -2161,12 +2163,17 @@
       <c r="I28" s="2">
         <v>5</v>
       </c>
-      <c r="K28" s="2"/>
+      <c r="K28" s="2">
+        <v>20</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="N28" s="62"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="63"/>
+      <c r="B29" s="63">
+        <f>SUM(B28:C28)</f>
+        <v>23</v>
+      </c>
       <c r="C29" s="63"/>
       <c r="D29" s="63"/>
       <c r="F29" s="63">
@@ -2175,7 +2182,10 @@
       <c r="G29" s="63"/>
       <c r="H29" s="63"/>
       <c r="I29" s="63"/>
-      <c r="K29" s="63"/>
+      <c r="K29" s="63">
+        <f>SUM(K28:L28)</f>
+        <v>20</v>
+      </c>
       <c r="L29" s="63"/>
       <c r="N29" s="44"/>
     </row>
@@ -2202,26 +2212,26 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="78"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="66"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="79"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="81"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="69"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="60" t="s">
@@ -2230,7 +2240,7 @@
       <c r="C36" s="60"/>
       <c r="D36" s="7"/>
       <c r="E36" s="54" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F36" s="55"/>
       <c r="G36" s="55"/>
@@ -2385,7 +2395,7 @@
         <v>123</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="I48" s="82"/>
+      <c r="I48" s="44"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
@@ -2398,7 +2408,6 @@
         <v>124</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="I49" s="83"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
@@ -2572,7 +2581,7 @@
         <v>81</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>85</v>
@@ -2610,10 +2619,10 @@
         <v>2</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H66" s="2">
         <v>2</v>
@@ -2624,7 +2633,9 @@
       <c r="J66" s="2">
         <v>2</v>
       </c>
-      <c r="K66" s="2"/>
+      <c r="K66" s="2">
+        <v>2</v>
+      </c>
       <c r="M66" s="2">
         <v>5</v>
       </c>
@@ -2649,19 +2660,19 @@
       </c>
       <c r="H69" s="57"/>
       <c r="K69" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B70" s="46">
         <f>SUM(B66:K66,M66:P66,R66:S66,K70)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C70" s="46"/>
       <c r="E70" s="47"/>
       <c r="G70" s="46">
         <f>50-SUM(B66:K66,M66:P66,R66:S66,K70)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H70" s="46"/>
       <c r="K70" s="46">
@@ -2684,6 +2695,8 @@
     <mergeCell ref="B64:K64"/>
     <mergeCell ref="B61:S62"/>
     <mergeCell ref="M64:P64"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="K26:L26"/>
@@ -2695,15 +2708,13 @@
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:H11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
     <mergeCell ref="E70:E71"/>
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="B70:C71"/>
     <mergeCell ref="G69:H69"/>
     <mergeCell ref="G70:H71"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
     <mergeCell ref="K70:K71"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
@@ -2760,40 +2771,40 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="66"/>
+      <c r="B2" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="72"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="67"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="75"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2941,24 +2952,24 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="64" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
+      <c r="B14" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="69"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="75"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
@@ -3053,30 +3064,30 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
+      <c r="B23" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="72"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="69"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="75"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="60" t="s">
@@ -3127,7 +3138,7 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="70">
+      <c r="M27" s="76">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
@@ -3162,7 +3173,7 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="70"/>
+      <c r="M28" s="76"/>
       <c r="N28" s="7"/>
       <c r="O28" s="47"/>
       <c r="P28" s="8"/>
@@ -3190,26 +3201,26 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="66"/>
+      <c r="B32" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="67"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="69"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="60" t="s">
@@ -3503,44 +3514,44 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="64" t="s">
-        <v>136</v>
-      </c>
-      <c r="C58" s="65"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-      <c r="I58" s="65"/>
-      <c r="J58" s="65"/>
-      <c r="K58" s="65"/>
-      <c r="L58" s="65"/>
-      <c r="M58" s="65"/>
-      <c r="N58" s="65"/>
-      <c r="O58" s="65"/>
-      <c r="P58" s="65"/>
-      <c r="Q58" s="65"/>
-      <c r="R58" s="66"/>
+      <c r="B58" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="71"/>
+      <c r="G58" s="71"/>
+      <c r="H58" s="71"/>
+      <c r="I58" s="71"/>
+      <c r="J58" s="71"/>
+      <c r="K58" s="71"/>
+      <c r="L58" s="71"/>
+      <c r="M58" s="71"/>
+      <c r="N58" s="71"/>
+      <c r="O58" s="71"/>
+      <c r="P58" s="71"/>
+      <c r="Q58" s="71"/>
+      <c r="R58" s="72"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="67"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="68"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="68"/>
-      <c r="J59" s="68"/>
-      <c r="K59" s="68"/>
-      <c r="L59" s="68"/>
-      <c r="M59" s="68"/>
-      <c r="N59" s="68"/>
-      <c r="O59" s="68"/>
-      <c r="P59" s="68"/>
-      <c r="Q59" s="68"/>
-      <c r="R59" s="69"/>
+      <c r="B59" s="73"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="74"/>
+      <c r="K59" s="74"/>
+      <c r="L59" s="74"/>
+      <c r="M59" s="74"/>
+      <c r="N59" s="74"/>
+      <c r="O59" s="74"/>
+      <c r="P59" s="74"/>
+      <c r="Q59" s="74"/>
+      <c r="R59" s="75"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="60" t="s">
@@ -3706,51 +3717,51 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
-      <c r="I72" s="66"/>
+      <c r="B72" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="72"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="67"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
-      <c r="I73" s="69"/>
+      <c r="B73" s="73"/>
+      <c r="C73" s="74"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="74"/>
+      <c r="G73" s="74"/>
+      <c r="H73" s="74"/>
+      <c r="I73" s="75"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="I75" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="K75" s="57" t="s">
         <v>22</v>
@@ -3876,16 +3887,16 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3899,10 +3910,10 @@
         <v>45763</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -3916,10 +3927,10 @@
         <v>45803</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -3933,10 +3944,10 @@
         <v>45817</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -3956,7 +3967,7 @@
         <v>103</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -3973,7 +3984,7 @@
         <v>104</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -3990,7 +4001,7 @@
         <v>105</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -4007,7 +4018,7 @@
         <v>106</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -4024,7 +4035,7 @@
         <v>107</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -4035,7 +4046,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D13" s="28">
         <v>45728</v>
@@ -4044,7 +4055,7 @@
         <v>84</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -4052,16 +4063,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D14" s="28">
         <v>45747</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -4069,16 +4080,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D15" s="28">
         <v>45784</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -4086,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D16" s="20">
         <v>45806</v>
@@ -4095,7 +4106,7 @@
         <v>85</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -4103,16 +4114,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D17" s="20">
         <v>45817</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -4120,16 +4131,16 @@
         <v>0</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D18" s="20">
         <v>45819</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -4141,13 +4152,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D20" s="20">
         <v>45820</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -4155,13 +4166,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D21" s="20">
         <v>45820</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -4179,10 +4190,10 @@
         <v>45728</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -4196,10 +4207,10 @@
         <v>45742</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4213,10 +4224,10 @@
         <v>45756</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -4230,10 +4241,10 @@
         <v>45770</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -4247,10 +4258,10 @@
         <v>45784</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -4264,10 +4275,10 @@
         <v>45798</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -4281,10 +4292,10 @@
         <v>45812</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -4301,10 +4312,10 @@
         <v>45764</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -4318,7 +4329,7 @@
         <v>45815</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -4332,10 +4343,10 @@
         <v>45814</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -4349,10 +4360,10 @@
         <v>45767</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -4366,7 +4377,7 @@
         <v>45775</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -4380,10 +4391,10 @@
         <v>45794</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -4397,10 +4408,10 @@
         <v>45784</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -4414,10 +4425,10 @@
         <v>45798</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -4431,10 +4442,10 @@
         <v>45805</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4467,54 +4478,54 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79"/>
+      <c r="F2" s="77" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+      <c r="J2" s="77" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="F2" s="71" t="s">
-        <v>204</v>
-      </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="J2" s="71" t="s">
-        <v>205</v>
-      </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="73"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="79"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L3" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4530,7 +4541,7 @@
       </c>
       <c r="H4" s="14"/>
       <c r="J4" s="37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K4" s="14">
         <v>4</v>
@@ -4539,7 +4550,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -4555,7 +4566,7 @@
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K5" s="2">
         <v>4</v>
@@ -4564,7 +4575,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4580,7 +4591,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="J6" s="38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K6" s="2">
         <v>5</v>
@@ -4589,7 +4600,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4605,7 +4616,7 @@
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K7" s="2">
         <v>5</v>
@@ -4614,7 +4625,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -4630,7 +4641,7 @@
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K8" s="2">
         <v>12</v>
@@ -4639,7 +4650,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -4656,26 +4667,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="75"/>
+      <c r="B11" s="80" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="81"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="75"/>
+      <c r="F11" s="80" t="s">
+        <v>195</v>
+      </c>
+      <c r="G11" s="81"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="K11" s="75"/>
+      <c r="J11" s="80" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11" s="81"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - POTEC - project and labs
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374CC67-EA74-4F6A-AC75-6B427581DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60543D3C-71EE-4D16-9EE0-C3329DDD987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -1101,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1299,25 +1299,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1719,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,19 +2054,19 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="67"/>
       <c r="N23" s="46" t="s">
         <v>129</v>
       </c>
@@ -2070,17 +2076,17 @@
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="69"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="70"/>
       <c r="N24" s="46"/>
       <c r="O24" s="46"/>
       <c r="Q24" s="7"/>
@@ -2136,7 +2142,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="61">
+      <c r="N27" s="63">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.2133333333333329</v>
       </c>
@@ -2167,26 +2173,26 @@
         <v>20</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="N28" s="62"/>
+      <c r="N28" s="64"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="63">
+      <c r="B29" s="71">
         <f>SUM(B28:C28)</f>
         <v>23</v>
       </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="F29" s="63">
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="F29" s="71">
         <v>5</v>
       </c>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="K29" s="63">
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="K29" s="71">
         <f>SUM(K28:L28)</f>
         <v>20</v>
       </c>
-      <c r="L29" s="63"/>
+      <c r="L29" s="71"/>
       <c r="N29" s="44"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2212,26 +2218,26 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="67"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="69"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="60" t="s">
@@ -2271,10 +2277,12 @@
       <c r="B38" s="2">
         <v>17</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2">
+        <v>20</v>
+      </c>
       <c r="E38" s="2">
         <f>C57</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F38" s="2">
         <f>G52</f>
@@ -2314,7 +2322,7 @@
       </c>
       <c r="I42" s="2">
         <f>SUM(B38:C38,E38:H38)</f>
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="J42" s="7"/>
       <c r="L42" s="7"/>
@@ -2323,7 +2331,9 @@
       <c r="B43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
       <c r="F43" s="2" t="s">
         <v>118</v>
       </c>
@@ -2373,7 +2383,7 @@
       </c>
       <c r="G46" s="2"/>
       <c r="I46" s="13">
-        <v>3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -2431,7 +2441,9 @@
       <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2">
+        <v>2</v>
+      </c>
       <c r="F52" s="2" t="s">
         <v>48</v>
       </c>
@@ -2444,7 +2456,9 @@
       <c r="B53" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -2464,7 +2478,7 @@
       </c>
       <c r="C57" s="2">
         <f>SUM(C42:C55)</f>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2771,40 +2785,40 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="74"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="77"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2952,24 +2966,24 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="72"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="74"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="73"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="77"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
@@ -3064,30 +3078,30 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="74"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="73"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="75"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="77"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="60" t="s">
@@ -3138,7 +3152,7 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="76">
+      <c r="M27" s="78">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
@@ -3173,7 +3187,7 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="76"/>
+      <c r="M28" s="78"/>
       <c r="N28" s="7"/>
       <c r="O28" s="47"/>
       <c r="P28" s="8"/>
@@ -3201,26 +3215,26 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="70" t="s">
+      <c r="B32" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="74"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="73"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="77"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="60" t="s">
@@ -3514,44 +3528,44 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="70" t="s">
+      <c r="B58" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="71"/>
-      <c r="F58" s="71"/>
-      <c r="G58" s="71"/>
-      <c r="H58" s="71"/>
-      <c r="I58" s="71"/>
-      <c r="J58" s="71"/>
-      <c r="K58" s="71"/>
-      <c r="L58" s="71"/>
-      <c r="M58" s="71"/>
-      <c r="N58" s="71"/>
-      <c r="O58" s="71"/>
-      <c r="P58" s="71"/>
-      <c r="Q58" s="71"/>
-      <c r="R58" s="72"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="73"/>
+      <c r="M58" s="73"/>
+      <c r="N58" s="73"/>
+      <c r="O58" s="73"/>
+      <c r="P58" s="73"/>
+      <c r="Q58" s="73"/>
+      <c r="R58" s="74"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="73"/>
-      <c r="C59" s="74"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="74"/>
-      <c r="J59" s="74"/>
-      <c r="K59" s="74"/>
-      <c r="L59" s="74"/>
-      <c r="M59" s="74"/>
-      <c r="N59" s="74"/>
-      <c r="O59" s="74"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="74"/>
-      <c r="R59" s="75"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="76"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="76"/>
+      <c r="O59" s="76"/>
+      <c r="P59" s="76"/>
+      <c r="Q59" s="76"/>
+      <c r="R59" s="77"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="60" t="s">
@@ -3717,26 +3731,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="70" t="s">
+      <c r="B72" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="C72" s="71"/>
-      <c r="D72" s="71"/>
-      <c r="E72" s="71"/>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="72"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
+      <c r="E72" s="73"/>
+      <c r="F72" s="73"/>
+      <c r="G72" s="73"/>
+      <c r="H72" s="73"/>
+      <c r="I72" s="74"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="73"/>
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="74"/>
-      <c r="H73" s="74"/>
-      <c r="I73" s="75"/>
+      <c r="B73" s="75"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="77"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3872,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,19 +4107,19 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="28">
         <v>45806</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="27" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4432,19 +4446,19 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" s="21" t="s">
+      <c r="B41" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="28">
         <v>45805</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="27" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4478,21 +4492,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="79"/>
-      <c r="F2" s="77" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="F2" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="J2" s="77" t="s">
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="J2" s="79" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="79"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="81"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4667,26 +4681,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="C11" s="81"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="80" t="s">
+      <c r="F11" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="G11" s="81"/>
+      <c r="G11" s="83"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="K11" s="81"/>
+      <c r="K11" s="83"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - SYSY - labs 2 and 5
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60543D3C-71EE-4D16-9EE0-C3329DDD987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8793264-63DB-413E-9767-49B253B37FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -1725,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,10 +1861,18 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="K7" s="2">
         <v>12</v>
       </c>
@@ -1891,13 +1899,13 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="46">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>25.7</v>
+        <v>41.6</v>
       </c>
       <c r="C10" s="46"/>
       <c r="E10" s="61"/>
       <c r="G10" s="46">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>40.299999999999997</v>
+        <v>24.4</v>
       </c>
       <c r="H10" s="46"/>
     </row>
@@ -2002,22 +2010,26 @@
       </c>
       <c r="L18" s="46">
         <f>SUM(B19:F19,H19:J19)</f>
-        <v>29.5</v>
+        <v>42.5</v>
       </c>
       <c r="M18" s="46"/>
       <c r="O18" s="46">
         <f>50-SUM(B19:F19,H19:J19)</f>
-        <v>20.5</v>
+        <v>7.5</v>
       </c>
       <c r="P18" s="46"/>
       <c r="R18" s="47"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>6.5</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>6.5</v>
+      </c>
       <c r="H19" s="2">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
SYSY - labs 1, 3 and 4
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52DF30C-32C7-42D6-AF27-D65884F59E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13BF28C-868C-4D50-B8BC-1F66635A2391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -1101,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,9 +1152,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1223,37 +1220,67 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1270,15 +1297,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1305,24 +1323,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,6 +1360,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1725,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,40 +1761,40 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="50"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="53"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="62"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1884,17 +1890,17 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="57"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="57"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="46">
@@ -1902,7 +1908,7 @@
         <v>41.6</v>
       </c>
       <c r="C10" s="46"/>
-      <c r="E10" s="61"/>
+      <c r="E10" s="67"/>
       <c r="G10" s="46">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>24.4</v>
@@ -1912,7 +1918,7 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
-      <c r="E11" s="62"/>
+      <c r="E11" s="68"/>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
     </row>
@@ -1939,49 +1945,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="67"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="68"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
       <c r="H17" s="54" t="s">
         <v>97</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="56"/>
-      <c r="L17" s="57" t="s">
+      <c r="L17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="57"/>
-      <c r="O17" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="P17" s="57"/>
-      <c r="R17" s="9" t="s">
+      <c r="M17" s="63"/>
+      <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
+      <c r="P17" s="85"/>
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -2010,23 +2013,27 @@
       </c>
       <c r="L18" s="46">
         <f>SUM(B19:F19,H19:J19)</f>
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="M18" s="46"/>
-      <c r="O18" s="46">
-        <f>50-SUM(B19:F19,H19:J19)</f>
-        <v>-12</v>
-      </c>
-      <c r="P18" s="46"/>
-      <c r="R18" s="47"/>
+      <c r="O18" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="P18" s="84"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>7</v>
+      </c>
       <c r="C19" s="2">
         <v>6.5</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8</v>
+      </c>
       <c r="F19" s="2">
         <v>6.5</v>
       </c>
@@ -2041,9 +2048,8 @@
       </c>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="R19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="84"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2068,19 +2074,19 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="67"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
       <c r="N23" s="46" t="s">
         <v>129</v>
       </c>
@@ -2090,17 +2096,17 @@
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="68"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="70"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="53"/>
       <c r="N24" s="46"/>
       <c r="O24" s="46"/>
       <c r="Q24" s="7"/>
@@ -2108,17 +2114,17 @@
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="F26" s="60" t="s">
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="F26" s="66" t="s">
         <v>208</v>
       </c>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
       <c r="J26" s="7"/>
       <c r="K26" s="54" t="s">
         <v>128</v>
@@ -2156,7 +2162,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="63">
+      <c r="N27" s="69">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.2133333333333329</v>
       </c>
@@ -2187,7 +2193,7 @@
         <v>20</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="N28" s="64"/>
+      <c r="N28" s="70"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="71">
@@ -2207,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="71"/>
-      <c r="N29" s="44"/>
+      <c r="N29" s="38"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
@@ -2232,32 +2238,32 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="70"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="53"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="60"/>
+      <c r="C36" s="66"/>
       <c r="D36" s="7"/>
       <c r="E36" s="54" t="s">
         <v>144</v>
@@ -2307,10 +2313,10 @@
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="65"/>
       <c r="F41" s="46" t="s">
         <v>102</v>
       </c>
@@ -2368,7 +2374,7 @@
         <v>119</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="57" t="s">
+      <c r="I44" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2383,7 +2389,7 @@
         <v>120</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="I45" s="57"/>
+      <c r="I45" s="63"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2419,7 +2425,7 @@
         <v>123</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="I48" s="44"/>
+      <c r="I48" s="38"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
@@ -2518,70 +2524,70 @@
     </row>
     <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-      <c r="N61" s="49"/>
-      <c r="O61" s="49"/>
-      <c r="P61" s="49"/>
-      <c r="Q61" s="49"/>
-      <c r="R61" s="49"/>
-      <c r="S61" s="50"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
+      <c r="J61" s="58"/>
+      <c r="K61" s="58"/>
+      <c r="L61" s="58"/>
+      <c r="M61" s="58"/>
+      <c r="N61" s="58"/>
+      <c r="O61" s="58"/>
+      <c r="P61" s="58"/>
+      <c r="Q61" s="58"/>
+      <c r="R61" s="58"/>
+      <c r="S61" s="59"/>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="52"/>
-      <c r="M62" s="52"/>
-      <c r="N62" s="52"/>
-      <c r="O62" s="52"/>
-      <c r="P62" s="52"/>
-      <c r="Q62" s="52"/>
-      <c r="R62" s="52"/>
-      <c r="S62" s="53"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="61"/>
+      <c r="N62" s="61"/>
+      <c r="O62" s="61"/>
+      <c r="P62" s="61"/>
+      <c r="Q62" s="61"/>
+      <c r="R62" s="61"/>
+      <c r="S62" s="62"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B64" s="60" t="s">
+      <c r="B64" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
-      <c r="I64" s="60"/>
-      <c r="J64" s="60"/>
-      <c r="K64" s="60"/>
-      <c r="M64" s="60" t="s">
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="66"/>
+      <c r="H64" s="66"/>
+      <c r="I64" s="66"/>
+      <c r="J64" s="66"/>
+      <c r="K64" s="66"/>
+      <c r="M64" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="N64" s="60"/>
-      <c r="O64" s="60"/>
-      <c r="P64" s="60"/>
-      <c r="R64" s="60" t="s">
+      <c r="N64" s="66"/>
+      <c r="O64" s="66"/>
+      <c r="P64" s="66"/>
+      <c r="R64" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="S64" s="60"/>
+      <c r="S64" s="66"/>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
@@ -2676,18 +2682,18 @@
       <c r="S66" s="2"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="57" t="s">
+      <c r="B69" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C69" s="57"/>
+      <c r="C69" s="63"/>
       <c r="E69" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="57" t="s">
+      <c r="G69" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="H69" s="57"/>
-      <c r="K69" s="45" t="s">
+      <c r="H69" s="63"/>
+      <c r="K69" s="39" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2716,7 +2722,7 @@
       <c r="K71" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="40">
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="R64:S64"/>
     <mergeCell ref="B33:I34"/>
@@ -2730,7 +2736,6 @@
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="B23:L24"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="O17:P17"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="L17:M17"/>
@@ -2744,7 +2749,7 @@
     <mergeCell ref="G69:H69"/>
     <mergeCell ref="G70:H71"/>
     <mergeCell ref="K70:K71"/>
-    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="B2:P3"/>
@@ -2755,7 +2760,6 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="N23:O24"/>
-    <mergeCell ref="O18:P19"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
@@ -2836,14 +2840,14 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
@@ -2934,10 +2938,10 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="57"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
@@ -2948,14 +2952,14 @@
         <v>110</v>
       </c>
       <c r="C10" s="46"/>
-      <c r="E10" s="61">
+      <c r="E10" s="67">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
-      <c r="E11" s="62"/>
+      <c r="E11" s="68"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -3000,20 +3004,20 @@
       <c r="H15" s="77"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="F17" s="60" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="F17" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="J17" s="57" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="J17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="57"/>
+      <c r="K17" s="63"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3118,20 +3122,20 @@
       <c r="K24" s="77"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="60"/>
+      <c r="C26" s="66"/>
       <c r="E26" s="54" t="s">
         <v>21</v>
       </c>
       <c r="F26" s="55"/>
       <c r="G26" s="56"/>
-      <c r="I26" s="60" t="s">
+      <c r="I26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="66"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3251,17 +3255,17 @@
       <c r="I33" s="77"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="F35" s="60" t="s">
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="F35" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3318,10 +3322,10 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="59"/>
+      <c r="C40" s="65"/>
       <c r="F40" s="46" t="s">
         <v>36</v>
       </c>
@@ -3381,7 +3385,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="57" t="s">
+      <c r="I43" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3398,7 +3402,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="57"/>
+      <c r="I44" s="63"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3582,27 +3586,27 @@
       <c r="R59" s="77"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="60" t="s">
+      <c r="B61" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="60"/>
-      <c r="K61" s="60"/>
-      <c r="M61" s="60" t="s">
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="M61" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="60"/>
-      <c r="O61" s="60"/>
-      <c r="Q61" s="60" t="s">
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
+      <c r="Q61" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="60"/>
+      <c r="R61" s="66"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3699,10 +3703,10 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="57" t="s">
+      <c r="B66" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="57"/>
+      <c r="C66" s="63"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
@@ -3791,10 +3795,10 @@
       <c r="I75" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="K75" s="57" t="s">
+      <c r="K75" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="57"/>
+      <c r="L75" s="63"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3900,8 +3904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,261 +3932,261 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="b">
+      <c r="B3" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>45763</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="b">
+      <c r="B4" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="27">
+        <v>45812</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C5" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="20">
-        <v>45803</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="b">
+      <c r="D5" s="43">
+        <v>45817</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="30"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="27">
+        <v>45729</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="27">
+        <v>45743</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="27">
+        <v>45757</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="27">
+        <v>45785</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="27">
+        <v>45799</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="30"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="27">
+        <v>45728</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="27">
+        <v>45747</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="27">
+        <v>45784</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="27">
+        <v>45806</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="41">
-        <v>45817</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>149</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="28">
-        <v>45729</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="28">
-        <v>45743</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="28">
-        <v>45757</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="28">
-        <v>45785</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="28">
-        <v>45799</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="31"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="29" t="s">
+      <c r="C17" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="28">
-        <v>45728</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="28">
-        <v>45747</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="28">
-        <v>45784</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="28">
-        <v>45806</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>45817</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="b">
+      <c r="B18" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <v>45819</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="20" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="31"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="b">
+      <c r="B20" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <v>45820</v>
       </c>
       <c r="E20" s="17" t="s">
@@ -4190,13 +4194,13 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="b">
+      <c r="B21" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <v>45820</v>
       </c>
       <c r="E21" s="17" t="s">
@@ -4204,170 +4208,170 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="31"/>
-      <c r="D22" s="22"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="b">
+      <c r="B23" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="27">
         <v>45728</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="b">
+      <c r="B24" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="27">
         <v>45742</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="26" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="b">
+      <c r="B25" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="27">
         <v>45756</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="26" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="b">
+      <c r="B26" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="28">
+      <c r="D26" s="27">
         <v>45770</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="28" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="b">
+      <c r="B27" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="27">
         <v>45784</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="26" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="b">
+      <c r="B28" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="27">
         <v>45798</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="26" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="b">
+      <c r="B29" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="27">
+        <v>45812</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="30"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="27">
+        <v>45764</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="27">
+        <v>45815</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C33" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="20">
-        <v>45812</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="31"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="28">
-        <v>45764</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="28">
-        <v>45815</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="20">
+      <c r="D33" s="19">
         <v>45814</v>
       </c>
       <c r="E33" s="17" t="s">
@@ -4378,101 +4382,101 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="b">
+      <c r="B35" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="27">
         <v>45767</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="26" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="b">
+      <c r="B36" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="27">
         <v>45775</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="26" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="b">
+      <c r="B37" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="27">
         <v>45794</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="26" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="b">
+      <c r="B39" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="27">
         <v>45784</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="26" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="b">
+      <c r="B40" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="28">
+      <c r="D40" s="27">
         <v>45798</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F40" s="26" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="b">
+      <c r="B41" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="28">
+      <c r="D41" s="27">
         <v>45805</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="F41" s="27" t="s">
+      <c r="F41" s="26" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4487,8 +4491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA352BE-3E69-4CCA-8EEB-A9094B74606F}">
   <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4523,36 +4527,36 @@
       <c r="L2" s="81"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="35" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>130</v>
       </c>
       <c r="C4" s="14">
@@ -4561,14 +4565,14 @@
       <c r="D4" s="14">
         <v>4</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="36" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="14">
         <v>5</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>196</v>
       </c>
       <c r="K4" s="14">
@@ -4577,7 +4581,7 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="37" t="s">
         <v>131</v>
       </c>
       <c r="C5" s="2">
@@ -4586,14 +4590,14 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="37" t="s">
         <v>197</v>
       </c>
       <c r="K5" s="2">
@@ -4602,7 +4606,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>132</v>
       </c>
       <c r="C6" s="2">
@@ -4611,14 +4615,16 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>77</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="38" t="s">
+      <c r="H6" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J6" s="37" t="s">
         <v>198</v>
       </c>
       <c r="K6" s="2">
@@ -4627,7 +4633,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>133</v>
       </c>
       <c r="C7" s="2">
@@ -4636,14 +4642,14 @@
       <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="37" t="s">
         <v>199</v>
       </c>
       <c r="K7" s="2">
@@ -4652,7 +4658,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C8" s="2">
@@ -4661,14 +4667,14 @@
       <c r="D8" s="2">
         <v>4.5</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="37" t="s">
         <v>80</v>
       </c>
       <c r="G8" s="2">
         <v>11</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="37" t="s">
         <v>200</v>
       </c>
       <c r="K8" s="2">
@@ -4677,7 +4683,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>135</v>
       </c>
       <c r="C9" s="2">
@@ -4686,10 +4692,10 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="32"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
@@ -4699,7 +4705,7 @@
         <v>195</v>
       </c>
       <c r="C11" s="83"/>
-      <c r="D11" s="33">
+      <c r="D11" s="32">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
@@ -4707,15 +4713,15 @@
         <v>195</v>
       </c>
       <c r="G11" s="83"/>
-      <c r="H11" s="33">
+      <c r="H11" s="32">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J11" s="82" t="s">
         <v>195</v>
       </c>
       <c r="K11" s="83"/>
-      <c r="L11" s="33">
+      <c r="L11" s="32">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
New points - 3rd project - POTEC
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13BF28C-868C-4D50-B8BC-1F66635A2391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC233770-1B09-40FE-8A9D-14C357B2668A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="216">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -365,18 +365,12 @@
     <t>LAB5</t>
   </si>
   <si>
-    <t>LAB6</t>
-  </si>
-  <si>
     <t>LAB7</t>
   </si>
   <si>
     <t>LAB8</t>
   </si>
   <si>
-    <t>LAB9</t>
-  </si>
-  <si>
     <t>LAB10</t>
   </si>
   <si>
@@ -386,9 +380,6 @@
     <t>LAB12</t>
   </si>
   <si>
-    <t>LAB13</t>
-  </si>
-  <si>
     <t>LAB14</t>
   </si>
   <si>
@@ -399,24 +390,6 @@
   </si>
   <si>
     <t>PROJ3</t>
-  </si>
-  <si>
-    <t>PROJ4</t>
-  </si>
-  <si>
-    <t>PROJ5</t>
-  </si>
-  <si>
-    <t>PROJ6</t>
-  </si>
-  <si>
-    <t>PROJ7</t>
-  </si>
-  <si>
-    <t>BONUS1</t>
-  </si>
-  <si>
-    <t>BONUS2</t>
   </si>
   <si>
     <t>Laby [14*2 pkt]</t>
@@ -1101,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1248,58 +1221,76 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1308,24 +1299,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1363,9 +1336,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1729,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,85 +1731,85 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="59"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="62"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="59"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="H5" s="54" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="63"/>
+      <c r="H5" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="K5" s="54" t="s">
+      <c r="I5" s="63"/>
+      <c r="K5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="63"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
@@ -1890,37 +1860,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="64"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="64"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="65">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>41.6</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="67"/>
-      <c r="G10" s="46">
+      <c r="C10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="G10" s="65">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>24.4</v>
       </c>
-      <c r="H10" s="46"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="68"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="E11" s="67"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1965,36 +1935,36 @@
       <c r="H15" s="53"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="H17" s="54" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="H17" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
-      <c r="L17" s="63" t="s">
+      <c r="I17" s="68"/>
+      <c r="J17" s="63"/>
+      <c r="L17" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="63"/>
+      <c r="M17" s="64"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="P17" s="85"/>
+      <c r="P17" s="38"/>
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>92</v>
@@ -2011,15 +1981,14 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="65">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>85</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="O18" s="47">
+      <c r="M18" s="65"/>
+      <c r="O18" s="69">
         <v>4.5</v>
       </c>
-      <c r="P18" s="84"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
@@ -2046,10 +2015,9 @@
       <c r="J19" s="2">
         <v>19.5</v>
       </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="84"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="O19" s="69"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2087,10 +2055,10 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
       <c r="L23" s="50"/>
-      <c r="N23" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="O23" s="46"/>
+      <c r="N23" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="O23" s="65"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
@@ -2107,62 +2075,62 @@
       <c r="J24" s="52"/>
       <c r="K24" s="52"/>
       <c r="L24" s="53"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="F26" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="F26" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="L26" s="56"/>
+      <c r="K26" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="L26" s="63"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>73</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N27" s="69">
+        <v>118</v>
+      </c>
+      <c r="N27" s="60">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.2133333333333329</v>
       </c>
@@ -2193,26 +2161,26 @@
         <v>20</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="N28" s="70"/>
+      <c r="N28" s="61"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="71">
+      <c r="B29" s="46">
         <f>SUM(B28:C28)</f>
         <v>23</v>
       </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="F29" s="71">
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="F29" s="46">
         <v>5</v>
       </c>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="K29" s="71">
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="K29" s="46">
         <f>SUM(K28:L28)</f>
         <v>20</v>
       </c>
-      <c r="L29" s="71"/>
+      <c r="L29" s="46"/>
       <c r="N29" s="38"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,17 +2228,17 @@
       <c r="I34" s="53"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="66"/>
+      <c r="C36" s="47"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="56"/>
+      <c r="E36" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="63"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
@@ -2301,26 +2269,26 @@
         <v>20</v>
       </c>
       <c r="E38" s="2">
-        <f>C57</f>
+        <f>C54</f>
         <v>25</v>
       </c>
       <c r="F38" s="2">
-        <f>G52</f>
-        <v>19</v>
+        <f>G46</f>
+        <v>29</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="65"/>
-      <c r="F41" s="46" t="s">
+      <c r="B41" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="71"/>
+      <c r="F41" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="46"/>
+      <c r="G41" s="65"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -2335,14 +2303,14 @@
         <v>2</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G42" s="2">
         <v>9</v>
       </c>
       <c r="I42" s="2">
         <f>SUM(B38:C38,E38:H38)</f>
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="J42" s="7"/>
       <c r="L42" s="7"/>
@@ -2355,7 +2323,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G43" s="2">
         <v>10</v>
@@ -2371,10 +2339,12 @@
         <v>3</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="I44" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G44" s="2">
+        <v>10</v>
+      </c>
+      <c r="I44" s="64" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2385,11 +2355,9 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="I45" s="63"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="84"/>
+      <c r="I45" s="64"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2399,11 +2367,14 @@
         <v>4</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G46" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="G46" s="2">
+        <f>SUM(G42:G44)</f>
+        <v>29</v>
+      </c>
       <c r="I46" s="13">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -2411,20 +2382,18 @@
         <v>108</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="F47" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G47" s="2"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="84"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="F48" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G48" s="2"/>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
       <c r="I48" s="38"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -2434,321 +2403,265 @@
       <c r="C49" s="2">
         <v>2</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G49" s="2"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="F50" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G50" s="2"/>
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="F50" s="84"/>
+      <c r="G50" s="84"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C51" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="2">
-        <v>2</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G52" s="2">
-        <f>SUM(G42:G50)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="2">
-        <v>4</v>
-      </c>
+      <c r="C52" s="2"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="2">
-        <f>SUM(C42:C55)</f>
+      <c r="C54" s="2">
+        <f>SUM(C42:C52)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="6"/>
-      <c r="N59" s="6"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
-      <c r="Q59" s="6"/>
-      <c r="R59" s="6"/>
-      <c r="S59" s="6"/>
-    </row>
-    <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="57" t="s">
+    <row r="56" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="6"/>
+    </row>
+    <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
-      <c r="K61" s="58"/>
-      <c r="L61" s="58"/>
-      <c r="M61" s="58"/>
-      <c r="N61" s="58"/>
-      <c r="O61" s="58"/>
-      <c r="P61" s="58"/>
-      <c r="Q61" s="58"/>
-      <c r="R61" s="58"/>
-      <c r="S61" s="59"/>
-    </row>
-    <row r="62" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="60"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
-      <c r="I62" s="61"/>
-      <c r="J62" s="61"/>
-      <c r="K62" s="61"/>
-      <c r="L62" s="61"/>
-      <c r="M62" s="61"/>
-      <c r="N62" s="61"/>
-      <c r="O62" s="61"/>
-      <c r="P62" s="61"/>
-      <c r="Q62" s="61"/>
-      <c r="R62" s="61"/>
-      <c r="S62" s="62"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B64" s="66" t="s">
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="55"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="55"/>
+      <c r="N58" s="55"/>
+      <c r="O58" s="55"/>
+      <c r="P58" s="55"/>
+      <c r="Q58" s="55"/>
+      <c r="R58" s="55"/>
+      <c r="S58" s="56"/>
+    </row>
+    <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="57"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="58"/>
+      <c r="J59" s="58"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="58"/>
+      <c r="R59" s="58"/>
+      <c r="S59" s="59"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B61" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="66"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="66"/>
-      <c r="H64" s="66"/>
-      <c r="I64" s="66"/>
-      <c r="J64" s="66"/>
-      <c r="K64" s="66"/>
-      <c r="M64" s="66" t="s">
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="M61" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N64" s="66"/>
-      <c r="O64" s="66"/>
-      <c r="P64" s="66"/>
-      <c r="R64" s="66" t="s">
+      <c r="N61" s="47"/>
+      <c r="O61" s="47"/>
+      <c r="P61" s="47"/>
+      <c r="R61" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="S64" s="66"/>
-    </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
+      <c r="S61" s="47"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J65" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="K65" s="2" t="s">
+      <c r="J62" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K62" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="M62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N65" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O65" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="P65" s="2" t="s">
+      <c r="P62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R65" s="2" t="s">
+      <c r="R62" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S65" s="2" t="s">
+      <c r="S62" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
         <v>2</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C63" s="2">
         <v>2</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D63" s="2">
         <v>2</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E63" s="2">
         <v>2</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H66" s="2">
+      <c r="F63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H63" s="2">
         <v>2</v>
       </c>
-      <c r="I66" s="2">
+      <c r="I63" s="2">
         <v>2</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J63" s="2">
         <v>2</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K63" s="2">
         <v>2</v>
       </c>
-      <c r="M66" s="2">
+      <c r="M63" s="2">
         <v>5</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N63" s="2">
         <v>5</v>
       </c>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="R66" s="2"/>
-      <c r="S66" s="2"/>
-    </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="63" t="s">
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="R63" s="2"/>
+      <c r="S63" s="2"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C69" s="63"/>
-      <c r="E69" s="9" t="s">
+      <c r="C66" s="64"/>
+      <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="63" t="s">
+      <c r="G66" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="H69" s="63"/>
-      <c r="K69" s="39" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="46">
-        <f>SUM(B66:K66,M66:P66,R66:S66,K70)</f>
+      <c r="H66" s="64"/>
+      <c r="K66" s="39" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="65">
+        <f>SUM(B63:K63,M63:P63,R63:S63,K67)</f>
         <v>29</v>
       </c>
-      <c r="C70" s="46"/>
-      <c r="E70" s="47"/>
-      <c r="G70" s="46">
-        <f>50-SUM(B66:K66,M66:P66,R66:S66,K70)</f>
+      <c r="C67" s="65"/>
+      <c r="E67" s="69"/>
+      <c r="G67" s="65">
+        <f>50-SUM(B63:K63,M63:P63,R63:S63,K67)</f>
         <v>21</v>
       </c>
-      <c r="H70" s="46"/>
-      <c r="K70" s="46">
+      <c r="H67" s="65"/>
+      <c r="K67" s="65">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
-      <c r="E71" s="47"/>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46"/>
-      <c r="K71" s="46"/>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="65"/>
+      <c r="C68" s="65"/>
+      <c r="E68" s="69"/>
+      <c r="G68" s="65"/>
+      <c r="H68" s="65"/>
+      <c r="K68" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="B33:I34"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="B61:S62"/>
-    <mergeCell ref="M64:P64"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C71"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H71"/>
-    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="K67:K68"/>
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2763,6 +2676,31 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H68"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R61:S61"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B58:S59"/>
+    <mergeCell ref="M61:P61"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2804,7 +2742,7 @@
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C2" s="73"/>
       <c r="D2" s="73"/>
@@ -2840,23 +2778,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="63"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2938,28 +2876,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="64"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="65">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="67">
+      <c r="C10" s="65"/>
+      <c r="E10" s="66">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="68"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="E11" s="67"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2985,7 +2923,7 @@
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="72" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="73"/>
@@ -3004,20 +2942,20 @@
       <c r="H15" s="77"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="F17" s="66" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="F17" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="J17" s="63" t="s">
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="J17" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="63"/>
+      <c r="K17" s="64"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3041,12 +2979,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="65">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="M18" s="47">
+      <c r="K18" s="65"/>
+      <c r="M18" s="69">
         <v>5</v>
       </c>
     </row>
@@ -3069,9 +3007,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="M19" s="47"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="M19" s="69"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3097,7 +3035,7 @@
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" s="72" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C23" s="73"/>
       <c r="D23" s="73"/>
@@ -3122,20 +3060,20 @@
       <c r="K24" s="77"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="E26" s="54" t="s">
+      <c r="C26" s="47"/>
+      <c r="E26" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="I26" s="66" t="s">
+      <c r="F26" s="68"/>
+      <c r="G26" s="63"/>
+      <c r="I26" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3175,7 +3113,7 @@
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="47">
+      <c r="O27" s="69">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3207,7 +3145,7 @@
       </c>
       <c r="M28" s="78"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="47"/>
+      <c r="O28" s="69"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3234,7 +3172,7 @@
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="72" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
@@ -3255,17 +3193,17 @@
       <c r="I33" s="77"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="F35" s="66" t="s">
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="F35" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3322,14 +3260,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="65"/>
-      <c r="F40" s="46" t="s">
+      <c r="C40" s="71"/>
+      <c r="F40" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="65"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3385,7 +3323,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="63" t="s">
+      <c r="I43" s="64" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3402,7 +3340,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="63"/>
+      <c r="I44" s="64"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3547,7 +3485,7 @@
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B58" s="72" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
@@ -3586,27 +3524,27 @@
       <c r="R59" s="77"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="66" t="s">
+      <c r="B61" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="66"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="M61" s="66" t="s">
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="M61" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="66"/>
-      <c r="O61" s="66"/>
-      <c r="Q61" s="66" t="s">
+      <c r="N61" s="47"/>
+      <c r="O61" s="47"/>
+      <c r="Q61" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="66"/>
+      <c r="R61" s="47"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3703,28 +3641,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="64"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="46">
+      <c r="B67" s="65">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="E67" s="47">
+      <c r="C67" s="65"/>
+      <c r="E67" s="69">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="E68" s="47"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="65"/>
+      <c r="E68" s="69"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3750,7 +3688,7 @@
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B72" s="72" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
@@ -3772,33 +3710,33 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K75" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="K75" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="63"/>
+      <c r="L75" s="64"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3828,11 +3766,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="46">
+      <c r="K76" s="65">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="46"/>
+      <c r="L76" s="65"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3860,6 +3798,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B23:K24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B72:I73"/>
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="K76:L76"/>
@@ -3870,30 +3832,6 @@
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B23:K24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3904,8 +3842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3919,16 +3857,16 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3942,10 +3880,10 @@
         <v>45763</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -3959,10 +3897,10 @@
         <v>45812</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -3976,10 +3914,10 @@
         <v>45817</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -3999,7 +3937,7 @@
         <v>103</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -4016,7 +3954,7 @@
         <v>104</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -4033,7 +3971,7 @@
         <v>105</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -4050,7 +3988,7 @@
         <v>106</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -4067,7 +4005,7 @@
         <v>107</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -4078,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D13" s="27">
         <v>45728</v>
@@ -4087,7 +4025,7 @@
         <v>84</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -4095,16 +4033,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D14" s="27">
         <v>45747</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -4112,16 +4050,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D15" s="27">
         <v>45784</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -4129,7 +4067,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D16" s="27">
         <v>45806</v>
@@ -4138,24 +4076,24 @@
         <v>85</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="19">
+      <c r="B17" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="27">
         <v>45817</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>166</v>
+      <c r="E17" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -4163,16 +4101,16 @@
         <v>0</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D18" s="19">
         <v>45819</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -4184,13 +4122,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D20" s="19">
         <v>45820</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -4198,13 +4136,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D21" s="19">
         <v>45820</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -4222,10 +4160,10 @@
         <v>45728</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -4239,10 +4177,10 @@
         <v>45742</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4256,10 +4194,10 @@
         <v>45756</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -4273,10 +4211,10 @@
         <v>45770</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -4290,10 +4228,10 @@
         <v>45784</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -4307,10 +4245,10 @@
         <v>45798</v>
       </c>
       <c r="E28" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="26" t="s">
         <v>178</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -4324,10 +4262,10 @@
         <v>45812</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -4344,10 +4282,10 @@
         <v>45764</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -4361,24 +4299,24 @@
         <v>45815</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="20" t="s">
+      <c r="B33" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="27">
         <v>45814</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>221</v>
+      <c r="E33" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -4392,10 +4330,10 @@
         <v>45767</v>
       </c>
       <c r="E35" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="26" t="s">
         <v>179</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -4409,7 +4347,7 @@
         <v>45775</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -4423,10 +4361,10 @@
         <v>45794</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -4440,10 +4378,10 @@
         <v>45784</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -4457,10 +4395,10 @@
         <v>45798</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -4474,10 +4412,10 @@
         <v>45805</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4491,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA352BE-3E69-4CCA-8EEB-A9094B74606F}">
   <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4511,53 +4449,53 @@
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="79" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C2" s="80"/>
       <c r="D2" s="81"/>
       <c r="F2" s="79" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G2" s="80"/>
       <c r="H2" s="81"/>
       <c r="J2" s="79" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="K2" s="80"/>
       <c r="L2" s="81"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="33" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4573,7 +4511,7 @@
       </c>
       <c r="H4" s="14"/>
       <c r="J4" s="36" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K4" s="14">
         <v>4</v>
@@ -4582,7 +4520,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -4598,7 +4536,7 @@
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="37" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="K5" s="2">
         <v>4</v>
@@ -4607,7 +4545,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4625,7 +4563,7 @@
         <v>4.5</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="K6" s="2">
         <v>5</v>
@@ -4634,7 +4572,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4648,9 +4586,11 @@
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
       <c r="J7" s="37" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="K7" s="2">
         <v>5</v>
@@ -4659,7 +4599,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -4675,7 +4615,7 @@
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="37" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K8" s="2">
         <v>12</v>
@@ -4684,7 +4624,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -4702,7 +4642,7 @@
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="82" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C11" s="83"/>
       <c r="D11" s="32">
@@ -4710,15 +4650,15 @@
         <v>4.4333333333333336</v>
       </c>
       <c r="F11" s="82" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="G11" s="83"/>
       <c r="H11" s="32">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
-        <v>0.75</v>
+        <v>1.5833333333333333</v>
       </c>
       <c r="J11" s="82" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="K11" s="83"/>
       <c r="L11" s="32">

</xml_diff>

<commit_message>
New points - PBL2 -> passed
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC233770-1B09-40FE-8A9D-14C357B2668A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0EE2A9-3B2E-4037-8903-BB049E272633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="216">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -769,7 +769,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,12 +785,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1143,32 +1137,32 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1178,89 +1172,116 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1269,64 +1290,19 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1335,8 +1311,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1701,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,60 +1710,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="62"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="63"/>
-      <c r="H5" s="62" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="H5" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="K5" s="62" t="s">
+      <c r="I5" s="56"/>
+      <c r="K5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1860,37 +1839,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="64"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="64"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="65">
+      <c r="B10" s="46">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>41.6</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="E10" s="66"/>
-      <c r="G10" s="65">
+      <c r="C10" s="46"/>
+      <c r="E10" s="67"/>
+      <c r="G10" s="46">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>24.4</v>
       </c>
-      <c r="H10" s="65"/>
+      <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="E11" s="67"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="68"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1935,22 +1914,22 @@
       <c r="H15" s="53"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="H17" s="62" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="H17" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="68"/>
-      <c r="J17" s="63"/>
-      <c r="L17" s="64" t="s">
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="L17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="64"/>
+      <c r="M17" s="63"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1981,12 +1960,12 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="65">
+      <c r="L18" s="46">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>85</v>
       </c>
-      <c r="M18" s="65"/>
-      <c r="O18" s="69">
+      <c r="M18" s="46"/>
+      <c r="O18" s="47">
         <v>4.5</v>
       </c>
     </row>
@@ -2015,9 +1994,9 @@
       <c r="J19" s="2">
         <v>19.5</v>
       </c>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="O19" s="69"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="O19" s="47"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2055,10 +2034,10 @@
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
       <c r="L23" s="50"/>
-      <c r="N23" s="65" t="s">
+      <c r="N23" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="O23" s="65"/>
+      <c r="O23" s="46"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
@@ -2075,29 +2054,29 @@
       <c r="J24" s="52"/>
       <c r="K24" s="52"/>
       <c r="L24" s="53"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="F26" s="47" t="s">
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="F26" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="62" t="s">
+      <c r="K26" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="L26" s="63"/>
+      <c r="L26" s="56"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2130,7 +2109,7 @@
       <c r="L27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N27" s="60">
+      <c r="N27" s="69">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.2133333333333329</v>
       </c>
@@ -2161,26 +2140,26 @@
         <v>20</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="N28" s="61"/>
+      <c r="N28" s="70"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="46">
+      <c r="B29" s="71">
         <f>SUM(B28:C28)</f>
         <v>23</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="F29" s="46">
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="F29" s="71">
         <v>5</v>
       </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="K29" s="46">
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="K29" s="71">
         <f>SUM(K28:L28)</f>
         <v>20</v>
       </c>
-      <c r="L29" s="46"/>
+      <c r="L29" s="71"/>
       <c r="N29" s="38"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2228,17 +2207,17 @@
       <c r="I34" s="53"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="47"/>
+      <c r="C36" s="66"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="63"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="56"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
@@ -2281,14 +2260,14 @@
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="F41" s="65" t="s">
+      <c r="C41" s="65"/>
+      <c r="F41" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="65"/>
+      <c r="G41" s="46"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -2344,7 +2323,7 @@
       <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="I44" s="64" t="s">
+      <c r="I44" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2355,9 +2334,7 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="I45" s="64"/>
+      <c r="I45" s="63"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2382,8 +2359,6 @@
         <v>108</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="84"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -2392,8 +2367,6 @@
       <c r="C48" s="2">
         <v>2</v>
       </c>
-      <c r="F48" s="84"/>
-      <c r="G48" s="84"/>
       <c r="I48" s="38"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -2403,8 +2376,6 @@
       <c r="C49" s="2">
         <v>2</v>
       </c>
-      <c r="F49" s="84"/>
-      <c r="G49" s="84"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
@@ -2413,8 +2384,6 @@
       <c r="C50" s="2">
         <v>2</v>
       </c>
-      <c r="F50" s="84"/>
-      <c r="G50" s="84"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
@@ -2462,70 +2431,70 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="55"/>
-      <c r="M58" s="55"/>
-      <c r="N58" s="55"/>
-      <c r="O58" s="55"/>
-      <c r="P58" s="55"/>
-      <c r="Q58" s="55"/>
-      <c r="R58" s="55"/>
-      <c r="S58" s="56"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="49"/>
+      <c r="M58" s="49"/>
+      <c r="N58" s="49"/>
+      <c r="O58" s="49"/>
+      <c r="P58" s="49"/>
+      <c r="Q58" s="49"/>
+      <c r="R58" s="49"/>
+      <c r="S58" s="50"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="57"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="58"/>
-      <c r="O59" s="58"/>
-      <c r="P59" s="58"/>
-      <c r="Q59" s="58"/>
-      <c r="R59" s="58"/>
-      <c r="S59" s="59"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+      <c r="O59" s="52"/>
+      <c r="P59" s="52"/>
+      <c r="Q59" s="52"/>
+      <c r="R59" s="52"/>
+      <c r="S59" s="53"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="47"/>
-      <c r="M61" s="47" t="s">
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="M61" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="N61" s="47"/>
-      <c r="O61" s="47"/>
-      <c r="P61" s="47"/>
-      <c r="R61" s="47" t="s">
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
+      <c r="P61" s="66"/>
+      <c r="R61" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="S61" s="47"/>
+      <c r="S61" s="66"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2614,54 +2583,72 @@
       <c r="N63" s="2">
         <v>5</v>
       </c>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
+      <c r="O63" s="2">
+        <v>10</v>
+      </c>
+      <c r="P63" s="2">
+        <v>20</v>
+      </c>
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="64" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="64"/>
+      <c r="C66" s="63"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G66" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="H66" s="64"/>
-      <c r="K66" s="39" t="s">
+      <c r="G66" s="39" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="65">
-        <f>SUM(B63:K63,M63:P63,R63:S63,K67)</f>
-        <v>29</v>
-      </c>
-      <c r="C67" s="65"/>
-      <c r="E67" s="69"/>
-      <c r="G67" s="65">
-        <f>50-SUM(B63:K63,M63:P63,R63:S63,K67)</f>
-        <v>21</v>
-      </c>
-      <c r="H67" s="65"/>
-      <c r="K67" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="65"/>
-      <c r="C68" s="65"/>
-      <c r="E68" s="69"/>
-      <c r="G68" s="65"/>
-      <c r="H68" s="65"/>
-      <c r="K68" s="65"/>
+      <c r="H66" s="78"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="46">
+        <f>SUM(B63:K63,M63:P63,R63:S63,G67)</f>
+        <v>65</v>
+      </c>
+      <c r="C67" s="46"/>
+      <c r="E67" s="47"/>
+      <c r="G67" s="46">
+        <v>9</v>
+      </c>
+      <c r="H67" s="79"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="E68" s="47"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="K67:K68"/>
+  <mergeCells count="38">
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R61:S61"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B58:S59"/>
+    <mergeCell ref="M61:P61"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="G67:G68"/>
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2677,30 +2664,6 @@
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H68"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="R61:S61"/>
-    <mergeCell ref="B33:I34"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="B58:S59"/>
-    <mergeCell ref="M61:P61"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2713,7 +2676,7 @@
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,60 +2704,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="74"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="77"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="63"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="56"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2876,28 +2839,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="64"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="65">
+      <c r="B10" s="46">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="E10" s="66">
+      <c r="C10" s="46"/>
+      <c r="E10" s="67">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="E11" s="67"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="68"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2922,40 +2885,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="74"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="75"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="F17" s="47" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="F17" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="J17" s="64" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="J17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="64"/>
+      <c r="K17" s="63"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2979,12 +2942,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="65">
+      <c r="J18" s="46">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="65"/>
-      <c r="M18" s="69">
+      <c r="K18" s="46"/>
+      <c r="M18" s="47">
         <v>5</v>
       </c>
     </row>
@@ -3007,9 +2970,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="M19" s="69"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="M19" s="47"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3034,46 +2997,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="74"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="75"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="77"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="E26" s="62" t="s">
+      <c r="C26" s="66"/>
+      <c r="E26" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="68"/>
-      <c r="G26" s="63"/>
-      <c r="I26" s="47" t="s">
+      <c r="F26" s="55"/>
+      <c r="G26" s="56"/>
+      <c r="I26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="66"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3108,12 +3071,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="78">
+      <c r="M27" s="72">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="69">
+      <c r="O27" s="47">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3143,9 +3106,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="78"/>
+      <c r="M28" s="72"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="69"/>
+      <c r="O28" s="47"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3171,39 +3134,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="74"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="75"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="77"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="F35" s="47" t="s">
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="F35" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3260,14 +3223,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="F40" s="65" t="s">
+      <c r="C40" s="65"/>
+      <c r="F40" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="65"/>
+      <c r="G40" s="46"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3323,7 +3286,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="64" t="s">
+      <c r="I43" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3340,7 +3303,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="64"/>
+      <c r="I44" s="63"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3484,67 +3447,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="73"/>
-      <c r="M58" s="73"/>
-      <c r="N58" s="73"/>
-      <c r="O58" s="73"/>
-      <c r="P58" s="73"/>
-      <c r="Q58" s="73"/>
-      <c r="R58" s="74"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="49"/>
+      <c r="M58" s="49"/>
+      <c r="N58" s="49"/>
+      <c r="O58" s="49"/>
+      <c r="P58" s="49"/>
+      <c r="Q58" s="49"/>
+      <c r="R58" s="50"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="75"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="76"/>
-      <c r="G59" s="76"/>
-      <c r="H59" s="76"/>
-      <c r="I59" s="76"/>
-      <c r="J59" s="76"/>
-      <c r="K59" s="76"/>
-      <c r="L59" s="76"/>
-      <c r="M59" s="76"/>
-      <c r="N59" s="76"/>
-      <c r="O59" s="76"/>
-      <c r="P59" s="76"/>
-      <c r="Q59" s="76"/>
-      <c r="R59" s="77"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+      <c r="O59" s="52"/>
+      <c r="P59" s="52"/>
+      <c r="Q59" s="52"/>
+      <c r="R59" s="53"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="47"/>
-      <c r="M61" s="47" t="s">
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="M61" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="47"/>
-      <c r="O61" s="47"/>
-      <c r="Q61" s="47" t="s">
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
+      <c r="Q61" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="47"/>
+      <c r="R61" s="66"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3641,28 +3604,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="64"/>
+      <c r="C66" s="63"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="65">
+      <c r="B67" s="46">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="65"/>
-      <c r="E67" s="69">
+      <c r="C67" s="46"/>
+      <c r="E67" s="47">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="65"/>
-      <c r="C68" s="65"/>
-      <c r="E68" s="69"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="E68" s="47"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3687,26 +3650,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="72" t="s">
+      <c r="B72" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="C72" s="73"/>
-      <c r="D72" s="73"/>
-      <c r="E72" s="73"/>
-      <c r="F72" s="73"/>
-      <c r="G72" s="73"/>
-      <c r="H72" s="73"/>
-      <c r="I72" s="74"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="49"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="50"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="75"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="76"/>
-      <c r="H73" s="76"/>
-      <c r="I73" s="77"/>
+      <c r="B73" s="51"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="53"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3733,10 +3696,10 @@
       <c r="I75" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K75" s="64" t="s">
+      <c r="K75" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="64"/>
+      <c r="L75" s="63"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3766,11 +3729,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="65">
+      <c r="K76" s="46">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="65"/>
+      <c r="L76" s="46"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3798,20 +3761,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -3822,16 +3781,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3842,8 +3805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,19 +4060,19 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="20" t="s">
+      <c r="B18" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="27">
         <v>45819</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="28" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4430,7 +4393,7 @@
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4448,21 +4411,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="81"/>
-      <c r="F2" s="79" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="75"/>
+      <c r="F2" s="73" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="J2" s="79" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="75"/>
+      <c r="J2" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="81"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="75"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="33" t="s">
@@ -4641,26 +4604,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="83"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="32">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="83"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="32">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>1.5833333333333333</v>
       </c>
-      <c r="J11" s="82" t="s">
+      <c r="J11" s="76" t="s">
         <v>186</v>
       </c>
-      <c r="K11" s="83"/>
+      <c r="K11" s="77"/>
       <c r="L11" s="32">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
New points - final exam PBL2
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0EE2A9-3B2E-4037-8903-BB049E272633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F574BF-2489-4E09-8598-D6F07679B0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -1068,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1116,22 +1116,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1215,39 +1199,54 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,33 +1265,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1310,12 +1294,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1680,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P3"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R70" sqref="R70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,60 +1688,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="62"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="63"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="H5" s="54" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="43"/>
+      <c r="H5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="K5" s="54" t="s">
+      <c r="I5" s="43"/>
+      <c r="K5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="43"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1831,7 +1809,9 @@
       <c r="K7" s="2">
         <v>12</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2">
+        <v>13.5</v>
+      </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2">
         <v>6</v>
@@ -1839,37 +1819,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="52"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="52"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="53">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>41.6</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="67"/>
-      <c r="G10" s="46">
+        <v>55.1</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="E10" s="55"/>
+      <c r="G10" s="53">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>24.4</v>
-      </c>
-      <c r="H10" s="46"/>
+        <v>10.899999999999999</v>
+      </c>
+      <c r="H10" s="53"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="68"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="E11" s="56"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1894,46 +1874,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="H17" s="54" t="s">
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="H17" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
-      <c r="L17" s="63" t="s">
+      <c r="I17" s="57"/>
+      <c r="J17" s="43"/>
+      <c r="L17" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="63"/>
+      <c r="M17" s="52"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="P17" s="38"/>
+      <c r="P17" s="34"/>
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -1960,12 +1940,12 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="53">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>85</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="O18" s="47">
+      <c r="M18" s="53"/>
+      <c r="O18" s="54">
         <v>4.5</v>
       </c>
     </row>
@@ -1994,9 +1974,9 @@
       <c r="J19" s="2">
         <v>19.5</v>
       </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="O19" s="47"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="O19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2021,62 +2001,62 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="50"/>
-      <c r="N23" s="46" t="s">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="46"/>
+      <c r="N23" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="O23" s="46"/>
+      <c r="O23" s="53"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="53"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="49"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="F26" s="66" t="s">
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="F26" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="54" t="s">
+      <c r="K26" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="L26" s="56"/>
+      <c r="L26" s="43"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -2109,9 +2089,9 @@
       <c r="L27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N27" s="69">
+      <c r="N27" s="66">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
-        <v>4.2133333333333329</v>
+        <v>4.2733333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2140,27 +2120,27 @@
         <v>20</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="N28" s="70"/>
+      <c r="N28" s="67"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="71">
-        <f>SUM(B28:C28)</f>
-        <v>23</v>
-      </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="F29" s="71">
+      <c r="B29" s="51">
+        <f>SUM(B28:D28)</f>
+        <v>24</v>
+      </c>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="F29" s="51">
         <v>5</v>
       </c>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="K29" s="71">
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="K29" s="51">
         <f>SUM(K28:L28)</f>
         <v>20</v>
       </c>
-      <c r="L29" s="71"/>
-      <c r="N29" s="38"/>
+      <c r="L29" s="51"/>
+      <c r="N29" s="34"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
@@ -2185,39 +2165,39 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="53"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="49"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="66"/>
+      <c r="C36" s="50"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="54" t="s">
+      <c r="E36" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="43"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
@@ -2264,10 +2244,10 @@
         <v>117</v>
       </c>
       <c r="C41" s="65"/>
-      <c r="F41" s="46" t="s">
+      <c r="F41" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="46"/>
+      <c r="G41" s="53"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -2323,7 +2303,7 @@
       <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="I44" s="63" t="s">
+      <c r="I44" s="52" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2334,7 +2314,7 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="I45" s="63"/>
+      <c r="I45" s="52"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2367,7 +2347,7 @@
       <c r="C48" s="2">
         <v>2</v>
       </c>
-      <c r="I48" s="38"/>
+      <c r="I48" s="34"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
@@ -2431,70 +2411,70 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="49"/>
-      <c r="N58" s="49"/>
-      <c r="O58" s="49"/>
-      <c r="P58" s="49"/>
-      <c r="Q58" s="49"/>
-      <c r="R58" s="49"/>
-      <c r="S58" s="50"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="45"/>
+      <c r="P58" s="45"/>
+      <c r="Q58" s="45"/>
+      <c r="R58" s="45"/>
+      <c r="S58" s="46"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="52"/>
-      <c r="M59" s="52"/>
-      <c r="N59" s="52"/>
-      <c r="O59" s="52"/>
-      <c r="P59" s="52"/>
-      <c r="Q59" s="52"/>
-      <c r="R59" s="52"/>
-      <c r="S59" s="53"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
+      <c r="R59" s="48"/>
+      <c r="S59" s="49"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="66" t="s">
+      <c r="B61" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="66"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="M61" s="66" t="s">
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="M61" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="N61" s="66"/>
-      <c r="O61" s="66"/>
-      <c r="P61" s="66"/>
-      <c r="R61" s="66" t="s">
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
+      <c r="P61" s="50"/>
+      <c r="R61" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="S61" s="66"/>
+      <c r="S61" s="50"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2589,66 +2569,49 @@
       <c r="P63" s="2">
         <v>20</v>
       </c>
-      <c r="R63" s="2"/>
-      <c r="S63" s="2"/>
+      <c r="R63" s="2">
+        <v>25</v>
+      </c>
+      <c r="S63" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="52"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G66" s="39" t="s">
+      <c r="G66" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="H66" s="78"/>
+      <c r="H66" s="11"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="46">
+      <c r="B67" s="53">
         <f>SUM(B63:K63,M63:P63,R63:S63,G67)</f>
-        <v>65</v>
-      </c>
-      <c r="C67" s="46"/>
-      <c r="E67" s="47"/>
-      <c r="G67" s="46">
+        <v>98</v>
+      </c>
+      <c r="C67" s="53"/>
+      <c r="E67" s="54">
+        <v>5</v>
+      </c>
+      <c r="G67" s="53">
         <v>9</v>
       </c>
-      <c r="H67" s="79"/>
+      <c r="H67" s="7"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="E68" s="47"/>
-      <c r="G68" s="46"/>
-      <c r="H68" s="79"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="53"/>
+      <c r="E68" s="54"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="R61:S61"/>
-    <mergeCell ref="B33:I34"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="B58:S59"/>
-    <mergeCell ref="M61:P61"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="G67:G68"/>
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2663,7 +2626,30 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="G67:G68"/>
     <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R61:S61"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B58:S59"/>
+    <mergeCell ref="M61:P61"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2704,60 +2690,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="50"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="53"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="56"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="43"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2839,28 +2825,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="52"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="53">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="67">
+      <c r="C10" s="53"/>
+      <c r="E10" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="68"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2885,40 +2871,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="F17" s="66" t="s">
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="F17" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="J17" s="63" t="s">
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="J17" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="63"/>
+      <c r="K17" s="52"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2942,12 +2928,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="53">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="M18" s="47">
+      <c r="K18" s="53"/>
+      <c r="M18" s="54">
         <v>5</v>
       </c>
     </row>
@@ -2970,9 +2956,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="M19" s="47"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="M19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2997,46 +2983,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="50"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="53"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="49"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="E26" s="54" t="s">
+      <c r="C26" s="50"/>
+      <c r="E26" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="I26" s="66" t="s">
+      <c r="F26" s="57"/>
+      <c r="G26" s="43"/>
+      <c r="I26" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3071,12 +3057,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="72">
+      <c r="M27" s="68">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="47">
+      <c r="O27" s="54">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3106,9 +3092,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="72"/>
+      <c r="M28" s="68"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="47"/>
+      <c r="O28" s="54"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3134,39 +3120,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="50"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="51"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="53"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="49"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="F35" s="66" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="F35" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3227,10 +3213,10 @@
         <v>35</v>
       </c>
       <c r="C40" s="65"/>
-      <c r="F40" s="46" t="s">
+      <c r="F40" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="53"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3286,7 +3272,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="63" t="s">
+      <c r="I43" s="52" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3303,7 +3289,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="63"/>
+      <c r="I44" s="52"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3447,67 +3433,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="49"/>
-      <c r="N58" s="49"/>
-      <c r="O58" s="49"/>
-      <c r="P58" s="49"/>
-      <c r="Q58" s="49"/>
-      <c r="R58" s="50"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="45"/>
+      <c r="P58" s="45"/>
+      <c r="Q58" s="45"/>
+      <c r="R58" s="46"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="52"/>
-      <c r="M59" s="52"/>
-      <c r="N59" s="52"/>
-      <c r="O59" s="52"/>
-      <c r="P59" s="52"/>
-      <c r="Q59" s="52"/>
-      <c r="R59" s="53"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
+      <c r="R59" s="49"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="66" t="s">
+      <c r="B61" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="66"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="M61" s="66" t="s">
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="M61" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="66"/>
-      <c r="O61" s="66"/>
-      <c r="Q61" s="66" t="s">
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
+      <c r="Q61" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="66"/>
+      <c r="R61" s="50"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3604,28 +3590,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="52"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="46">
+      <c r="B67" s="53">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="E67" s="47">
+      <c r="C67" s="53"/>
+      <c r="E67" s="54">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="E68" s="47"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="53"/>
+      <c r="E68" s="54"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3650,26 +3636,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="48" t="s">
+      <c r="B72" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="49"/>
-      <c r="H72" s="49"/>
-      <c r="I72" s="50"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="46"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="53"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="49"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3696,10 +3682,10 @@
       <c r="I75" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K75" s="63" t="s">
+      <c r="K75" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="63"/>
+      <c r="L75" s="52"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3729,11 +3715,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="46">
+      <c r="K76" s="53">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="46"/>
+      <c r="L76" s="53"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -3761,6 +3747,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B23:K24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B72:I73"/>
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="K76:L76"/>
@@ -3771,30 +3781,6 @@
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B23:K24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3806,7 +3792,7 @@
   <dimension ref="B1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,551 +3819,551 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="b">
+      <c r="B3" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="20">
         <v>45763</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="19" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="b">
+      <c r="B4" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="23">
         <v>45812</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="22" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="b">
+      <c r="B5" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="39">
         <v>45817</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="41" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="30"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="b">
+      <c r="B7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="23">
         <v>45729</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="22" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="b">
+      <c r="B8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="23">
         <v>45743</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="22" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="b">
+      <c r="B9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="23">
         <v>45757</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="22" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="b">
+      <c r="B10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="23">
         <v>45785</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="22" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="b">
+      <c r="B11" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="23">
         <v>45799</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="22" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="30"/>
+      <c r="C12" s="26"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="b">
+      <c r="B13" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="23">
         <v>45728</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="b">
+      <c r="B14" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="23">
         <v>45747</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="22" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="b">
+      <c r="B15" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="23">
         <v>45784</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="22" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="b">
+      <c r="B16" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="23">
         <v>45806</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="22" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="b">
+      <c r="B17" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="23">
         <v>45817</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="24" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="b">
+      <c r="B18" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="23">
         <v>45819</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="24" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="30"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="23">
         <v>45820</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="22" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="23">
         <v>45820</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="22" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="30"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="b">
+      <c r="B23" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="23">
         <v>45728</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="22" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="b">
+      <c r="B24" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="23">
         <v>45742</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="22" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="22" t="b">
+      <c r="B25" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="23">
         <v>45756</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="22" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="b">
+      <c r="B26" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="23">
         <v>45770</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="24" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="b">
+      <c r="B27" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="23">
         <v>45784</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="22" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="b">
+      <c r="B28" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="23">
         <v>45798</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="22" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="b">
+      <c r="B29" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="23">
         <v>45812</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="24" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="30"/>
+      <c r="C30" s="26"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="22" t="b">
+      <c r="B31" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="23">
         <v>45764</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="22" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="b">
+      <c r="B32" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="23">
         <v>45815</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="22" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="22" t="b">
+      <c r="B33" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="23">
         <v>45814</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="22" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="22" t="b">
+      <c r="B35" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D35" s="23">
         <v>45767</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="22" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="22" t="b">
+      <c r="B36" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="27">
+      <c r="D36" s="23">
         <v>45775</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="22" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="b">
+      <c r="B37" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="27">
+      <c r="D37" s="23">
         <v>45794</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="22" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="22" t="b">
+      <c r="B39" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D39" s="23">
         <v>45784</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="22" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="b">
+      <c r="B40" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D40" s="23">
         <v>45798</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="22" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="b">
+      <c r="B41" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D41" s="23">
         <v>45805</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F41" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4393,7 +4379,7 @@
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,53 +4397,53 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
-      <c r="F2" s="73" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="F2" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75"/>
-      <c r="J2" s="73" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="J2" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="75"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="31" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C4" s="14">
@@ -4466,14 +4452,14 @@
       <c r="D4" s="14">
         <v>4</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="32" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="14">
         <v>5</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="32" t="s">
         <v>187</v>
       </c>
       <c r="K4" s="14">
@@ -4482,7 +4468,7 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>122</v>
       </c>
       <c r="C5" s="2">
@@ -4491,14 +4477,14 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="33" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="33" t="s">
         <v>188</v>
       </c>
       <c r="K5" s="2">
@@ -4507,7 +4493,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="33" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="2">
@@ -4516,7 +4502,7 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="33" t="s">
         <v>77</v>
       </c>
       <c r="G6" s="2">
@@ -4525,7 +4511,7 @@
       <c r="H6" s="2">
         <v>4.5</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="33" t="s">
         <v>189</v>
       </c>
       <c r="K6" s="2">
@@ -4534,7 +4520,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="33" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="2">
@@ -4543,7 +4529,7 @@
       <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="33" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="2">
@@ -4552,7 +4538,7 @@
       <c r="H7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="33" t="s">
         <v>190</v>
       </c>
       <c r="K7" s="2">
@@ -4561,7 +4547,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>125</v>
       </c>
       <c r="C8" s="2">
@@ -4570,14 +4556,16 @@
       <c r="D8" s="2">
         <v>4.5</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="33" t="s">
         <v>80</v>
       </c>
       <c r="G8" s="2">
         <v>11</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="J8" s="37" t="s">
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="33" t="s">
         <v>191</v>
       </c>
       <c r="K8" s="2">
@@ -4586,7 +4574,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="33" t="s">
         <v>126</v>
       </c>
       <c r="C9" s="2">
@@ -4595,36 +4583,36 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="31"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="31"/>
+      <c r="J9" s="27"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="77"/>
-      <c r="D11" s="32">
+      <c r="C11" s="73"/>
+      <c r="D11" s="28">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="32">
+      <c r="G11" s="73"/>
+      <c r="H11" s="28">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
-        <v>1.5833333333333333</v>
-      </c>
-      <c r="J11" s="76" t="s">
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="J11" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="K11" s="77"/>
-      <c r="L11" s="32">
+      <c r="K11" s="73"/>
+      <c r="L11" s="28">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
New points - MAT3 and FIZ1 exams -> everything passed and holidays!@
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F574BF-2489-4E09-8598-D6F07679B0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C43C02-BBA6-40DA-B027-5612C705B080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="215">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Prez. końcowa</t>
   </si>
   <si>
-    <t>Do zdania brakuje:</t>
-  </si>
-  <si>
     <t>Ustny [30 pkt]</t>
   </si>
   <si>
@@ -338,12 +335,6 @@
     <t>Wykłady [20 + 20 pkt]</t>
   </si>
   <si>
-    <t>BONUS 1</t>
-  </si>
-  <si>
-    <t>BONUS 2</t>
-  </si>
-  <si>
     <t>Laby</t>
   </si>
   <si>
@@ -401,9 +392,6 @@
     <t>Egzamin [20+10 pkt]</t>
   </si>
   <si>
-    <t>W = 0,4E + 0,3C + 0,3L</t>
-  </si>
-  <si>
     <t>MAT1</t>
   </si>
   <si>
@@ -687,6 +675,15 @@
   </si>
   <si>
     <t>Mini-projekt [10 pkt]</t>
+  </si>
+  <si>
+    <t>Średnia:</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>W = (E/30)*0,4*5 + (C/25)*0,3*5 + 0,3L</t>
   </si>
 </sst>
 </file>
@@ -769,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,12 +782,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1121,32 +1112,32 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1156,47 +1147,47 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1205,28 +1196,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1247,24 +1238,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1280,13 +1253,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1294,6 +1267,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1658,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R70" sqref="R70"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1657,7 @@
     <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" style="1" customWidth="1"/>
@@ -1688,40 +1667,40 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="60"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="61"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="63"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1748,25 +1727,25 @@
     </row>
     <row r="6" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>24</v>
@@ -1816,7 +1795,9 @@
       <c r="N7" s="2">
         <v>6</v>
       </c>
-      <c r="P7" s="2"/>
+      <c r="P7" s="2">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
@@ -1826,30 +1807,27 @@
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="52"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="53">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>55.1</v>
+        <v>94.1</v>
       </c>
       <c r="C10" s="53"/>
-      <c r="E10" s="55"/>
-      <c r="G10" s="53">
-        <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>10.899999999999999</v>
-      </c>
-      <c r="H10" s="53"/>
+      <c r="E10" s="55">
+        <v>4</v>
+      </c>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
       <c r="E11" s="56"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1895,14 +1873,14 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
       <c r="H17" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="57"/>
       <c r="J17" s="43"/>
@@ -1917,28 +1895,28 @@
     </row>
     <row r="18" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="L18" s="53">
         <f>SUM(B19:F19,H19:J19)</f>
@@ -2015,7 +1993,7 @@
       <c r="K23" s="45"/>
       <c r="L23" s="46"/>
       <c r="N23" s="53" t="s">
-        <v>120</v>
+        <v>214</v>
       </c>
       <c r="O23" s="53"/>
       <c r="Q23" s="7"/>
@@ -2047,51 +2025,57 @@
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="F26" s="50" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G26" s="50"/>
       <c r="H26" s="50"/>
       <c r="I26" s="50"/>
       <c r="J26" s="7"/>
       <c r="K26" s="42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L26" s="43"/>
       <c r="N26" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="O26" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>73</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="N27" s="66">
+        <v>115</v>
+      </c>
+      <c r="N27" s="60">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
-        <v>4.2733333333333334</v>
+        <v>4.9399999999999995</v>
+      </c>
+      <c r="O27" s="54">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2119,8 +2103,11 @@
       <c r="K28" s="2">
         <v>20</v>
       </c>
-      <c r="L28" s="2"/>
-      <c r="N28" s="67"/>
+      <c r="L28" s="2">
+        <v>10</v>
+      </c>
+      <c r="N28" s="61"/>
+      <c r="O28" s="54"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="51">
@@ -2137,7 +2124,7 @@
       <c r="I29" s="51"/>
       <c r="K29" s="51">
         <f>SUM(K28:L28)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L29" s="51"/>
       <c r="N29" s="34"/>
@@ -2188,16 +2175,16 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="50"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="43"/>
+      <c r="E36" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
@@ -2207,16 +2194,13 @@
         <v>7</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="O37" s="7"/>
     </row>
@@ -2235,17 +2219,18 @@
         <f>G46</f>
         <v>29</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="G38" s="2">
+        <v>2</v>
+      </c>
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="C41" s="65"/>
+      <c r="B41" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="59"/>
       <c r="F41" s="53" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G41" s="53"/>
       <c r="I41" s="9" t="s">
@@ -2256,33 +2241,33 @@
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C42" s="2">
         <v>2</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G42" s="2">
         <v>9</v>
       </c>
       <c r="I42" s="2">
-        <f>SUM(B38:C38,E38:H38)</f>
-        <v>91</v>
+        <f>SUM(B38:C38,E38:G38)</f>
+        <v>93</v>
       </c>
       <c r="J42" s="7"/>
       <c r="L42" s="7"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C43" s="2">
         <v>2</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G43" s="2">
         <v>10</v>
@@ -2292,13 +2277,13 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2">
         <v>3</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G44" s="2">
         <v>10</v>
@@ -2309,7 +2294,7 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C45" s="2">
         <v>4</v>
@@ -2318,7 +2303,7 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C46" s="2">
         <v>4</v>
@@ -2336,13 +2321,13 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C48" s="2">
         <v>2</v>
@@ -2351,7 +2336,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C49" s="2">
         <v>2</v>
@@ -2359,7 +2344,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C50" s="2">
         <v>2</v>
@@ -2367,7 +2352,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2">
         <v>4</v>
@@ -2375,7 +2360,7 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C52" s="2"/>
     </row>
@@ -2466,7 +2451,7 @@
       <c r="J61" s="50"/>
       <c r="K61" s="50"/>
       <c r="M61" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N61" s="50"/>
       <c r="O61" s="50"/>
@@ -2502,7 +2487,7 @@
         <v>81</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>85</v>
@@ -2520,10 +2505,10 @@
         <v>71</v>
       </c>
       <c r="R62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S62" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="S62" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -2540,10 +2525,10 @@
         <v>2</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H63" s="2">
         <v>2</v>
@@ -2573,7 +2558,7 @@
         <v>25</v>
       </c>
       <c r="S63" s="2">
-        <v>8</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
@@ -2585,13 +2570,13 @@
         <v>67</v>
       </c>
       <c r="G66" s="35" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="53">
-        <f>SUM(B63:K63,M63:P63,R63:S63,G67)</f>
+        <f>_xlfn.CEILING.MATH(SUM(B63:K63,M63:P63,R63:S63,G67))</f>
         <v>98</v>
       </c>
       <c r="C67" s="53"/>
@@ -2611,7 +2596,7 @@
       <c r="H68" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="37">
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -2624,10 +2609,9 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="N23:O24"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="B9:C9"/>
@@ -2635,7 +2619,6 @@
     <mergeCell ref="G67:G68"/>
     <mergeCell ref="E67:E68"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H11"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="F26:I26"/>
@@ -2650,6 +2633,7 @@
     <mergeCell ref="M61:P61"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E36:G36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2691,7 +2675,7 @@
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
@@ -2872,7 +2856,7 @@
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C14" s="45"/>
       <c r="D14" s="45"/>
@@ -2984,7 +2968,7 @@
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" s="44" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
@@ -3057,7 +3041,7 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="68">
+      <c r="M27" s="62">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
@@ -3092,7 +3076,7 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="68"/>
+      <c r="M28" s="62"/>
       <c r="N28" s="7"/>
       <c r="O28" s="54"/>
       <c r="P28" s="8"/>
@@ -3121,7 +3105,7 @@
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="44" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="45"/>
@@ -3209,10 +3193,10 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="65"/>
+      <c r="C40" s="59"/>
       <c r="F40" s="53" t="s">
         <v>36</v>
       </c>
@@ -3434,7 +3418,7 @@
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B58" s="44" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C58" s="45"/>
       <c r="D58" s="45"/>
@@ -3637,7 +3621,7 @@
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B72" s="44" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C72" s="45"/>
       <c r="D72" s="45"/>
@@ -3659,28 +3643,28 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="G75" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="H75" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="I75" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="K75" s="52" t="s">
         <v>22</v>
@@ -3792,7 +3776,7 @@
   <dimension ref="B1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,16 +3790,16 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -3829,10 +3813,10 @@
         <v>45763</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -3846,10 +3830,10 @@
         <v>45812</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -3863,10 +3847,10 @@
         <v>45817</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -3883,10 +3867,10 @@
         <v>45729</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -3900,10 +3884,10 @@
         <v>45743</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -3917,10 +3901,10 @@
         <v>45757</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -3934,10 +3918,10 @@
         <v>45785</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -3951,10 +3935,10 @@
         <v>45799</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -3965,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D13" s="23">
         <v>45728</v>
@@ -3974,7 +3958,7 @@
         <v>84</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -3982,16 +3966,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D14" s="23">
         <v>45747</v>
       </c>
       <c r="E14" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -3999,16 +3983,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D15" s="23">
         <v>45784</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -4016,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D16" s="23">
         <v>45806</v>
@@ -4025,7 +4009,7 @@
         <v>85</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -4033,16 +4017,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D17" s="23">
         <v>45817</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -4050,16 +4034,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D18" s="23">
         <v>45819</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -4071,13 +4055,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D20" s="23">
         <v>45820</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -4085,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D21" s="23">
         <v>45820</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -4109,10 +4093,10 @@
         <v>45728</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -4126,10 +4110,10 @@
         <v>45742</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4143,10 +4127,10 @@
         <v>45756</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -4160,10 +4144,10 @@
         <v>45770</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -4177,10 +4161,10 @@
         <v>45784</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -4194,10 +4178,10 @@
         <v>45798</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -4211,10 +4195,10 @@
         <v>45812</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -4231,10 +4215,10 @@
         <v>45764</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -4248,7 +4232,7 @@
         <v>45815</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -4262,10 +4246,10 @@
         <v>45814</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -4279,10 +4263,10 @@
         <v>45767</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -4296,7 +4280,7 @@
         <v>45775</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -4310,10 +4294,10 @@
         <v>45794</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -4327,10 +4311,10 @@
         <v>45784</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -4344,10 +4328,10 @@
         <v>45798</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -4361,10 +4345,10 @@
         <v>45805</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4379,7 +4363,7 @@
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,54 +4381,54 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="69" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="71"/>
-      <c r="F2" s="69" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
-      <c r="J2" s="69" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
+      <c r="B2" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
+      <c r="F2" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="64"/>
+      <c r="H2" s="65"/>
+      <c r="J2" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4458,9 +4442,11 @@
       <c r="G4" s="14">
         <v>5</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="14">
+        <v>4</v>
+      </c>
       <c r="J4" s="32" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K4" s="14">
         <v>4</v>
@@ -4469,7 +4455,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -4483,9 +4469,11 @@
       <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
       <c r="J5" s="33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K5" s="2">
         <v>4</v>
@@ -4494,7 +4482,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4512,7 +4500,7 @@
         <v>4.5</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K6" s="2">
         <v>5</v>
@@ -4521,7 +4509,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4539,7 +4527,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K7" s="2">
         <v>5</v>
@@ -4548,7 +4536,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -4566,7 +4554,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K8" s="2">
         <v>12</v>
@@ -4575,7 +4563,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -4592,26 +4580,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" s="73"/>
+      <c r="B11" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="67"/>
       <c r="D11" s="28">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" s="73"/>
+      <c r="F11" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="67"/>
       <c r="H11" s="28">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
-        <v>3.4166666666666665</v>
-      </c>
-      <c r="J11" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="K11" s="73"/>
+        <v>4.75</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11" s="67"/>
       <c r="L11" s="28">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
2nd semester successfully ended - final points and marks
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C43C02-BBA6-40DA-B027-5612C705B080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405FF14-EBBA-4923-9B6D-DAC24ED607FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="25080" yWindow="300" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1267,12 +1267,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1637,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="F41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,7 +1785,9 @@
       <c r="L7" s="2">
         <v>13.5</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
       <c r="N7" s="2">
         <v>6</v>
       </c>
@@ -1807,27 +1803,27 @@
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="53">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
-        <v>94.1</v>
+        <v>99.1</v>
       </c>
       <c r="C10" s="53"/>
       <c r="E10" s="55">
         <v>4</v>
       </c>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
       <c r="E11" s="56"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2612,6 +2608,7 @@
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="O27:O28"/>
+    <mergeCell ref="H17:J17"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="B9:C9"/>
@@ -2620,7 +2617,6 @@
     <mergeCell ref="E67:E68"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="B23:L24"/>
@@ -2645,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5356A30-E1AA-4069-A4C8-FC0BE8204C56}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,8 +3771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated schedule - 3rd sem
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405FF14-EBBA-4923-9B6D-DAC24ED607FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB201D0-AF96-4BBA-AE1A-A92AE39289F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="300" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="II-semestr-25L" sheetId="1" r:id="rId1"/>
-    <sheet name="I-semestr-24Z" sheetId="2" r:id="rId2"/>
-    <sheet name="Terminy" sheetId="3" r:id="rId3"/>
-    <sheet name="Ostateczne-oceny" sheetId="4" r:id="rId4"/>
+    <sheet name="III-semestr-25Z" sheetId="5" r:id="rId1"/>
+    <sheet name="II-semestr-25L" sheetId="1" r:id="rId2"/>
+    <sheet name="I-semestr-24Z" sheetId="2" r:id="rId3"/>
+    <sheet name="Terminy 25L" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Terminy 25Z" sheetId="8" r:id="rId5"/>
+    <sheet name="Ostateczne-oceny" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="316">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -684,15 +686,319 @@
   </si>
   <si>
     <t>W = (E/30)*0,4*5 + (C/25)*0,3*5 + 0,3L</t>
+  </si>
+  <si>
+    <t>Lab1</t>
+  </si>
+  <si>
+    <t>Lab2</t>
+  </si>
+  <si>
+    <t>Lab3</t>
+  </si>
+  <si>
+    <t>Lab4</t>
+  </si>
+  <si>
+    <t>Lab5</t>
+  </si>
+  <si>
+    <t>Lab6</t>
+  </si>
+  <si>
+    <t>11 grudnia</t>
+  </si>
+  <si>
+    <t>6 listopada</t>
+  </si>
+  <si>
+    <t>19 listopada</t>
+  </si>
+  <si>
+    <t>3 grudnia</t>
+  </si>
+  <si>
+    <t>18 grudnia</t>
+  </si>
+  <si>
+    <t>15 stycznia</t>
+  </si>
+  <si>
+    <t>Badanie właściwości sygnałów z modulacjami cyfrowymi</t>
+  </si>
+  <si>
+    <t>Badanie kanału propagacyjnego</t>
+  </si>
+  <si>
+    <t>Badanie podstawowych elementów toru radiowego</t>
+  </si>
+  <si>
+    <t>Badanie anten</t>
+  </si>
+  <si>
+    <t>Badanie sygnałów CDMA</t>
+  </si>
+  <si>
+    <t>Badanie sygnałów OFDM</t>
+  </si>
+  <si>
+    <t>15 października</t>
+  </si>
+  <si>
+    <t>Ćwiczenia 1</t>
+  </si>
+  <si>
+    <t>22 października</t>
+  </si>
+  <si>
+    <t>29 października</t>
+  </si>
+  <si>
+    <t>17 grudnia</t>
+  </si>
+  <si>
+    <t>Ćwiczenia 4</t>
+  </si>
+  <si>
+    <t>Ćwiczenia 2</t>
+  </si>
+  <si>
+    <t>Ćwiczenia 3</t>
+  </si>
+  <si>
+    <t>Pomiary: obiekty i miary</t>
+  </si>
+  <si>
+    <t>Analiza sygnałów w dziedzinach czasu i częstotliwości</t>
+  </si>
+  <si>
+    <t>Generatory sygnałowe i analizatory obwodów</t>
+  </si>
+  <si>
+    <t>Pomiary sygnałów CDMA i OFDM. Przykład bilansu łącza radiowego</t>
+  </si>
+  <si>
+    <t>Godziny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:15-16:10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:15-16:50 </t>
+  </si>
+  <si>
+    <t>12:00-15:00</t>
+  </si>
+  <si>
+    <t>14:00-17:00</t>
+  </si>
+  <si>
+    <t>8:00-11:00</t>
+  </si>
+  <si>
+    <t>20 października</t>
+  </si>
+  <si>
+    <t>14:15-17:00</t>
+  </si>
+  <si>
+    <t>Sala</t>
+  </si>
+  <si>
+    <t>DS400</t>
+  </si>
+  <si>
+    <t>17 listopada</t>
+  </si>
+  <si>
+    <t>24 listopada</t>
+  </si>
+  <si>
+    <t>15 grudnia</t>
+  </si>
+  <si>
+    <t>12 stycznia</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Kolokwia [2*25 pkt]</t>
+  </si>
+  <si>
+    <t>Laboratoria [5*5 pkt]</t>
+  </si>
+  <si>
+    <t>Projekty [25 pkt]</t>
+  </si>
+  <si>
+    <t>1. Kolosy: minimum 11 pkt z każdego</t>
+  </si>
+  <si>
+    <t>2. Labki: minimum 2 pkt z każdego</t>
+  </si>
+  <si>
+    <t>3. Labki: minimum 13 pkt łącznie</t>
+  </si>
+  <si>
+    <t>4. Projekty: minimum 13 pkt łącznie</t>
+  </si>
+  <si>
+    <t>ZALICZENIE</t>
+  </si>
+  <si>
+    <t>5. SUMA &gt; 51 pkt</t>
+  </si>
+  <si>
+    <t>Ćwiczenia [4*1,5 pkt]</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Laboratoria [6*4 pkt]</t>
+  </si>
+  <si>
+    <t>Kolokwia [2*15 pkt]</t>
+  </si>
+  <si>
+    <t>Egzamin [40 pkt]</t>
+  </si>
+  <si>
+    <t>K1 [12 pkt]</t>
+  </si>
+  <si>
+    <t>K2 [12 pkt]</t>
+  </si>
+  <si>
+    <t>Aktywność [2 pkt]</t>
+  </si>
+  <si>
+    <t>Egzamin [30 + 20 pkt]</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>Zad 1</t>
+  </si>
+  <si>
+    <t>Zad 2</t>
+  </si>
+  <si>
+    <t>Zad 3</t>
+  </si>
+  <si>
+    <t>Zad 4</t>
+  </si>
+  <si>
+    <t>Zad 5</t>
+  </si>
+  <si>
+    <t>Zad 6</t>
+  </si>
+  <si>
+    <t>Etap 1</t>
+  </si>
+  <si>
+    <t>Etap 2</t>
+  </si>
+  <si>
+    <t>Etap 3</t>
+  </si>
+  <si>
+    <t>Prezentacja</t>
+  </si>
+  <si>
+    <t>Etap 1 [3 + 2 pkt]</t>
+  </si>
+  <si>
+    <t>Etap 2 [6 + 4 pkt]</t>
+  </si>
+  <si>
+    <t>Etap 3 [6 + 4 pkt]</t>
+  </si>
+  <si>
+    <t>18/19 listopada</t>
+  </si>
+  <si>
+    <t>Projekt - etap 1</t>
+  </si>
+  <si>
+    <t>16/17 grudnia</t>
+  </si>
+  <si>
+    <t>Projekt - etap 2</t>
+  </si>
+  <si>
+    <t>30 stycznia</t>
+  </si>
+  <si>
+    <t>Projekt - prezentacja finalna</t>
+  </si>
+  <si>
+    <t>Warsztaty [15 * 3 pkt]</t>
+  </si>
+  <si>
+    <t>Egzamin [30 pkt]</t>
+  </si>
+  <si>
+    <t>Projekt [25 pkt]</t>
+  </si>
+  <si>
+    <t>ANG</t>
+  </si>
+  <si>
+    <t>Testy cząstkowe</t>
+  </si>
+  <si>
+    <t>Starter Unit</t>
+  </si>
+  <si>
+    <t>4+</t>
+  </si>
+  <si>
+    <t>1. Warsztaty: minimum 50 %</t>
+  </si>
+  <si>
+    <t>2. Projekt: minimum 50 %</t>
+  </si>
+  <si>
+    <t>3. Egzamin: minimum 50 %</t>
+  </si>
+  <si>
+    <t>1. Ćwiczenia: minimum 12 pkt</t>
+  </si>
+  <si>
+    <t>2. Egzamin: minimum 26 pkt</t>
+  </si>
+  <si>
+    <t>1. Całość: minimum 51 pkt</t>
+  </si>
+  <si>
+    <t>2. Egzamin: minimum 21 pkt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-415]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -766,7 +1072,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -806,6 +1112,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEDF4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1190,51 +1508,102 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,6 +1635,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,11 +1684,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDEEDF4"/>
       <color rgb="FFFF8585"/>
       <color rgb="FFFDBF8B"/>
       <color rgb="FFFDAF6F"/>
       <color rgb="FFFFCC66"/>
-      <color rgb="FFDEEDF4"/>
       <color rgb="FFE3EAEF"/>
     </mruColors>
   </colors>
@@ -1628,11 +2036,892 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFDB1E6-87C0-4917-B2B5-BFB3BFC54144}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:V52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="85" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87"/>
+      <c r="R2" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="90"/>
+      <c r="R3" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="68"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R4" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="68"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="E5" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="K5" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="R5" s="66" t="s">
+        <v>266</v>
+      </c>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="68"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>283</v>
+      </c>
+      <c r="L6" s="49" t="s">
+        <v>284</v>
+      </c>
+      <c r="M6" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="O6" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="P6" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="R6" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="68"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="R7" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="68"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="53">
+        <f>SUM(B7:C7,E7:I7,K7:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="64"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="65"/>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="87"/>
+      <c r="S14" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="T14" s="69"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="69"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="89"/>
+      <c r="P15" s="89"/>
+      <c r="Q15" s="90"/>
+      <c r="S15" s="66" t="s">
+        <v>314</v>
+      </c>
+      <c r="T15" s="67"/>
+      <c r="U15" s="67"/>
+      <c r="V15" s="68"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S16" s="66" t="s">
+        <v>315</v>
+      </c>
+      <c r="T16" s="67"/>
+      <c r="U16" s="67"/>
+      <c r="V16" s="68"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="52" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="G17" s="52" t="s">
+        <v>275</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="N17" s="52" t="s">
+        <v>276</v>
+      </c>
+      <c r="O17" s="52"/>
+      <c r="Q17" s="51" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="K18" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="L18" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="N18" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="O18" s="49" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q18" s="61"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="Q19" s="62"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="53">
+        <f>SUM(B19:E19,G19:L19,N19:O19,Q18)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="53"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="64"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="65"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="86"/>
+      <c r="Q26" s="87"/>
+      <c r="S26" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="T26" s="69"/>
+      <c r="U26" s="69"/>
+      <c r="V26" s="69"/>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="90"/>
+      <c r="S27" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="T27" s="67"/>
+      <c r="U27" s="67"/>
+      <c r="V27" s="68"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S28" s="66" t="s">
+        <v>313</v>
+      </c>
+      <c r="T28" s="67"/>
+      <c r="U28" s="67"/>
+      <c r="V28" s="68"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="G29" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="H29" s="52"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" s="53"/>
+      <c r="G30" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+    </row>
+    <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="86"/>
+      <c r="L34" s="86"/>
+      <c r="M34" s="86"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="86"/>
+      <c r="Q34" s="87"/>
+      <c r="S34" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="69"/>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="Q35" s="90"/>
+      <c r="S35" s="66" t="s">
+        <v>309</v>
+      </c>
+      <c r="T35" s="67"/>
+      <c r="U35" s="67"/>
+      <c r="V35" s="68"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S36" s="66" t="s">
+        <v>310</v>
+      </c>
+      <c r="T36" s="67"/>
+      <c r="U36" s="67"/>
+      <c r="V36" s="68"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="52" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
+      <c r="S37" s="66" t="s">
+        <v>311</v>
+      </c>
+      <c r="T37" s="67"/>
+      <c r="U37" s="67"/>
+      <c r="V37" s="68"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B38" s="49" t="s">
+        <v>282</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="M38" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="N38" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="O38" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="P38" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B41" s="52" t="s">
+        <v>304</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="I41" s="52" t="s">
+        <v>303</v>
+      </c>
+      <c r="J41" s="52"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B42" s="91" t="s">
+        <v>293</v>
+      </c>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="G42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+    </row>
+    <row r="43" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91"/>
+    </row>
+    <row r="45" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+    </row>
+    <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B47" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="86"/>
+      <c r="P47" s="86"/>
+      <c r="Q47" s="87"/>
+    </row>
+    <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="89"/>
+      <c r="N48" s="89"/>
+      <c r="O48" s="89"/>
+      <c r="P48" s="89"/>
+      <c r="Q48" s="90"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="52" t="s">
+        <v>306</v>
+      </c>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+    </row>
+    <row r="51" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="49" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="49" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="B47:Q48"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="S34:V34"/>
+    <mergeCell ref="S35:V35"/>
+    <mergeCell ref="S36:V36"/>
+    <mergeCell ref="S37:V37"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J44"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="S28:V28"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="S15:V15"/>
+    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B14:Q15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B26:Q27"/>
+    <mergeCell ref="B37:P37"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B34:Q35"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="F41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,60 +2950,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="57"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="60"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="43"/>
-      <c r="H5" s="42" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="71"/>
+      <c r="H5" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="43"/>
-      <c r="K5" s="42" t="s">
+      <c r="I5" s="71"/>
+      <c r="K5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="43"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="71"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1796,10 +3085,10 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
@@ -1812,7 +3101,7 @@
         <v>99.1</v>
       </c>
       <c r="C10" s="53"/>
-      <c r="E10" s="55">
+      <c r="E10" s="64">
         <v>4</v>
       </c>
       <c r="G10" s="7"/>
@@ -1821,7 +3110,7 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
-      <c r="E11" s="56"/>
+      <c r="E11" s="65"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
@@ -1848,42 +3137,42 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="57"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="H17" s="42" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="H17" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="57"/>
-      <c r="J17" s="43"/>
-      <c r="L17" s="52" t="s">
+      <c r="I17" s="74"/>
+      <c r="J17" s="71"/>
+      <c r="L17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="52"/>
+      <c r="M17" s="63"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1919,7 +3208,7 @@
         <v>85</v>
       </c>
       <c r="M18" s="53"/>
-      <c r="O18" s="54">
+      <c r="O18" s="73">
         <v>4.5</v>
       </c>
     </row>
@@ -1950,7 +3239,7 @@
       </c>
       <c r="L19" s="53"/>
       <c r="M19" s="53"/>
-      <c r="O19" s="54"/>
+      <c r="O19" s="73"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1975,19 +3264,19 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
       <c r="N23" s="53" t="s">
         <v>214</v>
       </c>
@@ -1997,17 +3286,17 @@
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="49"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="60"/>
       <c r="N24" s="53"/>
       <c r="O24" s="53"/>
       <c r="Q24" s="7"/>
@@ -2015,22 +3304,22 @@
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="F26" s="50" t="s">
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="F26" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="42" t="s">
+      <c r="K26" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="L26" s="43"/>
+      <c r="L26" s="71"/>
       <c r="N26" s="9" t="s">
         <v>212</v>
       </c>
@@ -2066,11 +3355,11 @@
       <c r="L27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N27" s="60">
+      <c r="N27" s="77">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.9399999999999995</v>
       </c>
-      <c r="O27" s="54">
+      <c r="O27" s="73">
         <v>5</v>
       </c>
     </row>
@@ -2102,27 +3391,27 @@
       <c r="L28" s="2">
         <v>10</v>
       </c>
-      <c r="N28" s="61"/>
-      <c r="O28" s="54"/>
+      <c r="N28" s="78"/>
+      <c r="O28" s="73"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="51">
+      <c r="B29" s="72">
         <f>SUM(B28:D28)</f>
         <v>24</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="F29" s="51">
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="F29" s="72">
         <v>5</v>
       </c>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="K29" s="51">
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="K29" s="72">
         <f>SUM(K28:L28)</f>
         <v>30</v>
       </c>
-      <c r="L29" s="51"/>
+      <c r="L29" s="72"/>
       <c r="N29" s="34"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2148,38 +3437,38 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="46"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="57"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="47"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="49"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="50"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,10 +3510,10 @@
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="76"/>
       <c r="F41" s="53" t="s">
         <v>99</v>
       </c>
@@ -2284,7 +3573,7 @@
       <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="I44" s="52" t="s">
+      <c r="I44" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2295,7 +3584,7 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="I45" s="52"/>
+      <c r="I45" s="63"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -2392,70 +3681,70 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
-      <c r="O58" s="45"/>
-      <c r="P58" s="45"/>
-      <c r="Q58" s="45"/>
-      <c r="R58" s="45"/>
-      <c r="S58" s="46"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="56"/>
+      <c r="Q58" s="56"/>
+      <c r="R58" s="56"/>
+      <c r="S58" s="57"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="47"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="48"/>
-      <c r="M59" s="48"/>
-      <c r="N59" s="48"/>
-      <c r="O59" s="48"/>
-      <c r="P59" s="48"/>
-      <c r="Q59" s="48"/>
-      <c r="R59" s="48"/>
-      <c r="S59" s="49"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="59"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="59"/>
+      <c r="R59" s="59"/>
+      <c r="S59" s="60"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="M61" s="50" t="s">
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54"/>
+      <c r="M61" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="N61" s="50"/>
-      <c r="O61" s="50"/>
-      <c r="P61" s="50"/>
-      <c r="R61" s="50" t="s">
+      <c r="N61" s="54"/>
+      <c r="O61" s="54"/>
+      <c r="P61" s="54"/>
+      <c r="R61" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="S61" s="50"/>
+      <c r="S61" s="54"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2558,10 +3847,10 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="52" t="s">
+      <c r="B66" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="52"/>
+      <c r="C66" s="63"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
@@ -2576,7 +3865,7 @@
         <v>98</v>
       </c>
       <c r="C67" s="53"/>
-      <c r="E67" s="54">
+      <c r="E67" s="73">
         <v>5</v>
       </c>
       <c r="G67" s="53">
@@ -2587,7 +3876,7 @@
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="53"/>
       <c r="C68" s="53"/>
-      <c r="E68" s="54"/>
+      <c r="E68" s="73"/>
       <c r="G68" s="53"/>
       <c r="H68" s="7"/>
     </row>
@@ -2637,8 +3926,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5356A30-E1AA-4069-A4C8-FC0BE8204C56}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -2670,60 +3962,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="57"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="60"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="43"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="71"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2805,10 +4097,10 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="63"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
@@ -2819,14 +4111,14 @@
         <v>110</v>
       </c>
       <c r="C10" s="53"/>
-      <c r="E10" s="55">
+      <c r="E10" s="64">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
-      <c r="E11" s="56"/>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2851,40 +4143,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="57"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="F17" s="50" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="F17" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="J17" s="52" t="s">
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="J17" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="52"/>
+      <c r="K17" s="63"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -2913,7 +4205,7 @@
         <v>93</v>
       </c>
       <c r="K18" s="53"/>
-      <c r="M18" s="54">
+      <c r="M18" s="73">
         <v>5</v>
       </c>
     </row>
@@ -2938,7 +4230,7 @@
       </c>
       <c r="J19" s="53"/>
       <c r="K19" s="53"/>
-      <c r="M19" s="54"/>
+      <c r="M19" s="73"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -2963,46 +4255,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="57"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="49"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="60"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="E26" s="42" t="s">
+      <c r="C26" s="54"/>
+      <c r="E26" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="43"/>
-      <c r="I26" s="50" t="s">
+      <c r="F26" s="74"/>
+      <c r="G26" s="71"/>
+      <c r="I26" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -3037,12 +4329,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="62">
+      <c r="M27" s="79">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="54">
+      <c r="O27" s="73">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -3072,9 +4364,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="62"/>
+      <c r="M28" s="79"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="54"/>
+      <c r="O28" s="73"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3100,39 +4392,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="46"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="57"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="47"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="49"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="F35" s="50" t="s">
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="F35" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -3189,10 +4481,10 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="59"/>
+      <c r="C40" s="76"/>
       <c r="F40" s="53" t="s">
         <v>36</v>
       </c>
@@ -3252,7 +4544,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="52" t="s">
+      <c r="I43" s="63" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3269,7 +4561,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="52"/>
+      <c r="I44" s="63"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3413,67 +4705,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
-      <c r="O58" s="45"/>
-      <c r="P58" s="45"/>
-      <c r="Q58" s="45"/>
-      <c r="R58" s="46"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="56"/>
+      <c r="Q58" s="56"/>
+      <c r="R58" s="57"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="47"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="48"/>
-      <c r="M59" s="48"/>
-      <c r="N59" s="48"/>
-      <c r="O59" s="48"/>
-      <c r="P59" s="48"/>
-      <c r="Q59" s="48"/>
-      <c r="R59" s="49"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="59"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="59"/>
+      <c r="R59" s="60"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="M61" s="50" t="s">
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54"/>
+      <c r="M61" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="50"/>
-      <c r="O61" s="50"/>
-      <c r="Q61" s="50" t="s">
+      <c r="N61" s="54"/>
+      <c r="O61" s="54"/>
+      <c r="Q61" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="50"/>
+      <c r="R61" s="54"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3570,10 +4862,10 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="52" t="s">
+      <c r="B66" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="52"/>
+      <c r="C66" s="63"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
@@ -3584,14 +4876,14 @@
         <v>85.5</v>
       </c>
       <c r="C67" s="53"/>
-      <c r="E67" s="54">
+      <c r="E67" s="73">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B68" s="53"/>
       <c r="C68" s="53"/>
-      <c r="E68" s="54"/>
+      <c r="E68" s="73"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -3616,26 +4908,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="44" t="s">
+      <c r="B72" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="46"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="56"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
+      <c r="G72" s="56"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="57"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="47"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="49"/>
+      <c r="B73" s="58"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="60"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -3662,10 +4954,10 @@
       <c r="I75" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K75" s="52" t="s">
+      <c r="K75" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="52"/>
+      <c r="L75" s="63"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -3767,12 +5059,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA0BBB-B59A-4C0E-8304-D0FA810EECB4}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,8 +5649,417 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD1FAA5-236E-4DD4-8E6C-D46CD3E83407}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
+  <dimension ref="B1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="97" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="97" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="97" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H4" s="2">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="2">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>296</v>
+      </c>
+      <c r="E20" s="93" t="s">
+        <v>289</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA352BE-3E69-4CCA-8EEB-A9094B74606F}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4377,21 +6081,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="80" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="63" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="82"/>
+      <c r="F2" s="80" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="J2" s="63" t="s">
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="J2" s="80" t="s">
         <v>190</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="82"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
@@ -4576,26 +6280,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="28">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="67"/>
+      <c r="G11" s="84"/>
       <c r="H11" s="28">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>4.75</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="84"/>
       <c r="L11" s="28">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
Updated schedule - FIZ2 colloquium
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB201D0-AF96-4BBA-AE1A-A92AE39289F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A983F3-682A-4E4A-8C85-CD5E131CE62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="III-semestr-25Z" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="318">
   <si>
     <t>1. Krypto</t>
   </si>
@@ -989,6 +989,12 @@
   </si>
   <si>
     <t>2. Egzamin: minimum 21 pkt</t>
+  </si>
+  <si>
+    <t>14 listopada</t>
+  </si>
+  <si>
+    <t>Kolos 1</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1538,15 +1544,81 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1565,60 +1637,30 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1635,45 +1677,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2042,7 +2045,7 @@
   </sheetPr>
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -2060,87 +2063,87 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="87"/>
-      <c r="R2" s="69" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
+      <c r="R2" s="64" t="s">
         <v>268</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90"/>
-      <c r="R3" s="66" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="62"/>
+      <c r="R3" s="65" t="s">
         <v>264</v>
       </c>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="68"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="67"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="65" t="s">
         <v>265</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="67"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="63" t="s">
         <v>261</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="E5" s="52" t="s">
+      <c r="C5" s="63"/>
+      <c r="E5" s="63" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="K5" s="52" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="K5" s="63" t="s">
         <v>263</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="R5" s="66" t="s">
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="R5" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="68"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="67"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="49" t="s">
@@ -2182,12 +2185,12 @@
       <c r="P6" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="R6" s="66" t="s">
+      <c r="R6" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="68"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="67"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="50"/>
@@ -2203,37 +2206,37 @@
       <c r="N7" s="50"/>
       <c r="O7" s="50"/>
       <c r="P7" s="50"/>
-      <c r="R7" s="66" t="s">
+      <c r="R7" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="68"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="67"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="1"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="53">
+      <c r="B10" s="70">
         <f>SUM(B7:C7,E7:I7,K7:P7)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="64"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="65"/>
+      <c r="E11" s="72"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2261,82 +2264,82 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="87"/>
-      <c r="S14" s="69" t="s">
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="59"/>
+      <c r="S14" s="64" t="s">
         <v>268</v>
       </c>
-      <c r="T14" s="69"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="69"/>
+      <c r="T14" s="64"/>
+      <c r="U14" s="64"/>
+      <c r="V14" s="64"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="88"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="90"/>
-      <c r="S15" s="66" t="s">
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="62"/>
+      <c r="S15" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="T15" s="67"/>
-      <c r="U15" s="67"/>
-      <c r="V15" s="68"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S16" s="66" t="s">
+      <c r="S16" s="65" t="s">
         <v>315</v>
       </c>
-      <c r="T16" s="67"/>
-      <c r="U16" s="67"/>
-      <c r="V16" s="68"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="67"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="G17" s="52" t="s">
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="G17" s="63" t="s">
         <v>275</v>
       </c>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="N17" s="52" t="s">
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="N17" s="63" t="s">
         <v>276</v>
       </c>
-      <c r="O17" s="52"/>
+      <c r="O17" s="63"/>
       <c r="Q17" s="51" t="s">
         <v>277</v>
       </c>
@@ -2378,7 +2381,7 @@
       <c r="O18" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="Q18" s="61"/>
+      <c r="Q18" s="73"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" s="49"/>
@@ -2393,32 +2396,32 @@
       <c r="L19" s="49"/>
       <c r="N19" s="49"/>
       <c r="O19" s="49"/>
-      <c r="Q19" s="62"/>
+      <c r="Q19" s="74"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="63"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="1"/>
       <c r="E21" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="53">
+      <c r="B22" s="70">
         <f>SUM(B19:E19,G19:L19,N19:O19,Q18)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="53"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="64"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="65"/>
+      <c r="E23" s="72"/>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
@@ -2446,74 +2449,74 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="86"/>
-      <c r="M26" s="86"/>
-      <c r="N26" s="86"/>
-      <c r="O26" s="86"/>
-      <c r="P26" s="86"/>
-      <c r="Q26" s="87"/>
-      <c r="S26" s="69" t="s">
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="59"/>
+      <c r="S26" s="64" t="s">
         <v>268</v>
       </c>
-      <c r="T26" s="69"/>
-      <c r="U26" s="69"/>
-      <c r="V26" s="69"/>
+      <c r="T26" s="64"/>
+      <c r="U26" s="64"/>
+      <c r="V26" s="64"/>
     </row>
     <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="88"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="90"/>
-      <c r="S27" s="66" t="s">
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="62"/>
+      <c r="S27" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="T27" s="67"/>
-      <c r="U27" s="67"/>
-      <c r="V27" s="68"/>
+      <c r="T27" s="66"/>
+      <c r="U27" s="66"/>
+      <c r="V27" s="67"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S28" s="66" t="s">
+      <c r="S28" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="T28" s="67"/>
-      <c r="U28" s="67"/>
-      <c r="V28" s="68"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="67"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="G29" s="52" t="s">
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="G29" s="63" t="s">
         <v>281</v>
       </c>
-      <c r="H29" s="52"/>
+      <c r="H29" s="63"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -2522,10 +2525,10 @@
       <c r="C30" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="70" t="s">
         <v>280</v>
       </c>
-      <c r="E30" s="53"/>
+      <c r="E30" s="70"/>
       <c r="G30" s="49" t="s">
         <v>73</v>
       </c>
@@ -2536,8 +2539,8 @@
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
     </row>
@@ -2567,87 +2570,87 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="85" t="s">
+      <c r="B34" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-      <c r="M34" s="86"/>
-      <c r="N34" s="86"/>
-      <c r="O34" s="86"/>
-      <c r="P34" s="86"/>
-      <c r="Q34" s="87"/>
-      <c r="S34" s="69" t="s">
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="59"/>
+      <c r="S34" s="64" t="s">
         <v>268</v>
       </c>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="69"/>
+      <c r="T34" s="64"/>
+      <c r="U34" s="64"/>
+      <c r="V34" s="64"/>
     </row>
     <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="88"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="89"/>
-      <c r="L35" s="89"/>
-      <c r="M35" s="89"/>
-      <c r="N35" s="89"/>
-      <c r="O35" s="89"/>
-      <c r="P35" s="89"/>
-      <c r="Q35" s="90"/>
-      <c r="S35" s="66" t="s">
+      <c r="B35" s="60"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="62"/>
+      <c r="S35" s="65" t="s">
         <v>309</v>
       </c>
-      <c r="T35" s="67"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="68"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
+      <c r="V35" s="67"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S36" s="66" t="s">
+      <c r="S36" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="T36" s="67"/>
-      <c r="U36" s="67"/>
-      <c r="V36" s="68"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="67"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="63" t="s">
         <v>302</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
-      <c r="N37" s="52"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
-      <c r="S37" s="66" t="s">
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="S37" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="T37" s="67"/>
-      <c r="U37" s="67"/>
-      <c r="V37" s="68"/>
+      <c r="T37" s="66"/>
+      <c r="U37" s="66"/>
+      <c r="V37" s="67"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B38" s="49" t="s">
@@ -2714,34 +2717,34 @@
       <c r="P39" s="49"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="63" t="s">
         <v>304</v>
       </c>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="I41" s="52" t="s">
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="I41" s="63" t="s">
         <v>303</v>
       </c>
-      <c r="J41" s="52"/>
+      <c r="J41" s="63"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="68" t="s">
         <v>293</v>
       </c>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91" t="s">
+      <c r="C42" s="68"/>
+      <c r="D42" s="68" t="s">
         <v>294</v>
       </c>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91" t="s">
+      <c r="E42" s="68"/>
+      <c r="F42" s="68" t="s">
         <v>295</v>
       </c>
-      <c r="G42" s="91"/>
-      <c r="I42" s="91"/>
-      <c r="J42" s="91"/>
+      <c r="G42" s="68"/>
+      <c r="I42" s="68"/>
+      <c r="J42" s="68"/>
     </row>
     <row r="43" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -2762,8 +2765,8 @@
       <c r="G43" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B44" s="50"/>
@@ -2772,8 +2775,8 @@
       <c r="E44" s="50"/>
       <c r="F44" s="50"/>
       <c r="G44" s="50"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91"/>
+      <c r="I44" s="68"/>
+      <c r="J44" s="68"/>
     </row>
     <row r="45" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
@@ -2801,53 +2804,53 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
-      <c r="E47" s="86"/>
-      <c r="F47" s="86"/>
-      <c r="G47" s="86"/>
-      <c r="H47" s="86"/>
-      <c r="I47" s="86"/>
-      <c r="J47" s="86"/>
-      <c r="K47" s="86"/>
-      <c r="L47" s="86"/>
-      <c r="M47" s="86"/>
-      <c r="N47" s="86"/>
-      <c r="O47" s="86"/>
-      <c r="P47" s="86"/>
-      <c r="Q47" s="87"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="59"/>
     </row>
     <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="88"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="89"/>
-      <c r="J48" s="89"/>
-      <c r="K48" s="89"/>
-      <c r="L48" s="89"/>
-      <c r="M48" s="89"/>
-      <c r="N48" s="89"/>
-      <c r="O48" s="89"/>
-      <c r="P48" s="89"/>
-      <c r="Q48" s="90"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="61"/>
+      <c r="P48" s="61"/>
+      <c r="Q48" s="62"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="52" t="s">
+      <c r="B50" s="63" t="s">
         <v>306</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
     </row>
     <row r="51" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="49" t="s">
@@ -2861,12 +2864,29 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B47:Q48"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="S34:V34"/>
-    <mergeCell ref="S35:V35"/>
-    <mergeCell ref="S36:V36"/>
-    <mergeCell ref="S37:V37"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B34:Q35"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B26:Q27"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B14:Q15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="K5:P5"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
@@ -2883,30 +2903,13 @@
     <mergeCell ref="R6:U6"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="G17:L17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="B14:Q15"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B26:Q27"/>
+    <mergeCell ref="B47:Q48"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="S34:V34"/>
+    <mergeCell ref="S35:V35"/>
+    <mergeCell ref="S36:V36"/>
+    <mergeCell ref="S37:V37"/>
     <mergeCell ref="B37:P37"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B34:Q35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2950,60 +2953,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="57"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="79"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="60"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="71"/>
-      <c r="H5" s="70" t="s">
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
+      <c r="H5" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="K5" s="70" t="s">
+      <c r="I5" s="85"/>
+      <c r="K5" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="71"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="85"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -3085,10 +3088,10 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="69"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
@@ -3096,21 +3099,21 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="53">
+      <c r="B10" s="70">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>99.1</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="E10" s="64">
+      <c r="C10" s="70"/>
+      <c r="E10" s="71">
         <v>4</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="E11" s="65"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="E11" s="72"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
@@ -3137,42 +3140,42 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="82"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="H17" s="70" t="s">
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="H17" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="71"/>
-      <c r="L17" s="63" t="s">
+      <c r="I17" s="84"/>
+      <c r="J17" s="85"/>
+      <c r="L17" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="63"/>
+      <c r="M17" s="69"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3203,12 +3206,12 @@
       <c r="J18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L18" s="53">
+      <c r="L18" s="70">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>85</v>
       </c>
-      <c r="M18" s="53"/>
-      <c r="O18" s="73">
+      <c r="M18" s="70"/>
+      <c r="O18" s="76">
         <v>4.5</v>
       </c>
     </row>
@@ -3237,9 +3240,9 @@
       <c r="J19" s="2">
         <v>19.5</v>
       </c>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="O19" s="73"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="O19" s="76"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3264,62 +3267,62 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
-      <c r="N23" s="53" t="s">
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="79"/>
+      <c r="N23" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="O23" s="53"/>
+      <c r="O23" s="70"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="58"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="60"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="82"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="F26" s="54" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="F26" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="70" t="s">
+      <c r="K26" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="L26" s="71"/>
+      <c r="L26" s="85"/>
       <c r="N26" s="9" t="s">
         <v>212</v>
       </c>
@@ -3355,11 +3358,11 @@
       <c r="L27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N27" s="77">
+      <c r="N27" s="88">
         <f>(K29/30*0.4*5)+(B29/25*0.3*5)+(0.3*F29)</f>
         <v>4.9399999999999995</v>
       </c>
-      <c r="O27" s="73">
+      <c r="O27" s="76">
         <v>5</v>
       </c>
     </row>
@@ -3391,27 +3394,27 @@
       <c r="L28" s="2">
         <v>10</v>
       </c>
-      <c r="N28" s="78"/>
-      <c r="O28" s="73"/>
+      <c r="N28" s="89"/>
+      <c r="O28" s="76"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="72">
+      <c r="B29" s="90">
         <f>SUM(B28:D28)</f>
         <v>24</v>
       </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="F29" s="72">
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="F29" s="90">
         <v>5</v>
       </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="K29" s="72">
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="K29" s="90">
         <f>SUM(K28:L28)</f>
         <v>30</v>
       </c>
-      <c r="L29" s="72"/>
+      <c r="L29" s="90"/>
       <c r="N29" s="34"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3437,38 +3440,38 @@
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="57"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="79"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="58"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="60"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="82"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="54"/>
+      <c r="C36" s="75"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="54" t="s">
+      <c r="E36" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3510,14 +3513,14 @@
       <c r="O38" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="F41" s="53" t="s">
+      <c r="C41" s="87"/>
+      <c r="F41" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="53"/>
+      <c r="G41" s="70"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -3573,7 +3576,7 @@
       <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="I44" s="63" t="s">
+      <c r="I44" s="69" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3584,7 +3587,7 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="I45" s="63"/>
+      <c r="I45" s="69"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -3681,70 +3684,70 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="55" t="s">
+      <c r="B58" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="56"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
-      <c r="O58" s="56"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
-      <c r="R58" s="56"/>
-      <c r="S58" s="57"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="78"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="78"/>
+      <c r="K58" s="78"/>
+      <c r="L58" s="78"/>
+      <c r="M58" s="78"/>
+      <c r="N58" s="78"/>
+      <c r="O58" s="78"/>
+      <c r="P58" s="78"/>
+      <c r="Q58" s="78"/>
+      <c r="R58" s="78"/>
+      <c r="S58" s="79"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="58"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="59"/>
-      <c r="L59" s="59"/>
-      <c r="M59" s="59"/>
-      <c r="N59" s="59"/>
-      <c r="O59" s="59"/>
-      <c r="P59" s="59"/>
-      <c r="Q59" s="59"/>
-      <c r="R59" s="59"/>
-      <c r="S59" s="60"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="81"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+      <c r="F59" s="81"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="81"/>
+      <c r="K59" s="81"/>
+      <c r="L59" s="81"/>
+      <c r="M59" s="81"/>
+      <c r="N59" s="81"/>
+      <c r="O59" s="81"/>
+      <c r="P59" s="81"/>
+      <c r="Q59" s="81"/>
+      <c r="R59" s="81"/>
+      <c r="S59" s="82"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="54"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="54"/>
-      <c r="M61" s="54" t="s">
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="75"/>
+      <c r="K61" s="75"/>
+      <c r="M61" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="N61" s="54"/>
-      <c r="O61" s="54"/>
-      <c r="P61" s="54"/>
-      <c r="R61" s="54" t="s">
+      <c r="N61" s="75"/>
+      <c r="O61" s="75"/>
+      <c r="P61" s="75"/>
+      <c r="R61" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="S61" s="54"/>
+      <c r="S61" s="75"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3847,10 +3850,10 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="69"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
@@ -3860,28 +3863,49 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="53">
+      <c r="B67" s="70">
         <f>_xlfn.CEILING.MATH(SUM(B63:K63,M63:P63,R63:S63,G67))</f>
         <v>98</v>
       </c>
-      <c r="C67" s="53"/>
-      <c r="E67" s="73">
+      <c r="C67" s="70"/>
+      <c r="E67" s="76">
         <v>5</v>
       </c>
-      <c r="G67" s="53">
+      <c r="G67" s="70">
         <v>9</v>
       </c>
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
-      <c r="E68" s="73"/>
-      <c r="G68" s="53"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="E68" s="76"/>
+      <c r="G68" s="70"/>
       <c r="H68" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="R61:S61"/>
+    <mergeCell ref="B33:I34"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B58:S59"/>
+    <mergeCell ref="M61:P61"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="F26:I26"/>
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -3898,27 +3922,6 @@
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="O27:O28"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="R61:S61"/>
-    <mergeCell ref="B33:I34"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="B58:S59"/>
-    <mergeCell ref="M61:P61"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E36:G36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3962,60 +3965,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="57"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="79"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="60"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="70" t="s">
+      <c r="K5" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="71"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="85"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -4097,28 +4100,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="69"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="53">
+      <c r="B10" s="70">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="E10" s="64">
+      <c r="C10" s="70"/>
+      <c r="E10" s="71">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="E11" s="65"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="E11" s="72"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -4143,40 +4146,40 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="82"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="F17" s="54" t="s">
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="F17" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="J17" s="63" t="s">
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="J17" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="63"/>
+      <c r="K17" s="69"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -4200,12 +4203,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="53">
+      <c r="J18" s="70">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="53"/>
-      <c r="M18" s="73">
+      <c r="K18" s="70"/>
+      <c r="M18" s="76">
         <v>5</v>
       </c>
     </row>
@@ -4228,9 +4231,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="M19" s="73"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="M19" s="76"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -4255,46 +4258,46 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="79"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="58"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="60"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="82"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="E26" s="70" t="s">
+      <c r="C26" s="75"/>
+      <c r="E26" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="74"/>
-      <c r="G26" s="71"/>
-      <c r="I26" s="54" t="s">
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
+      <c r="I26" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -4329,12 +4332,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="79">
+      <c r="M27" s="91">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="73">
+      <c r="O27" s="76">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -4364,9 +4367,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="79"/>
+      <c r="M28" s="91"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="73"/>
+      <c r="O28" s="76"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4392,39 +4395,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="57"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="79"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="58"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="60"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="82"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="F35" s="54" t="s">
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="F35" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -4481,14 +4484,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="76"/>
-      <c r="F40" s="53" t="s">
+      <c r="C40" s="87"/>
+      <c r="F40" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="53"/>
+      <c r="G40" s="70"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -4544,7 +4547,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="63" t="s">
+      <c r="I43" s="69" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4561,7 +4564,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="63"/>
+      <c r="I44" s="69"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -4705,67 +4708,67 @@
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="55" t="s">
+      <c r="B58" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="56"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
-      <c r="O58" s="56"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
-      <c r="R58" s="57"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="78"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="78"/>
+      <c r="K58" s="78"/>
+      <c r="L58" s="78"/>
+      <c r="M58" s="78"/>
+      <c r="N58" s="78"/>
+      <c r="O58" s="78"/>
+      <c r="P58" s="78"/>
+      <c r="Q58" s="78"/>
+      <c r="R58" s="79"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="58"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="59"/>
-      <c r="L59" s="59"/>
-      <c r="M59" s="59"/>
-      <c r="N59" s="59"/>
-      <c r="O59" s="59"/>
-      <c r="P59" s="59"/>
-      <c r="Q59" s="59"/>
-      <c r="R59" s="60"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="81"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+      <c r="F59" s="81"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="81"/>
+      <c r="K59" s="81"/>
+      <c r="L59" s="81"/>
+      <c r="M59" s="81"/>
+      <c r="N59" s="81"/>
+      <c r="O59" s="81"/>
+      <c r="P59" s="81"/>
+      <c r="Q59" s="81"/>
+      <c r="R59" s="82"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="54"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="54"/>
-      <c r="M61" s="54" t="s">
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="75"/>
+      <c r="K61" s="75"/>
+      <c r="M61" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="54"/>
-      <c r="O61" s="54"/>
-      <c r="Q61" s="54" t="s">
+      <c r="N61" s="75"/>
+      <c r="O61" s="75"/>
+      <c r="Q61" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="54"/>
+      <c r="R61" s="75"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -4862,28 +4865,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="69"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="53">
+      <c r="B67" s="70">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="53"/>
-      <c r="E67" s="73">
+      <c r="C67" s="70"/>
+      <c r="E67" s="76">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
-      <c r="E68" s="73"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="E68" s="76"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -4908,26 +4911,26 @@
     </row>
     <row r="71" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="55" t="s">
+      <c r="B72" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="56"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="56"/>
-      <c r="I72" s="57"/>
+      <c r="C72" s="78"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="78"/>
+      <c r="F72" s="78"/>
+      <c r="G72" s="78"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="79"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="58"/>
-      <c r="C73" s="59"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="59"/>
-      <c r="F73" s="59"/>
-      <c r="G73" s="59"/>
-      <c r="H73" s="59"/>
-      <c r="I73" s="60"/>
+      <c r="B73" s="80"/>
+      <c r="C73" s="81"/>
+      <c r="D73" s="81"/>
+      <c r="E73" s="81"/>
+      <c r="F73" s="81"/>
+      <c r="G73" s="81"/>
+      <c r="H73" s="81"/>
+      <c r="I73" s="82"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
@@ -4954,10 +4957,10 @@
       <c r="I75" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K75" s="63" t="s">
+      <c r="K75" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="63"/>
+      <c r="L75" s="69"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -4987,11 +4990,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="53">
+      <c r="K76" s="70">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="53"/>
+      <c r="L76" s="70"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -5019,20 +5022,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -5043,16 +5042,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5654,10 +5657,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5675,19 +5678,19 @@
       <c r="C2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="97" t="s">
+      <c r="F2" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="97" t="s">
+      <c r="G2" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="56" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5695,13 +5698,13 @@
       <c r="B3" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="54" t="s">
         <v>251</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="55" t="s">
         <v>215</v>
       </c>
       <c r="F3" s="14"/>
@@ -5956,7 +5959,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="43" t="b">
         <v>0</v>
       </c>
@@ -5976,7 +5979,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="43" t="b">
         <v>0</v>
       </c>
@@ -5996,7 +5999,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="43" t="b">
         <v>0</v>
       </c>
@@ -6006,16 +6009,14 @@
       <c r="D20" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="52" t="s">
         <v>289</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="43" t="b">
         <v>0</v>
       </c>
@@ -6032,7 +6033,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="43" t="b">
         <v>0</v>
       </c>
@@ -6047,6 +6048,23 @@
       </c>
       <c r="F22" s="2" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6081,21 +6099,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="F2" s="80" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="F2" s="92" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
-      <c r="J2" s="80" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="J2" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="K2" s="81"/>
-      <c r="L2" s="82"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
@@ -6280,26 +6298,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="28">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="F11" s="83" t="s">
+      <c r="F11" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="84"/>
+      <c r="G11" s="96"/>
       <c r="H11" s="28">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>4.75</v>
       </c>
-      <c r="J11" s="83" t="s">
+      <c r="J11" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="K11" s="84"/>
+      <c r="K11" s="96"/>
       <c r="L11" s="28">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
UKEL - 1st colloquium
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\IoT-studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47000B-0B62-409C-B25A-964830BFC10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7296C38C-8B2F-4A19-9C1D-2D7FA827F972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="III-semestr-25Z" sheetId="5" r:id="rId1"/>
@@ -1571,6 +1571,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1608,21 +1623,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2057,8 +2057,8 @@
   </sheetPr>
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,87 +2075,87 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="61"/>
-      <c r="R2" s="69" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="66"/>
+      <c r="R2" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="64"/>
-      <c r="R3" s="70" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="69"/>
+      <c r="R3" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="72"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="61"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="R4" s="70" t="s">
+      <c r="R4" s="59" t="s">
         <v>265</v>
       </c>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="72"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="61"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="63" t="s">
         <v>261</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="E5" s="58" t="s">
+      <c r="C5" s="63"/>
+      <c r="E5" s="63" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="K5" s="58" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="K5" s="63" t="s">
         <v>263</v>
       </c>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="R5" s="70" t="s">
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="R5" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="72"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="61"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="49" t="s">
@@ -2197,66 +2197,74 @@
       <c r="P6" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="R6" s="70" t="s">
+      <c r="R6" s="59" t="s">
         <v>267</v>
       </c>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="72"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="61"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="E7" s="49">
+      <c r="B7" s="2">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
         <v>4.7</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="K7" s="49">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="49">
+      <c r="L7" s="2">
         <v>1</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="2">
         <v>2</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="R7" s="70" t="s">
+      <c r="N7" s="2">
+        <v>3</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="R7" s="59" t="s">
         <v>269</v>
       </c>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="72"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="61"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="1"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="57">
+      <c r="B10" s="62">
         <f>SUM(B7:C7,E7:I7,K7:P7)</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C10" s="57"/>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="C10" s="62"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="66"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="67"/>
+      <c r="E11" s="72"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2284,82 +2292,82 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="64" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="61"/>
-      <c r="S14" s="69" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="66"/>
+      <c r="S14" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="T14" s="69"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="69"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="62"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="64"/>
-      <c r="S15" s="70" t="s">
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="69"/>
+      <c r="S15" s="59" t="s">
         <v>314</v>
       </c>
-      <c r="T15" s="71"/>
-      <c r="U15" s="71"/>
-      <c r="V15" s="72"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="61"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S16" s="70" t="s">
+      <c r="S16" s="59" t="s">
         <v>315</v>
       </c>
-      <c r="T16" s="71"/>
-      <c r="U16" s="71"/>
-      <c r="V16" s="72"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="61"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="G17" s="58" t="s">
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="G17" s="63" t="s">
         <v>275</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="N17" s="58" t="s">
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="N17" s="63" t="s">
         <v>276</v>
       </c>
-      <c r="O17" s="58"/>
+      <c r="O17" s="63"/>
       <c r="Q17" s="51" t="s">
         <v>277</v>
       </c>
@@ -2401,7 +2409,7 @@
       <c r="O18" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="Q18" s="73"/>
+      <c r="Q18" s="57"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" s="49"/>
@@ -2416,32 +2424,32 @@
       <c r="L19" s="49"/>
       <c r="N19" s="49"/>
       <c r="O19" s="49"/>
-      <c r="Q19" s="74"/>
+      <c r="Q19" s="58"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="65"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="1"/>
       <c r="E21" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="57">
+      <c r="B22" s="62">
         <f>SUM(B19:E19,G19:L19,N19:O19,Q18)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="62"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="66"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="67"/>
+      <c r="E23" s="72"/>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
@@ -2469,74 +2477,74 @@
     </row>
     <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="64" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="61"/>
-      <c r="S26" s="69" t="s">
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="66"/>
+      <c r="S26" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="T26" s="69"/>
-      <c r="U26" s="69"/>
-      <c r="V26" s="69"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="74"/>
+      <c r="V26" s="74"/>
     </row>
     <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="64"/>
-      <c r="S27" s="70" t="s">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="68"/>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="69"/>
+      <c r="S27" s="59" t="s">
         <v>312</v>
       </c>
-      <c r="T27" s="71"/>
-      <c r="U27" s="71"/>
-      <c r="V27" s="72"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="61"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S28" s="70" t="s">
+      <c r="S28" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="T28" s="71"/>
-      <c r="U28" s="71"/>
-      <c r="V28" s="72"/>
+      <c r="T28" s="60"/>
+      <c r="U28" s="60"/>
+      <c r="V28" s="61"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="G29" s="58" t="s">
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="G29" s="63" t="s">
         <v>281</v>
       </c>
-      <c r="H29" s="58"/>
+      <c r="H29" s="63"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -2545,10 +2553,10 @@
       <c r="C30" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="57" t="s">
+      <c r="D30" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="E30" s="57"/>
+      <c r="E30" s="62"/>
       <c r="G30" s="49" t="s">
         <v>73</v>
       </c>
@@ -2557,12 +2565,14 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>8</v>
+      </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="57">
+      <c r="D31" s="62">
         <v>1</v>
       </c>
-      <c r="E31" s="57"/>
+      <c r="E31" s="62"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
     </row>
@@ -2592,87 +2602,87 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="60"/>
-      <c r="O34" s="60"/>
-      <c r="P34" s="60"/>
-      <c r="Q34" s="61"/>
-      <c r="S34" s="69" t="s">
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="66"/>
+      <c r="S34" s="74" t="s">
         <v>268</v>
       </c>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="69"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="74"/>
     </row>
     <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="63"/>
-      <c r="K35" s="63"/>
-      <c r="L35" s="63"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="63"/>
-      <c r="O35" s="63"/>
-      <c r="P35" s="63"/>
-      <c r="Q35" s="64"/>
-      <c r="S35" s="70" t="s">
+      <c r="B35" s="67"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="69"/>
+      <c r="S35" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="T35" s="71"/>
-      <c r="U35" s="71"/>
-      <c r="V35" s="72"/>
+      <c r="T35" s="60"/>
+      <c r="U35" s="60"/>
+      <c r="V35" s="61"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S36" s="70" t="s">
+      <c r="S36" s="59" t="s">
         <v>310</v>
       </c>
-      <c r="T36" s="71"/>
-      <c r="U36" s="71"/>
-      <c r="V36" s="72"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+      <c r="V36" s="61"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="63" t="s">
         <v>302</v>
       </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="S37" s="70" t="s">
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="S37" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="T37" s="71"/>
-      <c r="U37" s="71"/>
-      <c r="V37" s="72"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="61"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B38" s="49" t="s">
@@ -2739,18 +2749,18 @@
       <c r="P39" s="49"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="63" t="s">
         <v>304</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="I41" s="58" t="s">
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="I41" s="63" t="s">
         <v>303</v>
       </c>
-      <c r="J41" s="58"/>
+      <c r="J41" s="63"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B42" s="75" t="s">
@@ -2826,53 +2836,53 @@
     </row>
     <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="64" t="s">
         <v>305</v>
       </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
-      <c r="N47" s="60"/>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="61"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="65"/>
+      <c r="L47" s="65"/>
+      <c r="M47" s="65"/>
+      <c r="N47" s="65"/>
+      <c r="O47" s="65"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="66"/>
     </row>
     <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="62"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
-      <c r="K48" s="63"/>
-      <c r="L48" s="63"/>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="63"/>
-      <c r="P48" s="63"/>
-      <c r="Q48" s="64"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="68"/>
+      <c r="J48" s="68"/>
+      <c r="K48" s="68"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="68"/>
+      <c r="N48" s="68"/>
+      <c r="O48" s="68"/>
+      <c r="P48" s="68"/>
+      <c r="Q48" s="69"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="63" t="s">
         <v>306</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
     </row>
     <row r="51" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="49" t="s">
@@ -2902,11 +2912,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="S28:V28"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="S15:V15"/>
     <mergeCell ref="S16:V16"/>
     <mergeCell ref="B47:Q48"/>
     <mergeCell ref="B50:H50"/>
@@ -2948,6 +2953,11 @@
     <mergeCell ref="B26:Q27"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="B29:E29"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="S28:V28"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="S15:V15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3126,10 +3136,10 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="70"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
@@ -3137,21 +3147,21 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="57">
+      <c r="B10" s="62">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>99.1</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="E10" s="66">
+      <c r="C10" s="62"/>
+      <c r="E10" s="71">
         <v>4</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="E11" s="67"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="E11" s="72"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
@@ -3198,22 +3208,22 @@
       <c r="H15" s="83"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
       <c r="H17" s="76" t="s">
         <v>96</v>
       </c>
       <c r="I17" s="86"/>
       <c r="J17" s="77"/>
-      <c r="L17" s="65" t="s">
+      <c r="L17" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="65"/>
+      <c r="M17" s="70"/>
       <c r="O17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3244,11 +3254,11 @@
       <c r="J18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L18" s="57">
+      <c r="L18" s="62">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>85</v>
       </c>
-      <c r="M18" s="57"/>
+      <c r="M18" s="62"/>
       <c r="O18" s="85">
         <v>4.5</v>
       </c>
@@ -3278,8 +3288,8 @@
       <c r="J19" s="2">
         <v>19.5</v>
       </c>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
       <c r="O19" s="85"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3318,10 +3328,10 @@
       <c r="J23" s="79"/>
       <c r="K23" s="79"/>
       <c r="L23" s="80"/>
-      <c r="N23" s="57" t="s">
+      <c r="N23" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="O23" s="57"/>
+      <c r="O23" s="62"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
@@ -3338,24 +3348,24 @@
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
       <c r="L24" s="83"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="F26" s="68" t="s">
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="F26" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
       <c r="J26" s="7"/>
       <c r="K26" s="76" t="s">
         <v>116</v>
@@ -3500,16 +3510,16 @@
       <c r="I34" s="83"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="68" t="s">
+      <c r="B36" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="68"/>
+      <c r="C36" s="73"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3555,10 +3565,10 @@
         <v>114</v>
       </c>
       <c r="C41" s="88"/>
-      <c r="F41" s="57" t="s">
+      <c r="F41" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="57"/>
+      <c r="G41" s="62"/>
       <c r="I41" s="9" t="s">
         <v>22</v>
       </c>
@@ -3614,7 +3624,7 @@
       <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="I44" s="65" t="s">
+      <c r="I44" s="70" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3625,7 +3635,7 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="I45" s="65"/>
+      <c r="I45" s="70"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
@@ -3764,28 +3774,28 @@
       <c r="S59" s="83"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="68" t="s">
+      <c r="B61" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="68"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="68"/>
-      <c r="F61" s="68"/>
-      <c r="G61" s="68"/>
-      <c r="H61" s="68"/>
-      <c r="I61" s="68"/>
-      <c r="J61" s="68"/>
-      <c r="K61" s="68"/>
-      <c r="M61" s="68" t="s">
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="M61" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="N61" s="68"/>
-      <c r="O61" s="68"/>
-      <c r="P61" s="68"/>
-      <c r="R61" s="68" t="s">
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+      <c r="P61" s="73"/>
+      <c r="R61" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="S61" s="68"/>
+      <c r="S61" s="73"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3888,10 +3898,10 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="65" t="s">
+      <c r="B66" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="65"/>
+      <c r="C66" s="70"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
@@ -3901,24 +3911,24 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="57">
+      <c r="B67" s="62">
         <f>_xlfn.CEILING.MATH(SUM(B63:K63,M63:P63,R63:S63,G67))</f>
         <v>98</v>
       </c>
-      <c r="C67" s="57"/>
+      <c r="C67" s="62"/>
       <c r="E67" s="85">
         <v>5</v>
       </c>
-      <c r="G67" s="57">
+      <c r="G67" s="62">
         <v>9</v>
       </c>
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
       <c r="E68" s="85"/>
-      <c r="G68" s="57"/>
+      <c r="G68" s="62"/>
       <c r="H68" s="7"/>
     </row>
   </sheetData>
@@ -4040,14 +4050,14 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
@@ -4138,28 +4148,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="70"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="57">
+      <c r="B10" s="62">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="E10" s="66">
+      <c r="C10" s="62"/>
+      <c r="E10" s="71">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="E11" s="67"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="E11" s="72"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -4204,20 +4214,20 @@
       <c r="H15" s="83"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="F17" s="68" t="s">
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="F17" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="J17" s="65" t="s">
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="J17" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="65"/>
+      <c r="K17" s="70"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -4241,11 +4251,11 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="57">
+      <c r="J18" s="62">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="57"/>
+      <c r="K18" s="62"/>
       <c r="M18" s="85">
         <v>5</v>
       </c>
@@ -4269,8 +4279,8 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
       <c r="M19" s="85"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4322,20 +4332,20 @@
       <c r="K24" s="83"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="73"/>
       <c r="E26" s="76" t="s">
         <v>21</v>
       </c>
       <c r="F26" s="86"/>
       <c r="G26" s="77"/>
-      <c r="I26" s="68" t="s">
+      <c r="I26" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -4455,17 +4465,17 @@
       <c r="I33" s="83"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="68" t="s">
+      <c r="B35" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="F35" s="68" t="s">
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="F35" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -4526,10 +4536,10 @@
         <v>35</v>
       </c>
       <c r="C40" s="88"/>
-      <c r="F40" s="57" t="s">
+      <c r="F40" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="57"/>
+      <c r="G40" s="62"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -4585,7 +4595,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="65" t="s">
+      <c r="I43" s="70" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4602,7 +4612,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="65"/>
+      <c r="I44" s="70"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -4786,27 +4796,27 @@
       <c r="R59" s="83"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="68" t="s">
+      <c r="B61" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="68"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="68"/>
-      <c r="F61" s="68"/>
-      <c r="G61" s="68"/>
-      <c r="H61" s="68"/>
-      <c r="I61" s="68"/>
-      <c r="J61" s="68"/>
-      <c r="K61" s="68"/>
-      <c r="M61" s="68" t="s">
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="M61" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="68"/>
-      <c r="O61" s="68"/>
-      <c r="Q61" s="68" t="s">
+      <c r="N61" s="73"/>
+      <c r="O61" s="73"/>
+      <c r="Q61" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="68"/>
+      <c r="R61" s="73"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -4903,27 +4913,27 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="65" t="s">
+      <c r="B66" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="65"/>
+      <c r="C66" s="70"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="57">
+      <c r="B67" s="62">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="57"/>
+      <c r="C67" s="62"/>
       <c r="E67" s="85">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
       <c r="E68" s="85"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4995,10 +5005,10 @@
       <c r="I75" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K75" s="65" t="s">
+      <c r="K75" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="65"/>
+      <c r="L75" s="70"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -5028,11 +5038,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="57">
+      <c r="K76" s="62">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="57"/>
+      <c r="L76" s="62"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -5697,7 +5707,7 @@
   </sheetPr>
   <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>